<commit_message>
Test case NEW_SC03 scripting and dry run completed.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816BAF9A-EDBF-450F-90EA-3B65AC113AD9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43C3F57-AE46-406D-B70E-431C0A10D454}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="117">
   <si>
     <t>addressLine1</t>
   </si>
@@ -383,25 +383,34 @@
   </si>
   <si>
     <t>3001712</t>
+  </si>
+  <si>
+    <t>CHANGE_SALARY_BASIS_FOR_EXISTING_EMP</t>
+  </si>
+  <si>
+    <t>3040301</t>
+  </si>
+  <si>
+    <t>3259840</t>
+  </si>
+  <si>
+    <t>EDIT_SALARY_PROPOSAL_REASON</t>
+  </si>
+  <si>
+    <t>15.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -443,10 +452,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -720,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19A3390-A6AD-4713-A279-A24D2033F2ED}">
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:BB9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AR9" sqref="AR9"/>
+      <selection activeCell="AX9" sqref="AX9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,6 +1889,322 @@
         <v>100</v>
       </c>
     </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AS8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB8" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB9" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated catch block with Assert.fail() for the methods developed.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43C3F57-AE46-406D-B70E-431C0A10D454}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFE5609-3992-4F31-B5E5-278438C4CF9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="116">
   <si>
     <t>addressLine1</t>
   </si>
@@ -389,9 +389,6 @@
   </si>
   <si>
     <t>3040301</t>
-  </si>
-  <si>
-    <t>3259840</t>
   </si>
   <si>
     <t>EDIT_SALARY_PROPOSAL_REASON</t>
@@ -728,7 +725,7 @@
   <dimension ref="A1:BB9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AX9" sqref="AX9"/>
+      <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,7 +2011,7 @@
         <v>73</v>
       </c>
       <c r="AR8" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="AS8" s="1" t="s">
         <v>109</v>
@@ -2049,7 +2046,7 @@
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>58</v>
@@ -2175,7 +2172,7 @@
         <v>107</v>
       </c>
       <c r="AS9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AT9" s="1" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Updated Assert in all methods, COmpleted Work Schedule 3 tests, added few common methods, updated Jar to handle numeric value from data sheet
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1EC8CB-B42B-4D1F-BF4F-C10A3A9224AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3984CB86-25F9-4DFF-A18C-0DA98ABA3D51}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
-    <sheet name="Change_Manager" sheetId="4" r:id="rId2"/>
-    <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
-    <sheet name="Termination_Approval" sheetId="6" r:id="rId4"/>
+    <sheet name="Manage_Calendar_Events" sheetId="7" r:id="rId2"/>
+    <sheet name="Change_Manager" sheetId="4" r:id="rId3"/>
+    <sheet name="Employee_Details" sheetId="5" r:id="rId4"/>
+    <sheet name="Termination_Approval" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="127">
   <si>
     <t>addressLine1</t>
   </si>
@@ -350,6 +351,66 @@
   </si>
   <si>
     <t>NEW_HIRE</t>
+  </si>
+  <si>
+    <t>effectiveFromDate</t>
+  </si>
+  <si>
+    <t>effectiveToDate</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>5 Days x 7 Hours</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Elapsed</t>
+  </si>
+  <si>
+    <t>27-Feb-2019</t>
+  </si>
+  <si>
+    <t>27-May-2019</t>
+  </si>
+  <si>
+    <t>WORK_SCHEDULE_CREATE</t>
+  </si>
+  <si>
+    <t>WORK_SCHEDULE_UPDATE</t>
+  </si>
+  <si>
+    <t>WORK_SCHEDULE_INACTIVE</t>
+  </si>
+  <si>
+    <t>patternName</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>TestWorkSchedule1</t>
+  </si>
+  <si>
+    <t>27-Jun-2019</t>
+  </si>
+  <si>
+    <t>3259981</t>
   </si>
 </sst>
 </file>
@@ -385,10 +446,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19A3390-A6AD-4713-A279-A24D2033F2ED}">
   <dimension ref="A1:BB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AR6" sqref="AR6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1000,7 +1062,7 @@
       <c r="AL2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AM2" s="3" t="s">
         <v>87</v>
       </c>
       <c r="AN2" s="1" t="s">
@@ -1632,7 +1694,9 @@
       <c r="AQ6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AR6" s="1"/>
+      <c r="AR6" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="AS6" s="1" t="s">
         <v>91</v>
       </c>
@@ -1671,6 +1735,149 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EB2B9D-610E-4BF5-9152-3B76A6C040A1}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8777768F-EEF9-4BC5-BAC7-FFF99A5CC805}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1682,7 +1889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B6DDF3-12E0-4DA3-8971-08738D1AF9F8}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1694,7 +1901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11F9D52-282A-4831-9943-74CFFB346BED}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixed few timeout issues and tested Talent Acquisition and Work Schedule
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3984CB86-25F9-4DFF-A18C-0DA98ABA3D51}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977B307B-20DB-4CE3-9509-15FBFF854870}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="126">
   <si>
     <t>addressLine1</t>
   </si>
@@ -408,9 +408,6 @@
   </si>
   <si>
     <t>27-Jun-2019</t>
-  </si>
-  <si>
-    <t>3259981</t>
   </si>
 </sst>
 </file>
@@ -1694,9 +1691,7 @@
       <c r="AQ6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AR6" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="AR6" s="1"/>
       <c r="AS6" s="1" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Code updated for US.AC.53
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1EC8CB-B42B-4D1F-BF4F-C10A3A9224AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B7DE3F-599F-453A-944C-C4955F90DDE4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="115">
   <si>
     <t>addressLine1</t>
   </si>
@@ -350,6 +350,30 @@
   </si>
   <si>
     <t>NEW_HIRE</t>
+  </si>
+  <si>
+    <t>NEW_ADDRESS_ALTERNATIVE_WORK_LOCATION</t>
+  </si>
+  <si>
+    <t>ADD_EMERGENCY_CONTACT_DETAILS</t>
+  </si>
+  <si>
+    <t>UPDATE_PERSONAL_PAYMENT_METHODS_EXPENSES_ONLY</t>
+  </si>
+  <si>
+    <t>UPDATE_PERSONAL_PAYMENT_METHODS_NON_EXPENSES_ONLY</t>
+  </si>
+  <si>
+    <t>UPDATE_ADDRESS_BIOGRAPHICAL_INFO_DRIVING_LICENSE_DOCUMENTS</t>
+  </si>
+  <si>
+    <t>UPDATE_REMOVE_I9_STATUS</t>
+  </si>
+  <si>
+    <t>i9Status</t>
+  </si>
+  <si>
+    <t>Ready to verify</t>
   </si>
 </sst>
 </file>
@@ -669,71 +693,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19A3390-A6AD-4713-A279-A24D2033F2ED}">
-  <dimension ref="A1:BB6"/>
+  <dimension ref="A1:BC7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -896,8 +920,11 @@
       <c r="BB1" t="s">
         <v>52</v>
       </c>
+      <c r="BC1" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="2" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:55" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -1046,7 +1073,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>106</v>
       </c>
@@ -1200,7 +1227,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1354,7 +1381,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1508,7 +1535,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1662,6 +1689,23 @@
       </c>
       <c r="BB6" s="1" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AX7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1676,7 +1720,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1684,12 +1728,954 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B6DDF3-12E0-4DA3-8971-08738D1AF9F8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB6" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1700,7 +2686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Scripts moved to respective feature files and page classes
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFE5609-3992-4F31-B5E5-278438C4CF9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8812DD8-395C-4FB1-9B35-C13D4F7B1F37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,16 +13,10 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Termination_Approval" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -31,15 +25,51 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={D1CD9F28-06B0-45F1-AC2F-A4B295A42627}</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="AR7" authorId="0" shapeId="0" xr:uid="{D1CD9F28-06B0-45F1-AC2F-A4B295A42627}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     3001660</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="AR2" authorId="0" shapeId="0" xr:uid="{FDF7D4B7-BF89-4F3B-A983-E7C31D0C0CEE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    3001660</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -47,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="116">
   <si>
     <t>addressLine1</t>
   </si>
@@ -724,69 +754,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19A3390-A6AD-4713-A279-A24D2033F2ED}">
   <dimension ref="A1:BB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AR8" sqref="AR8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -950,7 +980,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -1102,7 +1132,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>106</v>
       </c>
@@ -1258,7 +1288,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1414,7 +1444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1570,7 +1600,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1728,7 +1758,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -1886,7 +1916,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -2044,7 +2074,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -2215,21 +2245,718 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B6DDF3-12E0-4DA3-8971-08738D1AF9F8}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B6DDF3-12E0-4DA3-8971-08738D1AF9F8}">
+  <dimension ref="A1:BB4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AY4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AZ4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2239,7 +2966,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Edit Emp details
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03451188-CC6F-49B6-86D8-138DF766C177}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB432B05-07CF-456E-B457-1E92B394145C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
     <sheet name="Manage_Calendar_Events" sheetId="7" r:id="rId2"/>
-    <sheet name="Change_Manager" sheetId="4" r:id="rId3"/>
+    <sheet name="Line_Manager" sheetId="4" r:id="rId3"/>
     <sheet name="Employee_Details" sheetId="5" r:id="rId4"/>
-    <sheet name="Termination_Approval" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="169">
   <si>
     <t>addressLine1</t>
   </si>
@@ -362,12 +361,6 @@
     <t>UPDATE_PERSONAL_PAYMENT_METHODS_EXPENSES_ONLY</t>
   </si>
   <si>
-    <t>UPDATE_PERSONAL_PAYMENT_METHODS_NON_EXPENSES_ONLY</t>
-  </si>
-  <si>
-    <t>UPDATE_ADDRESS_BIOGRAPHICAL_INFO_DRIVING_LICENSE_DOCUMENTS</t>
-  </si>
-  <si>
     <t>UPDATE_REMOVE_I9_STATUS</t>
   </si>
   <si>
@@ -432,6 +425,117 @@
   </si>
   <si>
     <t>WORK_SCHEDULE_INACTIVE</t>
+  </si>
+  <si>
+    <t>bankName</t>
+  </si>
+  <si>
+    <t>organizationPaymentMethod</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>accountNumber</t>
+  </si>
+  <si>
+    <t>accountType</t>
+  </si>
+  <si>
+    <t>accountHolder</t>
+  </si>
+  <si>
+    <t>routingNumber</t>
+  </si>
+  <si>
+    <t>HSBC</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>464613164666</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Test Account Holder</t>
+  </si>
+  <si>
+    <t>122105155</t>
+  </si>
+  <si>
+    <t>Alternate Work Location Address</t>
+  </si>
+  <si>
+    <t>SMALLSYS INC, 795 E DRAGRAM</t>
+  </si>
+  <si>
+    <t>85705</t>
+  </si>
+  <si>
+    <t>contactsRelationship</t>
+  </si>
+  <si>
+    <t>contactsEmergencyContactName</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>changeManagerReason</t>
+  </si>
+  <si>
+    <t>employeeManagerChange</t>
+  </si>
+  <si>
+    <t>managerName</t>
+  </si>
+  <si>
+    <t>personName</t>
+  </si>
+  <si>
+    <t>Manager Change</t>
+  </si>
+  <si>
+    <t>arax sftqmplj</t>
+  </si>
+  <si>
+    <t>ovhjs, mopjyqh</t>
+  </si>
+  <si>
+    <t>TestAutoFname TestAutoLname</t>
+  </si>
+  <si>
+    <t>LINE_MANAGER_PERFORMS_CHANGE_MANAGER</t>
+  </si>
+  <si>
+    <t>LINE_MANAGER1_APPROVES_CHANGE_MANAGER_REQUEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINEMANAGER_TERMINATE_DIRECT_REPORTEES </t>
+  </si>
+  <si>
+    <t>PPS_APPROVES_TERMINATION</t>
+  </si>
+  <si>
+    <t>altWorkLocationAddressType</t>
+  </si>
+  <si>
+    <t>altWorkLocationCountry</t>
+  </si>
+  <si>
+    <t>altWorkLocationAddressLine1</t>
+  </si>
+  <si>
+    <t>altWorkLocationZipCode</t>
+  </si>
+  <si>
+    <t>aa, hfgtwc</t>
   </si>
 </sst>
 </file>
@@ -467,11 +571,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,7 +1089,7 @@
         <v>52</v>
       </c>
       <c r="BC1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:55" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1752,7 +1861,7 @@
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AN7" s="1" t="s">
         <v>88</v>
@@ -1764,7 +1873,7 @@
         <v>96</v>
       </c>
       <c r="BC7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1778,7 +1887,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,28 +1910,28 @@
         <v>101</v>
       </c>
       <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
         <v>115</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>118</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>119</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>120</v>
-      </c>
-      <c r="H1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" t="s">
-        <v>122</v>
       </c>
       <c r="J1" t="s">
         <v>38</v>
@@ -1833,31 +1942,31 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>88</v>
@@ -1868,16 +1977,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1891,14 +2000,14 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1918,12 +2027,105 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8777768F-EEF9-4BC5-BAC7-FFF99A5CC805}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1932,964 +2134,440 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B6DDF3-12E0-4DA3-8971-08738D1AF9F8}">
   <dimension ref="A1:BB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="6" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
+      <c r="B1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="2"/>
       <c r="W2" s="1"/>
-      <c r="X2" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-      <c r="AG2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
-      <c r="AK2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
-      <c r="AS2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="M3" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="2"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
-      <c r="AK3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AZ3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB3" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="1"/>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="2"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
-      <c r="AG4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
-      <c r="AK4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
-      <c r="AS4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AZ4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BA4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB4" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="1"/>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="2"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
-      <c r="AG5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI5" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
-      <c r="AK5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
-      <c r="AS5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY5" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AZ5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BA5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB5" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="2"/>
       <c r="W6" s="1"/>
-      <c r="X6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE6" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
-      <c r="AG6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI6" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
-      <c r="AK6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>
-      <c r="AS6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AY6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AZ6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BA6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB6" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11F9D52-282A-4831-9943-74CFFB346BED}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merged changes for GL.AC.01 and removed unwanted feature file TerminationApproavl.Renamed change Manager to Line Manager
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3F505D-2975-4D36-A75C-68672F0EC81E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
     <sheet name="Manage_Calendar_Events" sheetId="7" r:id="rId2"/>
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
-    <sheet name="Termination_Approval" sheetId="6" r:id="rId4"/>
+    <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="154">
   <si>
     <t>scenario</t>
   </si>
@@ -458,13 +457,40 @@
   </si>
   <si>
     <t>VALIDATE_ADDRESS_FORMAT</t>
+  </si>
+  <si>
+    <t>employeeName</t>
+  </si>
+  <si>
+    <t>actionManageSalary</t>
+  </si>
+  <si>
+    <t>actionReasonManageSalary</t>
+  </si>
+  <si>
+    <t>LINEMANAGER_CHANGE_OF_SALARY_ACTION</t>
+  </si>
+  <si>
+    <t>3056871</t>
+  </si>
+  <si>
+    <t>Welcome1</t>
+  </si>
+  <si>
+    <t>TestAutoFname TestAutoLname</t>
+  </si>
+  <si>
+    <t>Change Salary</t>
+  </si>
+  <si>
+    <t>Change in Working Hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,7 +587,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -596,7 +622,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -773,79 +799,79 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19A3390-A6AD-4713-A279-A24D2033F2ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.83984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.83984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.26171875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.83984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.15625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.83984375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.83984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.83984375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.83984375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="26.578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.15625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:54">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1035,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:54" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1158,7 +1184,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:54">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -1312,7 +1338,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:54">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1466,7 +1492,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:54">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1620,7 +1646,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:54">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1783,29 +1809,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EB2B9D-610E-4BF5-9152-3B76A6C040A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.41796875" customWidth="1"/>
-    <col min="8" max="8" width="14.578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.578125" customWidth="1"/>
-    <col min="10" max="10" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1840,7 +1866,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -1875,7 +1901,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>123</v>
       </c>
@@ -1898,7 +1924,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -1926,79 +1952,79 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B6DDF3-12E0-4DA3-8971-08738D1AF9F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:BI6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.20703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.15625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.83984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.68359375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.26171875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.15625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.83984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.15625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.41796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.15625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.26171875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.83984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.41796875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.83984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="22" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="36.26171875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.15625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.68359375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.83984375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="16" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="12" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.26171875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="29.41796875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.41796875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.26171875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.26171875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="24" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.5234375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.5234375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.7890625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.62890625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:61">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2209,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:61">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -2208,7 +2234,7 @@
         <v>3259228</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:61">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2233,7 +2259,7 @@
         <v>3040301</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:61">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2279,7 +2305,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:61">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2325,7 +2351,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:61">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -2345,13 +2371,62 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11F9D52-282A-4831-9943-74CFFB346BED}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="4">
+        <v>80572.460000000006</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2372,15 +2447,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -2613,6 +2679,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
@@ -2624,14 +2699,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2648,4 +2715,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL.AC.51 and added wait loads for common methods
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="160">
   <si>
     <t>scenario</t>
   </si>
@@ -484,6 +484,24 @@
   </si>
   <si>
     <t>Change in Working Hours</t>
+  </si>
+  <si>
+    <t>EDIT_PROJECTED_ENDDATE</t>
+  </si>
+  <si>
+    <t>projectedEndDate</t>
+  </si>
+  <si>
+    <t>correctEmploymentAction</t>
+  </si>
+  <si>
+    <t>correctEmploymentActionReason</t>
+  </si>
+  <si>
+    <t>3259988</t>
+  </si>
+  <si>
+    <t>Add Pending Worker</t>
   </si>
 </sst>
 </file>
@@ -519,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -527,6 +545,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB6"/>
+  <dimension ref="A1:BE7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BE7" sqref="BE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -869,9 +888,12 @@
     <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:57">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1034,8 +1056,17 @@
       <c r="BB1" t="s">
         <v>53</v>
       </c>
+      <c r="BC1" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BE1" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
-    <row r="2" spans="1:54" s="1" customFormat="1">
+    <row r="2" spans="1:57" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1184,7 +1215,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:54">
+    <row r="3" spans="1:57">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -1338,7 +1369,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:54">
+    <row r="4" spans="1:57">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1492,7 +1523,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:57">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1646,7 +1677,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:57">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1800,6 +1831,173 @@
       </c>
       <c r="BB6" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:57">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AX7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AY7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AZ7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BA7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BB7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BC7" s="5">
+        <v>43687</v>
+      </c>
+      <c r="BD7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BE7" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2374,8 +2572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated locator changes and fixed common methods to run 2 scenarios currently (new hire and i9)
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AEA62D-1381-4162-BA6C-587DB17D56FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,8 +14,8 @@
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="179">
   <si>
     <t>scenario</t>
   </si>
@@ -528,12 +529,6 @@
     <t>05Business Unit</t>
   </si>
   <si>
-    <t>Associate Accountant</t>
-  </si>
-  <si>
-    <t>US Consulting PPMXX</t>
-  </si>
-  <si>
     <t>ARG 01 05457</t>
   </si>
   <si>
@@ -547,13 +542,31 @@
   </si>
   <si>
     <t>1/1/1990</t>
+  </si>
+  <si>
+    <t>HA: Contractor</t>
+  </si>
+  <si>
+    <t>BT Financial Sales</t>
+  </si>
+  <si>
+    <t>UPDATE_REMOVE_I9_STATUS</t>
+  </si>
+  <si>
+    <t>Ready to verify</t>
+  </si>
+  <si>
+    <t>i9Status</t>
+  </si>
+  <si>
+    <t>500069</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -591,6 +604,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,82 +879,82 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1110,8 +1126,11 @@
       <c r="BE1" s="7" t="s">
         <v>157</v>
       </c>
+      <c r="BF1" s="7" t="s">
+        <v>177</v>
+      </c>
     </row>
-    <row r="2" spans="1:57" s="1" customFormat="1">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1260,7 +1279,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:57">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -1298,10 +1317,10 @@
         <v>65</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>68</v>
@@ -1336,7 +1355,7 @@
         <v>77</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>79</v>
@@ -1348,14 +1367,14 @@
         <v>81</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
         <v>161</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>85</v>
@@ -1377,7 +1396,7 @@
         <v>165</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>74</v>
@@ -1387,7 +1406,7 @@
         <v>92</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>94</v>
@@ -1414,7 +1433,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:57">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1568,7 +1587,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:57">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1722,7 +1741,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:57">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1878,7 +1897,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:57">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -2043,6 +2062,74 @@
       </c>
       <c r="BE7" s="1" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="8"/>
+      <c r="AW8" s="8"/>
+      <c r="AX8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AY8" s="8"/>
+      <c r="AZ8" s="8"/>
+      <c r="BA8" s="8"/>
+      <c r="BB8" s="8"/>
+      <c r="BC8" s="8"/>
+      <c r="BF8" s="8" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2052,29 +2139,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2109,7 +2196,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -2144,7 +2231,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>123</v>
       </c>
@@ -2167,7 +2254,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2195,79 +2282,79 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BI6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="22" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="16" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="12" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="24" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2452,7 +2539,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -2477,7 +2564,7 @@
         <v>3259228</v>
       </c>
     </row>
-    <row r="3" spans="1:61">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2502,7 +2589,7 @@
         <v>3040301</v>
       </c>
     </row>
-    <row r="4" spans="1:61">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2548,7 +2635,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2594,7 +2681,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -2614,16 +2701,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2646,7 +2733,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -2675,21 +2762,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -2922,6 +2994,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2932,16 +3019,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2960,6 +3037,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Write to excel method in core and tested with new hire and i9 update
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AEA62D-1381-4162-BA6C-587DB17D56FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{1FAAB044-F63D-47E8-BC0E-21F5B50BAC13}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
-    <sheet name="Manage_Calendar_Events" sheetId="7" r:id="rId2"/>
-    <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
-    <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
+    <sheet name="Talent_Acquisition" r:id="rId1" sheetId="2"/>
+    <sheet name="Manage_Calendar_Events" r:id="rId2" sheetId="7"/>
+    <sheet name="Employee_Details" r:id="rId3" sheetId="5"/>
+    <sheet name="Line_Manager" r:id="rId4" sheetId="8"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="181">
   <si>
     <t>scenario</t>
   </si>
@@ -559,13 +559,20 @@
     <t>i9Status</t>
   </si>
   <si>
-    <t>500069</t>
+    <t>500070</t>
+  </si>
+  <si>
+    <t>500071</t>
+  </si>
+  <si>
+    <t>500072</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -593,26 +600,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="15" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -629,10 +636,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -796,21 +803,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -827,7 +834,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -879,79 +886,79 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
       <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="21.453125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="26.26953125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="33.1796875" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="4.81640625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="26.54296875" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="17.1796875" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="24.54296875" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.35">
@@ -1130,7 +1137,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="2" s="1" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1401,7 +1408,9 @@
       <c r="AQ3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AR3" s="1"/>
+      <c r="AR3" t="s">
+        <v>178</v>
+      </c>
       <c r="AS3" s="1" t="s">
         <v>92</v>
       </c>
@@ -2064,7 +2073,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="8" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>175</v>
       </c>
@@ -2112,8 +2121,8 @@
       <c r="AO8" s="8"/>
       <c r="AP8" s="8"/>
       <c r="AQ8" s="8"/>
-      <c r="AR8" s="1" t="s">
-        <v>178</v>
+      <c r="AR8" t="s">
+        <v>180</v>
       </c>
       <c r="AS8" s="8"/>
       <c r="AT8" s="8"/>
@@ -2133,14 +2142,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -2148,17 +2157,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.54296875" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.26953125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="5.54296875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2276,14 +2285,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BI6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BJ6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -2291,67 +2300,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.453125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="22" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="36.26953125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="24" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="49.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.453125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="7.1796875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="27.81640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="25.1796875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="20.26953125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="26.81640625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="33.453125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="36.26953125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="21.7265625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="13.81640625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="29.453125" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.35">
@@ -2696,13 +2705,13 @@
       <c r="BI6" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -2757,7 +2766,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Scripts are update to run on Cognizant instant. Need to config.yaml with team
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{1FAAB044-F63D-47E8-BC0E-21F5B50BAC13}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D45C2C-2DB2-4431-A3C1-B790BAE7660B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Talent_Acquisition" r:id="rId1" sheetId="2"/>
-    <sheet name="Manage_Calendar_Events" r:id="rId2" sheetId="7"/>
-    <sheet name="Employee_Details" r:id="rId3" sheetId="5"/>
-    <sheet name="Line_Manager" r:id="rId4" sheetId="8"/>
+    <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
+    <sheet name="Manage_Calendar_Events" sheetId="7" r:id="rId2"/>
+    <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
+    <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="182">
   <si>
     <t>scenario</t>
   </si>
@@ -562,17 +562,19 @@
     <t>500070</t>
   </si>
   <si>
-    <t>500071</t>
-  </si>
-  <si>
     <t>500072</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>80000.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,26 +602,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="15" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -636,10 +638,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -803,21 +805,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -834,7 +836,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -886,82 +888,82 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AR8" sqref="AR8"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AX8" sqref="AX8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.453125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="21.453125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="33.1796875" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="4.81640625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="26.54296875" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="24.54296875" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1124,20 +1126,20 @@
       <c r="BB1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="7" t="s">
+      <c r="BC1" t="s">
         <v>155</v>
       </c>
-      <c r="BD1" s="7" t="s">
+      <c r="BD1" t="s">
         <v>156</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BE1" t="s">
         <v>157</v>
       </c>
-      <c r="BF1" s="7" t="s">
+      <c r="BF1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1286,7 +1288,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -1442,7 +1444,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1596,7 +1598,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1750,7 +1752,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1906,7 +1908,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -2073,104 +2075,104 @@
         <v>80</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:58" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:58" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
       <c r="AN8" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
       <c r="AR8" t="s">
-        <v>180</v>
-      </c>
-      <c r="AS8" s="8"/>
-      <c r="AT8" s="8"/>
-      <c r="AU8" s="8"/>
-      <c r="AV8" s="8"/>
-      <c r="AW8" s="8"/>
+        <v>179</v>
+      </c>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="7"/>
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="7"/>
       <c r="AX8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AY8" s="8"/>
-      <c r="AZ8" s="8"/>
-      <c r="BA8" s="8"/>
-      <c r="BB8" s="8"/>
-      <c r="BC8" s="8"/>
-      <c r="BF8" s="8" t="s">
+      <c r="AY8" s="7"/>
+      <c r="AZ8" s="7"/>
+      <c r="BA8" s="7"/>
+      <c r="BB8" s="7"/>
+      <c r="BC8" s="7"/>
+      <c r="BF8" s="7" t="s">
         <v>176</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2205,7 +2207,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -2240,7 +2242,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>123</v>
       </c>
@@ -2263,7 +2265,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2285,85 +2287,85 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BJ6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AR4" sqref="AR4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="49.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="7.1796875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="27.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="25.1796875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="20.26953125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="26.81640625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="33.453125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="36.26953125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="21.7265625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.81640625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="29.453125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="36.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2548,7 +2550,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -2560,20 +2562,20 @@
       <c r="AB2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AN2" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="AQ2" s="5"/>
       <c r="AR2">
-        <v>3001712</v>
-      </c>
-      <c r="AS2" s="4">
-        <v>80000</v>
-      </c>
-      <c r="AX2">
-        <v>3259228</v>
+        <v>500061</v>
+      </c>
+      <c r="AS2" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2585,20 +2587,20 @@
       <c r="AB3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AN3" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="AQ3" s="5"/>
       <c r="AR3">
-        <v>3259949</v>
-      </c>
-      <c r="AS3" s="4">
-        <v>80000</v>
-      </c>
-      <c r="AX3">
-        <v>3040301</v>
+        <v>500070</v>
+      </c>
+      <c r="AS3" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2610,17 +2612,17 @@
       <c r="AB4" s="5"/>
       <c r="AL4" s="5"/>
       <c r="AN4" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="AQ4" s="5"/>
       <c r="AR4">
-        <v>3259949</v>
-      </c>
-      <c r="AS4">
-        <v>15</v>
-      </c>
-      <c r="AX4">
-        <v>3259228</v>
+        <v>500061</v>
+      </c>
+      <c r="AS4" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>163</v>
       </c>
       <c r="BC4" t="s">
         <v>137</v>
@@ -2644,7 +2646,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2662,8 +2664,8 @@
       <c r="AR5">
         <v>3259949</v>
       </c>
-      <c r="AS5">
-        <v>15</v>
+      <c r="AS5" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="AX5">
         <v>3259228</v>
@@ -2690,7 +2692,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -2705,21 +2707,21 @@
       <c r="BI6" s="6"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2742,7 +2744,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -2766,11 +2768,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3003,21 +3020,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3028,6 +3030,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3046,16 +3058,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated code for address
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{1FAAB044-F63D-47E8-BC0E-21F5B50BAC13}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E3DB22-313B-4CD3-B1F8-2E88B0CD36FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Talent_Acquisition" r:id="rId1" sheetId="2"/>
-    <sheet name="Manage_Calendar_Events" r:id="rId2" sheetId="7"/>
-    <sheet name="Employee_Details" r:id="rId3" sheetId="5"/>
-    <sheet name="Line_Manager" r:id="rId4" sheetId="8"/>
+    <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
+    <sheet name="Manage_Calendar_Events" sheetId="7" r:id="rId2"/>
+    <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
+    <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="188">
   <si>
     <t>scenario</t>
   </si>
@@ -562,17 +562,37 @@
     <t>500070</t>
   </si>
   <si>
-    <t>500071</t>
-  </si>
-  <si>
     <t>500072</t>
+  </si>
+  <si>
+    <t>NEW_ADDRESS_ALTERNATIVE_WORK_LOCATION</t>
+  </si>
+  <si>
+    <t>altWorkLocationAddressLine1</t>
+  </si>
+  <si>
+    <t>altWorkLocationCountry</t>
+  </si>
+  <si>
+    <t>altWorkLocationZipCode</t>
+  </si>
+  <si>
+    <t>Crescent Loop Dr</t>
+  </si>
+  <si>
+    <t>test2019</t>
+  </si>
+  <si>
+    <t>altWorkLocationAddressType</t>
+  </si>
+  <si>
+    <t>Alternate work Location Address</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,26 +620,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="15" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -636,10 +656,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -803,21 +823,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -834,7 +854,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -886,82 +906,82 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.453125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="21.453125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="33.1796875" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="4.81640625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="26.54296875" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="24.54296875" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1137,7 +1157,7 @@
         <v>177</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1286,7 +1306,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -1442,7 +1462,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1596,7 +1616,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1750,7 +1770,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1906,7 +1926,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -2073,7 +2093,7 @@
         <v>80</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>175</v>
       </c>
@@ -2122,7 +2142,7 @@
       <c r="AP8" s="8"/>
       <c r="AQ8" s="8"/>
       <c r="AR8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AS8" s="8"/>
       <c r="AT8" s="8"/>
@@ -2142,35 +2162,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2205,7 +2225,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -2240,7 +2260,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>123</v>
       </c>
@@ -2263,7 +2283,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2285,85 +2305,85 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BJ6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BM7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
+      <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="49.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="7.1796875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="27.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="25.1796875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="20.26953125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="26.81640625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="33.453125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="36.26953125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="21.7265625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.81640625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="29.453125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="36.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2547,8 +2567,20 @@
       <c r="BI1" t="s">
         <v>136</v>
       </c>
+      <c r="BJ1" t="s">
+        <v>181</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>186</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>182</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>183</v>
+      </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -2573,7 +2605,7 @@
         <v>3259228</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2598,7 +2630,7 @@
         <v>3040301</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2644,7 +2676,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2690,7 +2722,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -2704,22 +2736,45 @@
       <c r="BF6" s="2"/>
       <c r="BI6" s="6"/>
     </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>180</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>185</v>
+      </c>
+      <c r="AX7">
+        <v>10171</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>184</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>187</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM7">
+        <v>48382</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2742,7 +2797,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -2766,7 +2821,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code for P17 add a New Address as an alternative work location
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E3DB22-313B-4CD3-B1F8-2E88B0CD36FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B633D-F0BA-4B24-A8EA-23CB64713694}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="189">
   <si>
     <t>scenario</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>Alternate work Location Address</t>
+  </si>
+  <si>
+    <t>ADD_EMERGENCY_CONTACT_DETAILS</t>
   </si>
 </sst>
 </file>
@@ -2312,10 +2315,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BM7"/>
+  <dimension ref="A1:BM8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BK7" sqref="BK7"/>
+    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="BN3" sqref="BN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,6 +2762,17 @@
         <v>48382</v>
       </c>
     </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>185</v>
+      </c>
+      <c r="AX8">
+        <v>10171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2826,6 +2840,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3058,7 +3081,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
@@ -3073,16 +3096,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3101,7 +3123,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3109,12 +3131,4 @@
     <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated CSV read and write method and implemented in New Hire class
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{1FAAB044-F63D-47E8-BC0E-21F5B50BAC13}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D1C629B8-2D63-4842-9A0B-F5806288B796}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
   <bookViews>
     <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="164">
   <si>
     <t>scenario</t>
   </si>
@@ -202,9 +202,6 @@
     <t>Full-time regular</t>
   </si>
   <si>
-    <t>Finance</t>
-  </si>
-  <si>
     <t>Irving</t>
   </si>
   <si>
@@ -223,15 +220,6 @@
     <t>Dallas</t>
   </si>
   <si>
-    <t>12-Apr-1988</t>
-  </si>
-  <si>
-    <t>Finance Internal Audit - EMEA</t>
-  </si>
-  <si>
-    <t>Pearson Inc</t>
-  </si>
-  <si>
     <t>Bilingual Indicator</t>
   </si>
   <si>
@@ -244,9 +232,6 @@
     <t>Global Temporary Assignment</t>
   </si>
   <si>
-    <t>GM Temporary Relocation</t>
-  </si>
-  <si>
     <t>13-Feb-2019</t>
   </si>
   <si>
@@ -259,54 +244,27 @@
     <t>E</t>
   </si>
   <si>
-    <t>Hire</t>
-  </si>
-  <si>
     <t>28-Jan-19</t>
   </si>
   <si>
-    <t>Additional Hire</t>
-  </si>
-  <si>
     <t>Salaried</t>
   </si>
   <si>
-    <t>Director Audit &amp; Compliance</t>
-  </si>
-  <si>
-    <t>NCS Pearson, Inc</t>
-  </si>
-  <si>
-    <t>AR-Buenos Aires-Humboldt 1509/13</t>
-  </si>
-  <si>
     <t>Single</t>
   </si>
   <si>
     <t>Social Security Number</t>
   </si>
   <si>
-    <t>12-Apr-2017</t>
-  </si>
-  <si>
     <t>2717522</t>
   </si>
   <si>
     <t>Welcome123</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Bi-Weekly Exempt</t>
-  </si>
-  <si>
     <t>21208.59</t>
   </si>
   <si>
-    <t>US Annual Salary</t>
-  </si>
-  <si>
     <t>TX</t>
   </si>
   <si>
@@ -328,9 +286,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>75038</t>
-  </si>
-  <si>
     <t>NEW_HIRE</t>
   </si>
   <si>
@@ -343,9 +298,6 @@
     <t>UPDATE_PERSONAL_ASSIGNMENT_DATA</t>
   </si>
   <si>
-    <t>International Assignment</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -499,12 +451,6 @@
     <t>correctEmploymentActionReason</t>
   </si>
   <si>
-    <t>3259988</t>
-  </si>
-  <si>
-    <t>Add Pending Worker</t>
-  </si>
-  <si>
     <t>New Hire</t>
   </si>
   <si>
@@ -562,10 +508,13 @@
     <t>500070</t>
   </si>
   <si>
+    <t>Career Progression</t>
+  </si>
+  <si>
+    <t>ChicagoTrust_DH</t>
+  </si>
+  <si>
     <t>500071</t>
-  </si>
-  <si>
-    <t>500072</t>
   </si>
 </sst>
 </file>
@@ -896,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AR8" sqref="AR8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,16 +1074,16 @@
         <v>53</v>
       </c>
       <c r="BC1" s="7" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="BD1" s="7" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="BE1" s="7" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="BF1" s="7" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:58" x14ac:dyDescent="0.35">
@@ -1154,141 +1103,148 @@
         <v>58</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="T2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="V2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="AE2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AL2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="BB2" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>55</v>
@@ -1303,148 +1259,148 @@
         <v>58</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="T3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="V3" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AL3" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>178</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="AY3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="BB3" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>55</v>
@@ -1459,146 +1415,148 @@
         <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="T4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="V4" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AL4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AW4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA4" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="BB4" s="1" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>55</v>
@@ -1613,146 +1571,148 @@
         <v>58</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="T5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="V5" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AL5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AW5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX5" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA5" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="BB5" s="1" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>55</v>
@@ -1767,148 +1727,148 @@
         <v>58</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="T6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="V6" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="Y6" s="1"/>
       <c r="Z6" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AL6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AW6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA6" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="BB6" s="1" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>55</v>
@@ -1923,159 +1883,148 @@
         <v>58</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="T7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="V7" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="Y7" s="1"/>
       <c r="Z7" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP7" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AL7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AP7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AR7" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="AS7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV7" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AW7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX7" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA7" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="BB7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BC7" s="5">
-        <v>43687</v>
-      </c>
-      <c r="BD7" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BE7" s="1" t="s">
-        <v>80</v>
+        <v>146</v>
       </c>
     </row>
     <row ht="29" r="8" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -2116,13 +2065,13 @@
       <c r="AL8" s="8"/>
       <c r="AM8" s="8"/>
       <c r="AN8" s="1" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8"/>
       <c r="AQ8" s="8"/>
       <c r="AR8" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="AS8" s="8"/>
       <c r="AT8" s="8"/>
@@ -2130,7 +2079,7 @@
       <c r="AV8" s="8"/>
       <c r="AW8" s="8"/>
       <c r="AX8" s="1" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="AY8" s="8"/>
       <c r="AZ8" s="8"/>
@@ -2138,7 +2087,7 @@
       <c r="BB8" s="8"/>
       <c r="BC8" s="8"/>
       <c r="BF8" s="8" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2175,28 +2124,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="G1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="I1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="J1" t="s">
         <v>39</v>
@@ -2207,81 +2156,81 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2527,30 +2476,30 @@
         <v>53</v>
       </c>
       <c r="BC1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="BD1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="BE1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="BF1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="BG1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="BH1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="BI1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
@@ -2560,7 +2509,7 @@
       <c r="AB2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AN2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AQ2" s="5"/>
       <c r="AR2">
@@ -2575,7 +2524,7 @@
     </row>
     <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
@@ -2585,7 +2534,7 @@
       <c r="AB3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AN3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AQ3" s="5"/>
       <c r="AR3">
@@ -2600,7 +2549,7 @@
     </row>
     <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
@@ -2610,7 +2559,7 @@
       <c r="AB4" s="5"/>
       <c r="AL4" s="5"/>
       <c r="AN4" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AQ4" s="5"/>
       <c r="AR4">
@@ -2623,30 +2572,30 @@
         <v>3259228</v>
       </c>
       <c r="BC4" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="BD4" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="BE4" s="6" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="BF4" s="2" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="BG4" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="BH4" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="BI4" s="6" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
@@ -2656,7 +2605,7 @@
       <c r="AB5" s="5"/>
       <c r="AL5" s="5"/>
       <c r="AN5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="AQ5" s="5"/>
       <c r="AR5">
@@ -2669,30 +2618,30 @@
         <v>3259228</v>
       </c>
       <c r="BC5" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="BD5" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="BE5" s="6" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="BF5" s="2" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="BG5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="BH5" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="BI5" s="6" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="D6" s="4"/>
       <c r="M6" s="5"/>
@@ -2730,13 +2679,13 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G1" t="s">
         <v>44</v>
@@ -2744,22 +2693,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="F2" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="G2" s="4">
         <v>80572.460000000006</v>

</xml_diff>

<commit_message>
Updated Driver Quit when failure occurs
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C8A039-0ED5-46E1-96F6-29CF3F33B4E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A3C8A039-0ED5-46E1-96F6-29CF3F33B4E7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
-    <sheet name="Manage_Calendar_Events" sheetId="7" r:id="rId2"/>
-    <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
-    <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
+    <sheet name="Talent_Acquisition" r:id="rId1" sheetId="2"/>
+    <sheet name="Manage_Calendar_Events" r:id="rId2" sheetId="7"/>
+    <sheet name="Employee_Details" r:id="rId3" sheetId="5"/>
+    <sheet name="Line_Manager" r:id="rId4" sheetId="8"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="164">
   <si>
     <t>scenario</t>
   </si>
@@ -521,6 +521,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,25 +549,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="15" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -583,10 +584,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -750,21 +751,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -781,7 +782,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -833,15 +834,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:BF8"/>
@@ -849,63 +850,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="21.453125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="26.26953125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="33.1796875" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="4.81640625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="26.54296875" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="17.1796875" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="24.54296875" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.35">
@@ -1084,7 +1085,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="2" s="1" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -2020,7 +2021,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
+    <row ht="29" r="8" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>156</v>
       </c>
@@ -2089,14 +2090,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -2104,17 +2105,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.26953125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="5.54296875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2232,14 +2233,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BI6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BJ6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -2247,67 +2248,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="6.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="26.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="33.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="36.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="8.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="21.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="10.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="29.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="49.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.453125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="7.1796875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="27.81640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="25.1796875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="20.26953125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="26.81640625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="33.453125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="36.26953125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="21.7265625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="13.81640625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="29.453125" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.35">
@@ -2652,13 +2653,13 @@
       <c r="BI6" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -2713,7 +2714,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Validate address format test scenario for cognizant instance.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B633D-F0BA-4B24-A8EA-23CB64713694}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03121093-3F65-4D05-A35C-FA3D767D8373}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="189">
   <si>
     <t>scenario</t>
   </si>
@@ -625,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -633,7 +633,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -923,68 +922,68 @@
       <selection activeCell="AR8" sqref="AR8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="14.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,20 +1146,20 @@
       <c r="BB1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="7" t="s">
+      <c r="BC1" t="s">
         <v>155</v>
       </c>
-      <c r="BD1" s="7" t="s">
+      <c r="BD1" t="s">
         <v>156</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BE1" t="s">
         <v>157</v>
       </c>
-      <c r="BF1" s="7" t="s">
+      <c r="BF1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -1465,7 +1464,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1929,7 +1928,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -2096,71 +2095,71 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:58" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
       <c r="AN8" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
       <c r="AR8" t="s">
         <v>179</v>
       </c>
-      <c r="AS8" s="8"/>
-      <c r="AT8" s="8"/>
-      <c r="AU8" s="8"/>
-      <c r="AV8" s="8"/>
-      <c r="AW8" s="8"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="7"/>
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="7"/>
       <c r="AX8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AY8" s="8"/>
-      <c r="AZ8" s="8"/>
-      <c r="BA8" s="8"/>
-      <c r="BB8" s="8"/>
-      <c r="BC8" s="8"/>
-      <c r="BF8" s="8" t="s">
+      <c r="AY8" s="7"/>
+      <c r="AZ8" s="7"/>
+      <c r="BA8" s="7"/>
+      <c r="BB8" s="7"/>
+      <c r="BC8" s="7"/>
+      <c r="BF8" s="7" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2178,22 +2177,22 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -2263,7 +2262,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>123</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2317,76 +2316,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BM8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
-      <selection activeCell="BN3" sqref="BN3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="49.15625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="7.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="27.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="25.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.15625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="6.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="20.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="26.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="33" max="33" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="33.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="36.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="36.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="8.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="21.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="46" max="46" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="48" max="48" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="10.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="29.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="18.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="8.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="56" max="56" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="9.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="10.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="16.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="12.83984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2583,7 +2582,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -2608,7 +2607,7 @@
         <v>3259228</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>3040301</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2679,7 +2678,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2725,7 +2724,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -2734,12 +2733,18 @@
       <c r="U6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AL6" s="5"/>
+      <c r="AN6" t="s">
+        <v>185</v>
+      </c>
       <c r="AQ6" s="5"/>
+      <c r="AX6">
+        <v>10171</v>
+      </c>
       <c r="BE6" s="6"/>
       <c r="BF6" s="2"/>
       <c r="BI6" s="6"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>180</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>48382</v>
       </c>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -2786,9 +2791,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2811,7 +2816,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Code for P17 and inprogress for P26
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B633D-F0BA-4B24-A8EA-23CB64713694}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73554CB6-9E6C-4AB2-AE4B-FE46A5A4B489}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="203">
   <si>
     <t>scenario</t>
   </si>
@@ -590,16 +590,66 @@
   </si>
   <si>
     <t>ADD_EMERGENCY_CONTACT_DETAILS</t>
+  </si>
+  <si>
+    <t>familyName</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>phoneType</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>emailType</t>
+  </si>
+  <si>
+    <t>Adamo Ave</t>
+  </si>
+  <si>
+    <t>altWorkLocationAddressLine2</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Work Mobile Phone</t>
+  </si>
+  <si>
+    <t>Work Email</t>
+  </si>
+  <si>
+    <t>Thomas.Edward@cognizant.com</t>
+  </si>
+  <si>
+    <t>6323145</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -622,10 +672,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -637,8 +688,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2315,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BM8"/>
+  <dimension ref="A1:BW8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
-      <selection activeCell="BN3" sqref="BN3"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BQ5" sqref="BQ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,7 +2439,7 @@
     <col min="61" max="61" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2574,16 +2627,46 @@
         <v>181</v>
       </c>
       <c r="BK1" t="s">
+        <v>195</v>
+      </c>
+      <c r="BL1" t="s">
         <v>186</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>182</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>183</v>
       </c>
+      <c r="BO1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>193</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -2608,7 +2691,7 @@
         <v>3259228</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2633,7 +2716,7 @@
         <v>3040301</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2679,7 +2762,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2725,7 +2808,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -2739,7 +2822,7 @@
       <c r="BF6" s="2"/>
       <c r="BI6" s="6"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>180</v>
       </c>
@@ -2753,16 +2836,19 @@
         <v>184</v>
       </c>
       <c r="BK7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BL7" t="s">
         <v>187</v>
       </c>
-      <c r="BL7" t="s">
+      <c r="BM7" t="s">
         <v>63</v>
       </c>
-      <c r="BM7">
+      <c r="BN7">
         <v>48382</v>
       </c>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -2772,8 +2858,38 @@
       <c r="AX8">
         <v>10171</v>
       </c>
+      <c r="BO8" t="s">
+        <v>196</v>
+      </c>
+      <c r="BP8" t="s">
+        <v>197</v>
+      </c>
+      <c r="BQ8" t="s">
+        <v>198</v>
+      </c>
+      <c r="BR8" t="s">
+        <v>76</v>
+      </c>
+      <c r="BS8" t="s">
+        <v>199</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>64</v>
+      </c>
+      <c r="BU8" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>200</v>
+      </c>
+      <c r="BW8" s="9" t="s">
+        <v>201</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="BW8" r:id="rId1" xr:uid="{A4719649-DD91-42CA-9ADF-E14D69C0891D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2840,12 +2956,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3082,24 +3204,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3124,11 +3242,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Datasheet with common data, added Demo features
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{A3C8A039-0ED5-46E1-96F6-29CF3F33B4E7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36824AB1-5DEE-4DB7-A8D9-33188CF4FBF3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Talent_Acquisition" r:id="rId1" sheetId="2"/>
-    <sheet name="Manage_Calendar_Events" r:id="rId2" sheetId="7"/>
-    <sheet name="Employee_Details" r:id="rId3" sheetId="5"/>
-    <sheet name="Line_Manager" r:id="rId4" sheetId="8"/>
+    <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
+    <sheet name="Manage_Calendar_Events" sheetId="7" r:id="rId2"/>
+    <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
+    <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="188">
   <si>
     <t>scenario</t>
   </si>
@@ -190,9 +190,6 @@
     <t>LOGIN_LOGOUT</t>
   </si>
   <si>
-    <t>527 Johns Avenue</t>
-  </si>
-  <si>
     <t>Suite 436</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
     <t>Bilingual Indicator</t>
   </si>
   <si>
-    <t>ADP Auto &amp; Home</t>
-  </si>
-  <si>
     <t>uatnewhire67@abc.com</t>
   </si>
   <si>
@@ -463,9 +457,6 @@
     <t>HCM.USER</t>
   </si>
   <si>
-    <t>10001</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -493,9 +484,6 @@
     <t>BT Financial Sales</t>
   </si>
   <si>
-    <t>UPDATE_REMOVE_I9_STATUS</t>
-  </si>
-  <si>
     <t>Ready to verify</t>
   </si>
   <si>
@@ -511,17 +499,100 @@
     <t>Career Progression</t>
   </si>
   <si>
-    <t>Hire Part-time Employee</t>
-  </si>
-  <si>
-    <t>500071</t>
+    <t>500103</t>
+  </si>
+  <si>
+    <t>Test Street</t>
+  </si>
+  <si>
+    <t>COMP_ELEMENT</t>
+  </si>
+  <si>
+    <t>Hire</t>
+  </si>
+  <si>
+    <t>94568</t>
+  </si>
+  <si>
+    <t>UPDATE_I9_STATUS</t>
+  </si>
+  <si>
+    <t>United States Hourly Salary Basis</t>
+  </si>
+  <si>
+    <t>NEW_ADDRESS_ALTERNATIVE_WORK_LOCATION</t>
+  </si>
+  <si>
+    <t>test2019</t>
+  </si>
+  <si>
+    <t>Crescent Loop Dr</t>
+  </si>
+  <si>
+    <t>Adamo Ave</t>
+  </si>
+  <si>
+    <t>Alternate work Location Address</t>
+  </si>
+  <si>
+    <t>ADD_EMERGENCY_CONTACT_DETAILS</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Work Mobile Phone</t>
+  </si>
+  <si>
+    <t>Work Email</t>
+  </si>
+  <si>
+    <t>Thomas.Edward@cognizant.com</t>
+  </si>
+  <si>
+    <t>altWorkLocationAddressLine1</t>
+  </si>
+  <si>
+    <t>altWorkLocationAddressLine2</t>
+  </si>
+  <si>
+    <t>altWorkLocationAddressType</t>
+  </si>
+  <si>
+    <t>altWorkLocationCountry</t>
+  </si>
+  <si>
+    <t>altWorkLocationZipCode</t>
+  </si>
+  <si>
+    <t>familyName</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>phoneType</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>emailType</t>
+  </si>
+  <si>
+    <t>locationContact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,25 +620,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="15" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -584,10 +655,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -751,21 +822,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -782,7 +853,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -834,79 +905,79 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:BF8"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="BF8" sqref="BF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.453125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="21.453125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="33.1796875" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="4.81640625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="26.54296875" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="24.54296875" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
+    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.35">
@@ -1031,7 +1102,7 @@
         <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="AP1" t="s">
         <v>41</v>
@@ -1073,168 +1144,168 @@
         <v>53</v>
       </c>
       <c r="BC1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE1" t="s">
         <v>139</v>
       </c>
-      <c r="BD1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>141</v>
-      </c>
       <c r="BF1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT2" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB2" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="BC2"/>
       <c r="BD2"/>
@@ -1243,787 +1314,787 @@
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="V3" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA3" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="AE3" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AL3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP3" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AQ3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AN3" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT3" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AW3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AV3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW3" s="1" t="s">
+      <c r="AX3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AY3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AX3" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AY3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AZ3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="BB3" s="1" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="T4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="V4" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA4" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="AE4" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AL4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP4" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AQ4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AN4" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AO4" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT4" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU4" s="1" t="s">
+      <c r="AW4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AV4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW4" s="1" t="s">
+      <c r="AX4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AY4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AX4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AY4" s="1" t="s">
+      <c r="AZ4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AZ4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA4" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="BB4" s="1" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="T5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="V5" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="AE5" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AL5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AQ5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AN5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AO5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>159</v>
-      </c>
-      <c r="AS5" s="1" t="s">
+      <c r="AT5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT5" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU5" s="1" t="s">
+      <c r="AW5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AV5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW5" s="1" t="s">
+      <c r="AX5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AY5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AX5" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AY5" s="1" t="s">
+      <c r="AZ5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AZ5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA5" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="BB5" s="1" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="T6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="V6" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA6" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="AE6" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AL6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP6" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AM6" s="1" t="s">
+      <c r="AQ6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AN6" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AS6" s="1" t="s">
+      <c r="AT6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU6" s="1" t="s">
+      <c r="AW6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AV6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW6" s="1" t="s">
+      <c r="AX6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AY6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AX6" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AY6" s="1" t="s">
+      <c r="AZ6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AZ6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA6" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="BB6" s="1" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="T7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="V7" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA7" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="AE7" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AL7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AM7" s="1" t="s">
+      <c r="AQ7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AN7" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AO7" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AP7" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>159</v>
-      </c>
-      <c r="AS7" s="1" t="s">
+      <c r="AT7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU7" s="1" t="s">
+      <c r="AW7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AV7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW7" s="1" t="s">
+      <c r="AX7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AY7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AX7" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AY7" s="1" t="s">
+      <c r="AZ7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AZ7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA7" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="BB7" s="1" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
-    <row ht="29" r="8" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2064,13 +2135,13 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
       <c r="AQ8" s="7"/>
       <c r="AR8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="7"/>
@@ -2078,7 +2149,7 @@
       <c r="AV8" s="7"/>
       <c r="AW8" s="7"/>
       <c r="AX8" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AY8" s="7"/>
       <c r="AZ8" s="7"/>
@@ -2086,18 +2157,18 @@
       <c r="BB8" s="7"/>
       <c r="BC8" s="7"/>
       <c r="BF8" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -2105,17 +2176,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2123,28 +2194,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>96</v>
-      </c>
-      <c r="H1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>98</v>
       </c>
       <c r="J1" t="s">
         <v>39</v>
@@ -2155,163 +2226,175 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BJ6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BW8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="AI8" sqref="AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="49.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="7.1796875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="27.81640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="25.1796875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="20.26953125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="26.81640625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="33.453125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="36.26953125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="21.7265625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.81640625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="5.54296875" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="29.453125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="1" max="1" width="51.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.6328125" customWidth="1"/>
+    <col min="63" max="63" width="26.90625" customWidth="1"/>
+    <col min="64" max="64" width="18.54296875" customWidth="1"/>
+    <col min="65" max="65" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="8" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:75" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2475,30 +2558,72 @@
         <v>53</v>
       </c>
       <c r="BC1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BE1" t="s">
         <v>114</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>115</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>116</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BH1" t="s">
         <v>117</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
         <v>118</v>
       </c>
-      <c r="BH1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>120</v>
+      <c r="BJ1" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="BM1" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="BN1" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="BR1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="BS1" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="BT1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BU1" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="BV1" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="BW1" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
@@ -2507,8 +2632,8 @@
       <c r="U2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AL2" s="5"/>
-      <c r="AN2" t="s">
-        <v>78</v>
+      <c r="AN2" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="AQ2" s="5"/>
       <c r="AR2">
@@ -2517,13 +2642,16 @@
       <c r="AS2" s="4">
         <v>80000</v>
       </c>
-      <c r="AX2">
-        <v>3259228</v>
+      <c r="AT2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
@@ -2532,8 +2660,8 @@
       <c r="U3" s="5"/>
       <c r="AB3" s="5"/>
       <c r="AL3" s="5"/>
-      <c r="AN3" t="s">
-        <v>78</v>
+      <c r="AN3" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="AQ3" s="5"/>
       <c r="AR3">
@@ -2542,13 +2670,16 @@
       <c r="AS3" s="4">
         <v>80000</v>
       </c>
-      <c r="AX3">
-        <v>3040301</v>
+      <c r="AT3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
@@ -2557,8 +2688,8 @@
       <c r="U4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AL4" s="5"/>
-      <c r="AN4" t="s">
-        <v>78</v>
+      <c r="AN4" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="AQ4" s="5"/>
       <c r="AR4">
@@ -2567,34 +2698,37 @@
       <c r="AS4">
         <v>15</v>
       </c>
-      <c r="AX4">
-        <v>3259228</v>
+      <c r="AT4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="BC4" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE4" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BF4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="BE4" s="6" t="s">
+      <c r="BG4" t="s">
         <v>123</v>
       </c>
-      <c r="BF4" s="2" t="s">
+      <c r="BH4" t="s">
         <v>124</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BI4" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="BH4" t="s">
-        <v>126</v>
-      </c>
-      <c r="BI4" s="6" t="s">
-        <v>127</v>
-      </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
@@ -2603,8 +2737,8 @@
       <c r="U5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AL5" s="5"/>
-      <c r="AN5" t="s">
-        <v>78</v>
+      <c r="AN5" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="AQ5" s="5"/>
       <c r="AR5">
@@ -2613,53 +2747,320 @@
       <c r="AS5">
         <v>15</v>
       </c>
-      <c r="AX5">
-        <v>3259228</v>
+      <c r="AT5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AX5" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="BC5" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="BD5" t="s">
+      <c r="BF5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="BE5" s="6" t="s">
+      <c r="BG5" t="s">
         <v>123</v>
       </c>
-      <c r="BF5" s="2" t="s">
+      <c r="BH5" t="s">
         <v>124</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="BI5" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="BH5" t="s">
+    </row>
+    <row r="6" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="BI5" s="6" t="s">
-        <v>127</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
+      <c r="AN6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AO6" s="7"/>
+      <c r="AP6" s="7"/>
+      <c r="AQ6" s="7"/>
+      <c r="AR6" s="7"/>
+      <c r="AS6" s="7"/>
+      <c r="AT6" s="7"/>
+      <c r="AU6" s="7"/>
+      <c r="AV6" s="7"/>
+      <c r="AW6" s="7"/>
+      <c r="AX6" s="7">
+        <v>10171</v>
+      </c>
+      <c r="AY6" s="7"/>
+      <c r="AZ6" s="7"/>
+      <c r="BA6" s="7"/>
+      <c r="BB6" s="7"/>
+      <c r="BC6" s="7"/>
+      <c r="BD6" s="7"/>
+      <c r="BE6" s="7"/>
+      <c r="BF6" s="7"/>
+      <c r="BG6" s="7"/>
+      <c r="BH6" s="7"/>
+      <c r="BI6" s="7"/>
+      <c r="BJ6" s="7"/>
+      <c r="BK6" s="7"/>
+      <c r="BL6" s="7"/>
+      <c r="BM6" s="7"/>
+      <c r="BN6" s="7"/>
+      <c r="BO6" s="7"/>
+      <c r="BP6" s="7"/>
+      <c r="BQ6" s="7"/>
+      <c r="BR6" s="7"/>
+      <c r="BS6" s="7"/>
+      <c r="BT6" s="7"/>
+      <c r="BU6" s="7"/>
+      <c r="BV6" s="7"/>
+      <c r="BW6" s="7"/>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="M6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AL6" s="5"/>
-      <c r="AQ6" s="5"/>
-      <c r="BE6" s="6"/>
-      <c r="BF6" s="2"/>
-      <c r="BI6" s="6"/>
+    <row r="7" spans="1:75" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
+      <c r="AN7" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AO7" s="7"/>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="7"/>
+      <c r="AS7" s="7"/>
+      <c r="AT7" s="7"/>
+      <c r="AU7" s="7"/>
+      <c r="AV7" s="7"/>
+      <c r="AW7" s="7"/>
+      <c r="AX7" s="7">
+        <v>10171</v>
+      </c>
+      <c r="AY7" s="7"/>
+      <c r="AZ7" s="7"/>
+      <c r="BA7" s="7"/>
+      <c r="BB7" s="7"/>
+      <c r="BC7" s="7"/>
+      <c r="BD7" s="7"/>
+      <c r="BE7" s="7"/>
+      <c r="BF7" s="7"/>
+      <c r="BG7" s="7"/>
+      <c r="BH7" s="7"/>
+      <c r="BI7" s="7"/>
+      <c r="BJ7" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="BK7" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="BL7" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="BM7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="BN7" s="7">
+        <v>48382</v>
+      </c>
+      <c r="BO7" s="7"/>
+      <c r="BP7" s="7"/>
+      <c r="BQ7" s="7"/>
+      <c r="BR7" s="7"/>
+      <c r="BS7" s="7"/>
+      <c r="BT7" s="7"/>
+      <c r="BU7" s="7"/>
+      <c r="BV7" s="7"/>
+      <c r="BW7" s="7"/>
+    </row>
+    <row r="8" spans="1:75" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="7"/>
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="7"/>
+      <c r="AX8" s="7">
+        <v>10171</v>
+      </c>
+      <c r="AY8" s="7"/>
+      <c r="AZ8" s="7"/>
+      <c r="BA8" s="7"/>
+      <c r="BB8" s="7"/>
+      <c r="BC8" s="7"/>
+      <c r="BD8" s="7"/>
+      <c r="BE8" s="7"/>
+      <c r="BF8" s="7"/>
+      <c r="BG8" s="7"/>
+      <c r="BH8" s="7"/>
+      <c r="BI8" s="7"/>
+      <c r="BJ8" s="7"/>
+      <c r="BK8" s="7"/>
+      <c r="BL8" s="7"/>
+      <c r="BM8" s="7"/>
+      <c r="BN8" s="7"/>
+      <c r="BO8" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="BP8" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BQ8" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="BR8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS8" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="BT8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="BU8" s="7">
+        <v>6323145</v>
+      </c>
+      <c r="BV8" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="BW8" s="7" t="s">
+        <v>176</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -2678,13 +3079,13 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
         <v>129</v>
-      </c>
-      <c r="E1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F1" t="s">
-        <v>131</v>
       </c>
       <c r="G1" t="s">
         <v>44</v>
@@ -2692,48 +3093,33 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" t="s">
         <v>135</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" t="s">
-        <v>137</v>
       </c>
       <c r="G2" s="4">
         <v>80572.460000000006</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -2966,6 +3352,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2976,16 +3377,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3004,6 +3395,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Scripting Photo update is completed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04752CB9-BD99-4552-8929-61A105A2BABA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E99947-10E2-433F-90B2-1970DC47C914}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="188">
   <si>
     <t>scenario</t>
   </si>
@@ -584,6 +584,9 @@
   </si>
   <si>
     <t>locationContact</t>
+  </si>
+  <si>
+    <t>EMPLOYEE_UPLOADS_A_PHOTO</t>
   </si>
 </sst>
 </file>
@@ -916,68 +919,68 @@
       <selection activeCell="BF8" sqref="BF8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1309,7 +1312,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2089,7 +2092,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2171,22 +2174,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2256,7 +2259,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2308,89 +2311,89 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BV8"/>
+  <dimension ref="A1:BV9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1:AO1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.6328125" customWidth="1"/>
-    <col min="62" max="62" width="26.90625" customWidth="1"/>
-    <col min="63" max="63" width="18.54296875" customWidth="1"/>
-    <col min="64" max="64" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2614,7 +2617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2670,7 +2673,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2719,7 +2722,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2768,7 +2771,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -2850,7 +2853,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:74" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>164</v>
       </c>
@@ -2942,7 +2945,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:74" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -3042,6 +3045,88 @@
         <v>175</v>
       </c>
     </row>
+    <row r="9" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="7"/>
+      <c r="AM9" s="7"/>
+      <c r="AN9" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="AO9" s="7"/>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="7"/>
+      <c r="AS9" s="7"/>
+      <c r="AT9" s="7"/>
+      <c r="AU9" s="7"/>
+      <c r="AV9" s="7"/>
+      <c r="AW9" s="7">
+        <v>10171</v>
+      </c>
+      <c r="AX9" s="7"/>
+      <c r="AY9" s="7"/>
+      <c r="AZ9" s="7"/>
+      <c r="BA9" s="7"/>
+      <c r="BB9" s="7"/>
+      <c r="BC9" s="7"/>
+      <c r="BD9" s="7"/>
+      <c r="BE9" s="7"/>
+      <c r="BF9" s="7"/>
+      <c r="BG9" s="7"/>
+      <c r="BH9" s="7"/>
+      <c r="BI9" s="7"/>
+      <c r="BJ9" s="7"/>
+      <c r="BK9" s="7"/>
+      <c r="BL9" s="7"/>
+      <c r="BM9" s="7"/>
+      <c r="BN9" s="7"/>
+      <c r="BO9" s="7"/>
+      <c r="BP9" s="7"/>
+      <c r="BQ9" s="7"/>
+      <c r="BR9" s="7"/>
+      <c r="BS9" s="7"/>
+      <c r="BT9" s="7"/>
+      <c r="BU9" s="7"/>
+      <c r="BV9" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3056,9 +3141,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3081,7 +3166,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3110,30 +3195,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3366,25 +3427,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3401,4 +3468,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Scripted 2nd test case
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E99947-10E2-433F-90B2-1970DC47C914}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4421C088-5A70-485F-BE50-B49F09948518}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="192">
   <si>
     <t>scenario</t>
   </si>
@@ -587,6 +587,18 @@
   </si>
   <si>
     <t>EMPLOYEE_UPLOADS_A_PHOTO</t>
+  </si>
+  <si>
+    <t>Active - No Payroll</t>
+  </si>
+  <si>
+    <t>Assignment Change</t>
+  </si>
+  <si>
+    <t>CHANGE_ASSIGNMENT_VIA_PRSN_MGMNT</t>
+  </si>
+  <si>
+    <t>assignmentStatus</t>
   </si>
 </sst>
 </file>
@@ -915,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF8"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="BF8" sqref="BF8"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,11 +2323,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BV9"/>
+  <dimension ref="A1:BW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="BR4" sqref="BR4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2391,9 +2403,10 @@
     <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2616,8 +2629,11 @@
       <c r="BV1" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="BW1" s="7" t="s">
+        <v>191</v>
+      </c>
     </row>
-    <row r="2" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2645,7 +2661,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2673,7 +2689,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2722,7 +2738,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2771,7 +2787,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -2853,7 +2869,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>164</v>
       </c>
@@ -2945,7 +2961,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -3045,7 +3061,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:74" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>187</v>
       </c>
@@ -3127,6 +3143,26 @@
       <c r="BU9" s="7"/>
       <c r="BV9" s="7"/>
     </row>
+    <row r="10" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="S10" t="s">
+        <v>189</v>
+      </c>
+      <c r="T10" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN10" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>142</v>
+      </c>
+      <c r="BW10" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3195,6 +3231,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3427,31 +3487,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3468,22 +3522,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Work in progress code for HDL data load
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04752CB9-BD99-4552-8929-61A105A2BABA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BE6FDC-FCB2-4E83-BB8B-126FFA997451}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="190">
   <si>
     <t>scenario</t>
   </si>
@@ -584,6 +584,15 @@
   </si>
   <si>
     <t>locationContact</t>
+  </si>
+  <si>
+    <t>UPLOAD_HDL_FILE</t>
+  </si>
+  <si>
+    <t>hdlFilePath</t>
+  </si>
+  <si>
+    <t>"C:\\Users\\4rven\\OneDrive\\Desktop\\Oracle Cloud\\HDL\\Testdata\\Salary.zip"</t>
   </si>
 </sst>
 </file>
@@ -916,68 +925,68 @@
       <selection activeCell="BF8" sqref="BF8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1153,7 +1162,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1309,7 +1318,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1465,7 +1474,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1621,7 +1630,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1933,7 +1942,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2089,7 +2098,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2171,22 +2180,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2221,7 +2230,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2256,7 +2265,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2279,7 +2288,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2308,89 +2317,89 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BV8"/>
+  <dimension ref="A1:BW9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1:AO1048576"/>
+    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="BX8" sqref="BX8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.6328125" customWidth="1"/>
-    <col min="62" max="62" width="26.90625" customWidth="1"/>
-    <col min="63" max="63" width="18.54296875" customWidth="1"/>
-    <col min="64" max="64" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:75" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2613,8 +2622,11 @@
       <c r="BV1" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="BW1" s="7" t="s">
+        <v>188</v>
+      </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2642,7 +2654,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2670,7 +2682,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2719,7 +2731,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2768,7 +2780,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -2850,7 +2862,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:74" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:75" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>164</v>
       </c>
@@ -2942,7 +2954,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:74" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:75" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -3009,11 +3021,21 @@
       <c r="BF8" s="7"/>
       <c r="BG8" s="7"/>
       <c r="BH8" s="7"/>
-      <c r="BI8" s="7"/>
-      <c r="BJ8" s="7"/>
-      <c r="BK8" s="7"/>
-      <c r="BL8" s="7"/>
-      <c r="BM8" s="7"/>
+      <c r="BI8" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BJ8" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="BK8" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="BL8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BM8" s="7">
+        <v>48382</v>
+      </c>
       <c r="BN8" s="7" t="s">
         <v>170</v>
       </c>
@@ -3040,6 +3062,20 @@
       </c>
       <c r="BV8" s="7" t="s">
         <v>175</v>
+      </c>
+      <c r="BW8" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3056,9 +3092,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3081,7 +3117,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
Updated file path variable
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E42D3E1-194C-4CF8-88D2-44BB54CCED79}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC34CD9-89AB-46E3-AA41-54561688548E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="195">
   <si>
     <t>scenario</t>
   </si>
@@ -602,6 +602,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>C:\\testdata\\TestImage.jpg</t>
+  </si>
+  <si>
+    <t>filePath</t>
   </si>
 </sst>
 </file>
@@ -637,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -647,6 +653,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,68 +943,68 @@
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1180,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1327,7 +1336,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1483,7 +1492,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1639,7 +1648,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1951,7 +1960,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2107,7 +2116,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2189,22 +2198,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2239,7 +2248,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2274,7 +2283,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2297,7 +2306,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2326,90 +2335,91 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BW11"/>
+  <dimension ref="A1:BX11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BP1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="BW4" sqref="BW4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.6328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5546875" customWidth="1"/>
-    <col min="62" max="62" width="26.88671875" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" customWidth="1"/>
-    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.54296875" customWidth="1"/>
+    <col min="62" max="62" width="26.90625" customWidth="1"/>
+    <col min="63" max="63" width="18.54296875" customWidth="1"/>
+    <col min="64" max="64" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="24.36328125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2635,8 +2645,11 @@
       <c r="BW1" s="7" t="s">
         <v>191</v>
       </c>
+      <c r="BX1" s="7" t="s">
+        <v>194</v>
+      </c>
     </row>
-    <row r="2" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2664,7 +2677,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2692,7 +2705,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2741,7 +2754,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2790,7 +2803,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -2872,7 +2885,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>164</v>
       </c>
@@ -2964,7 +2977,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -3064,7 +3077,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:76" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>187</v>
       </c>
@@ -3145,8 +3158,11 @@
       <c r="BT9" s="7"/>
       <c r="BU9" s="7"/>
       <c r="BV9" s="7"/>
+      <c r="BX9" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
-    <row r="10" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>190</v>
       </c>
@@ -3166,7 +3182,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:75" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>192</v>
       </c>
@@ -3185,9 +3201,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3210,7 +3226,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3239,30 +3255,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3495,25 +3487,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3530,4 +3528,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated global assignment date logic
Signed-off-by: Raghavendran Ramasubramanian <raghavendran.r1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E37035-6C81-4EA4-91EE-AC71D6CBAE90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0EB15-3102-4762-B086-7104119FEA0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -619,10 +619,10 @@
     <t>assignmentStatus</t>
   </si>
   <si>
-    <t>C:\\Users\\4rven\\OneDrive\\Desktop\\Oracle Cloud\\HDL\\Testdata\\Salary.zip</t>
-  </si>
-  <si>
-    <t>Harris HDLNEWHIRE</t>
+    <t>C:\\testdata\\Salary.zip</t>
+  </si>
+  <si>
+    <t>Matt HDLNEWHIRE</t>
   </si>
 </sst>
 </file>
@@ -955,71 +955,71 @@
   <dimension ref="A1:BF9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -2369,22 +2369,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2508,88 +2508,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
       <selection activeCell="BX9" sqref="BX9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5703125" customWidth="1"/>
-    <col min="62" max="62" width="26.85546875" customWidth="1"/>
-    <col min="63" max="63" width="18.5703125" customWidth="1"/>
-    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.54296875" customWidth="1"/>
+    <col min="62" max="62" width="26.81640625" customWidth="1"/>
+    <col min="63" max="63" width="18.54296875" customWidth="1"/>
+    <col min="64" max="64" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5703125" customWidth="1"/>
+    <col min="75" max="75" width="42.54296875" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -3058,7 +3058,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>164</v>
       </c>
@@ -3150,7 +3150,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>187</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>192</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>193</v>
       </c>
@@ -3326,9 +3326,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3380,12 +3380,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3622,24 +3628,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3664,11 +3666,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Personal Information xpath issue fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0EB15-3102-4762-B086-7104119FEA0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670F2A13-3768-47DE-B49C-E46927CCBA0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="202">
   <si>
     <t>scenario</t>
   </si>
@@ -623,6 +623,12 @@
   </si>
   <si>
     <t>Matt HDLNEWHIRE</t>
+  </si>
+  <si>
+    <t>Cloud123</t>
+  </si>
+  <si>
+    <t>sangameshwar.balur</t>
   </si>
 </sst>
 </file>
@@ -958,68 +964,68 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1201,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1351,7 +1357,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1507,7 +1513,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1663,7 +1669,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1975,7 +1981,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2131,7 +2137,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2199,7 +2205,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -2369,22 +2375,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2425,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2454,7 +2460,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2477,7 +2483,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2508,88 +2514,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BX9" sqref="BX9"/>
+    <sheetView tabSelected="1" topLeftCell="AL3" workbookViewId="0">
+      <selection activeCell="AX10" sqref="AX10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.54296875" customWidth="1"/>
-    <col min="62" max="62" width="26.81640625" customWidth="1"/>
-    <col min="63" max="63" width="18.54296875" customWidth="1"/>
-    <col min="64" max="64" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.54296875" customWidth="1"/>
+    <col min="75" max="75" width="42.5703125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:77" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2850,7 +2856,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2878,7 +2884,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2976,7 +2982,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -3058,7 +3064,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:77" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>164</v>
       </c>
@@ -3150,7 +3156,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:77" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -3261,7 +3267,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>187</v>
       </c>
@@ -3278,21 +3284,21 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:77" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>192</v>
       </c>
       <c r="AN10" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="AW10" s="7">
-        <v>10171</v>
+        <v>200</v>
+      </c>
+      <c r="AW10" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="BW10" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:77" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>193</v>
       </c>
@@ -3326,9 +3332,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3380,18 +3386,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3628,20 +3628,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3666,9 +3670,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
XPaths are updated for unidentified objects and updated logic in few methods
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670F2A13-3768-47DE-B49C-E46927CCBA0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1899F5-F016-41E2-B060-039F30DC7B71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="203">
   <si>
     <t>scenario</t>
   </si>
@@ -514,9 +514,6 @@
     <t>UPDATE_I9_STATUS</t>
   </si>
   <si>
-    <t>United States Hourly Salary Basis</t>
-  </si>
-  <si>
     <t>NEW_ADDRESS_ALTERNATIVE_WORK_LOCATION</t>
   </si>
   <si>
@@ -629,6 +626,12 @@
   </si>
   <si>
     <t>sangameshwar.balur</t>
+  </si>
+  <si>
+    <t>Aarnet.Ebenezer</t>
+  </si>
+  <si>
+    <t>Hourly Salary US</t>
   </si>
 </sst>
 </file>
@@ -644,12 +647,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -664,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -677,6 +686,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -960,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1159,7 @@
         <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AP1" t="s">
         <v>40</v>
@@ -2207,7 +2219,7 @@
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>158</v>
@@ -2284,7 +2296,7 @@
         <v>160</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC9" s="1" t="s">
         <v>139</v>
@@ -2514,8 +2526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL3" workbookViewId="0">
-      <selection activeCell="AX10" sqref="AX10"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2777,55 +2789,55 @@
         <v>117</v>
       </c>
       <c r="BI1" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BK1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BL1" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BM1" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="BN1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="BO1" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="BP1" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="BQ1" s="7" t="s">
         <v>23</v>
       </c>
       <c r="BR1" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="BS1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="BT1" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="BU1" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="BU1" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="BV1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="BW1" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BX1" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="BY1" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.25">
@@ -2840,20 +2852,20 @@
       <c r="AB2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AN2" s="1" t="s">
-        <v>141</v>
+        <v>199</v>
       </c>
       <c r="AP2" s="5"/>
       <c r="AQ2">
-        <v>3001712</v>
+        <v>10043</v>
       </c>
       <c r="AR2" s="4">
         <v>80000</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.25">
@@ -2868,20 +2880,20 @@
       <c r="AB3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AN3" s="1" t="s">
-        <v>141</v>
+        <v>199</v>
       </c>
       <c r="AP3" s="5"/>
       <c r="AQ3">
-        <v>3259949</v>
+        <v>10043</v>
       </c>
       <c r="AR3" s="4">
         <v>80000</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:77" x14ac:dyDescent="0.25">
@@ -2896,20 +2908,20 @@
       <c r="AB4" s="5"/>
       <c r="AL4" s="5"/>
       <c r="AN4" s="1" t="s">
-        <v>141</v>
+        <v>199</v>
       </c>
       <c r="AP4" s="5"/>
       <c r="AQ4">
-        <v>3259949</v>
+        <v>10043</v>
       </c>
       <c r="AR4">
         <v>15</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="AW4" s="1" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="BB4" t="s">
         <v>118</v>
@@ -2945,20 +2957,20 @@
       <c r="AB5" s="5"/>
       <c r="AL5" s="5"/>
       <c r="AN5" s="1" t="s">
-        <v>141</v>
+        <v>199</v>
       </c>
       <c r="AP5" s="5"/>
       <c r="AQ5">
-        <v>3259949</v>
+        <v>10043</v>
       </c>
       <c r="AR5">
         <v>15</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="AW5" s="1" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="BB5" t="s">
         <v>118</v>
@@ -3025,7 +3037,7 @@
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
@@ -3066,7 +3078,7 @@
     </row>
     <row r="7" spans="1:77" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3107,7 +3119,7 @@
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
@@ -3132,13 +3144,13 @@
       <c r="BG7" s="7"/>
       <c r="BH7" s="7"/>
       <c r="BI7" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="BJ7" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="BJ7" s="7" t="s">
+      <c r="BK7" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="BK7" s="7" t="s">
-        <v>168</v>
       </c>
       <c r="BL7" s="7" t="s">
         <v>60</v>
@@ -3158,7 +3170,7 @@
     </row>
     <row r="8" spans="1:77" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3199,7 +3211,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -3224,13 +3236,13 @@
       <c r="BG8" s="7"/>
       <c r="BH8" s="7"/>
       <c r="BI8" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="BJ8" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="BJ8" s="7" t="s">
+      <c r="BK8" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="BK8" s="7" t="s">
-        <v>168</v>
       </c>
       <c r="BL8" s="7" t="s">
         <v>60</v>
@@ -3239,19 +3251,19 @@
         <v>48382</v>
       </c>
       <c r="BN8" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="BO8" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="BO8" s="7" t="s">
+      <c r="BP8" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="BP8" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="BQ8" s="7" t="s">
         <v>68</v>
       </c>
       <c r="BR8" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="BS8" s="7" t="s">
         <v>61</v>
@@ -3260,16 +3272,16 @@
         <v>6323145</v>
       </c>
       <c r="BU8" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="BV8" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="BV8" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="BW8" s="7"/>
     </row>
     <row r="9" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AN9" s="1" t="s">
         <v>141</v>
@@ -3278,44 +3290,42 @@
         <v>142</v>
       </c>
       <c r="BW9" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="BX9" t="s">
         <v>198</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:77" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="AN10" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW10" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="BW10" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="AN10" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="AW10" s="7" t="s">
+      <c r="S11" t="s">
+        <v>193</v>
+      </c>
+      <c r="T11" s="1"/>
+      <c r="AN11" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW11" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="BW10" s="8" t="s">
+      <c r="BY11" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:77" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="S11" t="s">
-        <v>194</v>
-      </c>
-      <c r="T11" t="s">
-        <v>156</v>
-      </c>
-      <c r="AN11" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>142</v>
-      </c>
-      <c r="BY11" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New hire changes on dev instance
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0EB15-3102-4762-B086-7104119FEA0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -14,8 +13,8 @@
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="214">
   <si>
     <t>scenario</t>
   </si>
@@ -623,13 +622,55 @@
   </si>
   <si>
     <t>Matt HDLNEWHIRE</t>
+  </si>
+  <si>
+    <t>koushik.kadimcherla</t>
+  </si>
+  <si>
+    <t>Cloud123</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>GM Temporary Relocation</t>
+  </si>
+  <si>
+    <t>aarnet.ebenezer</t>
+  </si>
+  <si>
+    <t>Hire to fill vacant position</t>
+  </si>
+  <si>
+    <t>Acme Enterprises, US Ltd.</t>
+  </si>
+  <si>
+    <t>75037</t>
+  </si>
+  <si>
+    <t>US BU</t>
+  </si>
+  <si>
+    <t>US_CA_Redwood Shores</t>
+  </si>
+  <si>
+    <t>Quality Assurance-US_CA-ATS US</t>
+  </si>
+  <si>
+    <t>Quality Manager</t>
+  </si>
+  <si>
+    <t>BiWeekly</t>
+  </si>
+  <si>
+    <t>Annual Salary US</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -658,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -670,6 +711,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -944,82 +988,82 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BF9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AW3" sqref="AW3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:58">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1239,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1351,16 +1395,14 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:58" ht="30">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="2" t="s">
         <v>55</v>
       </c>
@@ -1368,7 +1410,7 @@
         <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>57</v>
@@ -1386,16 +1428,16 @@
         <v>61</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>62</v>
+        <v>202</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>149</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>155</v>
+        <v>210</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>206</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>63</v>
@@ -1410,7 +1452,7 @@
         <v>65</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>66</v>
@@ -1433,20 +1475,20 @@
         <v>70</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>139</v>
+        <v>205</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>150</v>
+        <v>211</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>72</v>
@@ -1462,13 +1504,13 @@
         <v>74</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>141</v>
+        <v>201</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>143</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>147</v>
+        <v>212</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>66</v>
@@ -1480,7 +1522,7 @@
         <v>76</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>148</v>
+        <v>213</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>77</v>
@@ -1492,7 +1534,7 @@
         <v>79</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="AY3" s="1" t="s">
         <v>81</v>
@@ -1504,10 +1546,10 @@
         <v>83</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>161</v>
+        <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1663,7 +1705,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1819,7 +1861,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:58">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1975,7 +2017,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:58">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2131,7 +2173,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:58" ht="30">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2199,7 +2241,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:58">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -2362,29 +2404,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.54296875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2461,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2454,7 +2496,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2477,7 +2519,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2505,91 +2547,91 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BX9" sqref="BX9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.54296875" customWidth="1"/>
-    <col min="62" max="62" width="26.81640625" customWidth="1"/>
-    <col min="63" max="63" width="18.54296875" customWidth="1"/>
-    <col min="64" max="64" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.54296875" customWidth="1"/>
+    <col min="75" max="75" width="42.5703125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:77" ht="60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2822,7 +2864,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:77">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2850,7 +2892,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:77">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2878,7 +2920,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:77">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2927,7 +2969,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:77">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2976,7 +3018,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:77" ht="45">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -3019,7 +3061,7 @@
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
@@ -3029,8 +3071,8 @@
       <c r="AT6" s="7"/>
       <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
-      <c r="AW6" s="7">
-        <v>10171</v>
+      <c r="AW6" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
@@ -3058,7 +3100,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:77" ht="45">
       <c r="A7" s="7" t="s">
         <v>164</v>
       </c>
@@ -3101,7 +3143,7 @@
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
@@ -3111,8 +3153,8 @@
       <c r="AT7" s="7"/>
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
-      <c r="AW7" s="7">
-        <v>10171</v>
+      <c r="AW7" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
@@ -3150,7 +3192,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:77" ht="75">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -3193,7 +3235,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -3203,8 +3245,8 @@
       <c r="AT8" s="7"/>
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
-      <c r="AW8" s="7">
-        <v>10171</v>
+      <c r="AW8" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
@@ -3261,7 +3303,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:77">
       <c r="A9" s="7" t="s">
         <v>187</v>
       </c>
@@ -3278,7 +3320,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:77">
       <c r="A10" s="7" t="s">
         <v>192</v>
       </c>
@@ -3292,7 +3334,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:77" ht="30">
       <c r="A11" s="7" t="s">
         <v>193</v>
       </c>
@@ -3319,16 +3361,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3351,7 +3393,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
Added Manager logic in New Hire
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="216">
   <si>
     <t>scenario</t>
   </si>
@@ -664,6 +664,12 @@
   </si>
   <si>
     <t>Annual Salary US</t>
+  </si>
+  <si>
+    <t>managerName</t>
+  </si>
+  <si>
+    <t>Kadimcherla, Koushik</t>
   </si>
 </sst>
 </file>
@@ -988,7 +994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -996,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BF9"/>
+  <dimension ref="A1:BG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AW3" sqref="AW3"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BG3" sqref="BG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1063,7 +1069,7 @@
     <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:59">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1238,8 +1244,11 @@
       <c r="BF1" t="s">
         <v>153</v>
       </c>
+      <c r="BG1" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="2" spans="1:58" s="1" customFormat="1">
+    <row r="2" spans="1:59" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1395,7 +1404,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:58" ht="30">
+    <row r="3" spans="1:59" ht="30">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1548,8 +1557,11 @@
       <c r="BB3" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="BG3" t="s">
+        <v>215</v>
+      </c>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:59">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1705,7 +1717,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:59">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1861,7 +1873,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:59">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -2017,7 +2029,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:59">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2173,7 +2185,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:58" ht="30">
+    <row r="8" spans="1:59" ht="30">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2241,7 +2253,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:59">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -3437,6 +3449,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3669,15 +3690,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
@@ -3689,6 +3701,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3705,12 +3725,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated code for P17 and P26 in new Dev instance
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A690119-33BE-4E8A-A4F6-76996AAF92CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13299B7-8CA6-4912-9203-AD191185A6D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="204">
   <si>
     <t>scenario</t>
   </si>
@@ -517,9 +517,6 @@
     <t>United States Hourly Salary Basis</t>
   </si>
   <si>
-    <t>NEW_ADDRESS_ALTERNATIVE_WORK_LOCATION</t>
-  </si>
-  <si>
     <t>test2019</t>
   </si>
   <si>
@@ -529,12 +526,6 @@
     <t>Adamo Ave</t>
   </si>
   <si>
-    <t>Alternate work Location Address</t>
-  </si>
-  <si>
-    <t>ADD_EMERGENCY_CONTACT_DETAILS</t>
-  </si>
-  <si>
     <t>Thomas</t>
   </si>
   <si>
@@ -623,6 +614,27 @@
   </si>
   <si>
     <t>Helen HDLNEWHIRE</t>
+  </si>
+  <si>
+    <t>Cloud123</t>
+  </si>
+  <si>
+    <t>venkatesan.manivannan</t>
+  </si>
+  <si>
+    <t>Mailing Address</t>
+  </si>
+  <si>
+    <t>High Hammock Dr</t>
+  </si>
+  <si>
+    <t>Causeway Blvd</t>
+  </si>
+  <si>
+    <t>ADD_NEW_EMERGENCY_CONTACT_DETAILS</t>
+  </si>
+  <si>
+    <t>ADD_NEW_ADDRESS_TYPE_DETAILS</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1153,7 @@
         <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AP1" t="s">
         <v>40</v>
@@ -2201,7 +2213,7 @@
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>158</v>
@@ -2278,7 +2290,7 @@
         <v>160</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AC9" s="1" t="s">
         <v>139</v>
@@ -2508,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
-      <selection activeCell="BX9" sqref="BX9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2771,55 +2783,55 @@
         <v>117</v>
       </c>
       <c r="BI1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="BL1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BM1" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="BK1" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="BL1" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="BN1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="BO1" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="BP1" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="BQ1" s="7" t="s">
         <v>23</v>
       </c>
       <c r="BR1" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="BS1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="BT1" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="BU1" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="BV1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="BW1" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="BX1" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="BY1" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.25">
@@ -3019,7 +3031,7 @@
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
@@ -3058,9 +3070,9 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3101,7 +3113,7 @@
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
@@ -3111,8 +3123,8 @@
       <c r="AT7" s="7"/>
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
-      <c r="AW7" s="7">
-        <v>10171</v>
+      <c r="AW7" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
@@ -3126,19 +3138,19 @@
       <c r="BG7" s="7"/>
       <c r="BH7" s="7"/>
       <c r="BI7" s="7" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="BJ7" s="7" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="BK7" s="7" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="BL7" s="7" t="s">
         <v>60</v>
       </c>
       <c r="BM7" s="7">
-        <v>48382</v>
+        <v>28749</v>
       </c>
       <c r="BN7" s="7"/>
       <c r="BO7" s="7"/>
@@ -3152,7 +3164,7 @@
     </row>
     <row r="8" spans="1:77" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3193,7 +3205,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -3203,8 +3215,8 @@
       <c r="AT8" s="7"/>
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
-      <c r="AW8" s="7">
-        <v>10171</v>
+      <c r="AW8" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
@@ -3218,34 +3230,34 @@
       <c r="BG8" s="7"/>
       <c r="BH8" s="7"/>
       <c r="BI8" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="BJ8" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="BJ8" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="BK8" s="7" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="BL8" s="7" t="s">
         <v>60</v>
       </c>
       <c r="BM8" s="7">
-        <v>48382</v>
+        <v>28749</v>
       </c>
       <c r="BN8" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="BO8" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="BP8" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="BQ8" s="7" t="s">
         <v>68</v>
       </c>
       <c r="BR8" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="BS8" s="7" t="s">
         <v>61</v>
@@ -3254,16 +3266,16 @@
         <v>6323145</v>
       </c>
       <c r="BU8" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="BV8" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="BW8" s="7"/>
     </row>
     <row r="9" spans="1:77" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AN9" s="1" t="s">
         <v>141</v>
@@ -3272,32 +3284,32 @@
         <v>142</v>
       </c>
       <c r="BW9" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="BX9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:77" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="AN10" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AW10" s="7">
         <v>10171</v>
       </c>
       <c r="BW10" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:77" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="S11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="T11" t="s">
         <v>156</v>
@@ -3309,7 +3321,7 @@
         <v>142</v>
       </c>
       <c r="BY11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3380,15 +3392,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3621,6 +3624,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3637,14 +3649,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3663,6 +3667,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
1. Changed the person number search hyperlink
2. Changed the text from Zip to ZIP for address validation

3. Changed the address format of hire date
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8AA147-A149-4477-9F4C-89D32C7B26E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,8 +14,8 @@
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="215">
   <si>
     <t>scenario</t>
   </si>
@@ -592,9 +593,6 @@
   </si>
   <si>
     <t>EDIT_SENIORITY_DATE</t>
-  </si>
-  <si>
-    <t>2/4/2019</t>
   </si>
   <si>
     <t>filePath</t>
@@ -675,8 +673,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -994,82 +992,82 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BG3" sqref="BG3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.62890625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1245,10 +1243,10 @@
         <v>153</v>
       </c>
       <c r="BG1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:59" s="1" customFormat="1">
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1404,7 +1402,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:59" ht="30">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1419,7 +1417,7 @@
         <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>57</v>
@@ -1437,16 +1435,16 @@
         <v>61</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>149</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>63</v>
@@ -1461,7 +1459,7 @@
         <v>65</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>66</v>
@@ -1484,20 +1482,20 @@
         <v>70</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>72</v>
@@ -1513,13 +1511,13 @@
         <v>74</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>143</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>66</v>
@@ -1531,7 +1529,7 @@
         <v>76</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>77</v>
@@ -1543,7 +1541,7 @@
         <v>79</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AY3" s="1" t="s">
         <v>81</v>
@@ -1555,13 +1553,13 @@
         <v>83</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BG3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1717,7 +1715,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1873,7 +1871,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -2029,7 +2027,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:59">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2185,7 +2183,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="30">
+    <row r="8" spans="1:59" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2253,161 +2251,66 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:59">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="2"/>
       <c r="W9" s="1"/>
-      <c r="X9" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
-      <c r="AG9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AH9" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI9" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
-      <c r="AK9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL9" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM9" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
       <c r="AN9" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AO9" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AP9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AQ9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR9" t="s">
-        <v>154</v>
-      </c>
-      <c r="AS9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AT9" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AU9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AV9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AW9" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
       <c r="AX9" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AY9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AZ9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BA9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BB9" s="1" t="s">
-        <v>161</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2416,29 +2319,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2473,7 +2376,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2508,7 +2411,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2531,7 +2434,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2559,91 +2462,91 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5703125" customWidth="1"/>
-    <col min="62" max="62" width="26.85546875" customWidth="1"/>
-    <col min="63" max="63" width="18.5703125" customWidth="1"/>
-    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.578125" customWidth="1"/>
+    <col min="62" max="62" width="26.83984375" customWidth="1"/>
+    <col min="63" max="63" width="18.578125" customWidth="1"/>
+    <col min="64" max="64" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.578125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5703125" customWidth="1"/>
+    <col min="75" max="75" width="42.578125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="60">
+    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2867,16 +2770,16 @@
         <v>17</v>
       </c>
       <c r="BW1" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BX1" s="7" t="s">
         <v>188</v>
       </c>
       <c r="BY1" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:77">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2904,7 +2807,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:77">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2932,7 +2835,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:77">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2981,7 +2884,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:77">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3030,7 +2933,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:77" ht="45">
+    <row r="6" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -3073,7 +2976,7 @@
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
@@ -3084,7 +2987,7 @@
       <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
       <c r="AW6" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
@@ -3112,7 +3015,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="45">
+    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>164</v>
       </c>
@@ -3155,7 +3058,7 @@
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
@@ -3166,7 +3069,7 @@
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
       <c r="AW7" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
@@ -3204,7 +3107,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="75">
+    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -3247,7 +3150,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -3258,7 +3161,7 @@
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
       <c r="AW8" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
@@ -3315,7 +3218,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
         <v>187</v>
       </c>
@@ -3326,15 +3229,15 @@
         <v>142</v>
       </c>
       <c r="BW9" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="BX9" t="s">
         <v>198</v>
       </c>
-      <c r="BX9" t="s">
-        <v>199</v>
-      </c>
     </row>
-    <row r="10" spans="1:77">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AN10" s="7" t="s">
         <v>165</v>
@@ -3343,15 +3246,15 @@
         <v>10171</v>
       </c>
       <c r="BW10" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:77" ht="30">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="S11" t="s">
         <v>193</v>
-      </c>
-      <c r="S11" t="s">
-        <v>194</v>
       </c>
       <c r="T11" t="s">
         <v>156</v>
@@ -3363,7 +3266,7 @@
         <v>142</v>
       </c>
       <c r="BY11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3373,16 +3276,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3405,7 +3308,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3434,30 +3337,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3690,25 +3569,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3725,4 +3610,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TestData.xlsx User name and password updated for couple of scenario's features/oracle_fusion_cloud/EmployeeEditMyDetails.feature : Scenario names updated.
java/framework/tests/pages/oracle_fusion_cloud/EmployeeEditMyDetailsPage.java : waituntil condition added for object to be visible.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF88DF54-C45E-432B-886B-9D9DB75C0672}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3717103E-7736-4631-85BA-07C3D71A7892}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -517,9 +517,6 @@
     <t>NEW_ADDRESS_ALTERNATIVE_WORK_LOCATION</t>
   </si>
   <si>
-    <t>test2019</t>
-  </si>
-  <si>
     <t>Crescent Loop Dr</t>
   </si>
   <si>
@@ -674,6 +671,9 @@
   </si>
   <si>
     <t>Aarnet.Ebenezer</t>
+  </si>
+  <si>
+    <t>sangameshwar.balur</t>
   </si>
 </sst>
 </file>
@@ -1012,68 +1012,68 @@
       <selection activeCell="AX2" sqref="AX2:AX9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AP1" t="s">
         <v>40</v>
@@ -1249,10 +1249,10 @@
         <v>153</v>
       </c>
       <c r="BG1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>74</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO2" s="1" t="s">
         <v>143</v>
@@ -1389,7 +1389,7 @@
         <v>79</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY2" s="1" t="s">
         <v>81</v>
@@ -1408,7 +1408,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>57</v>
@@ -1441,16 +1441,16 @@
         <v>61</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>149</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>63</v>
@@ -1465,7 +1465,7 @@
         <v>65</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>66</v>
@@ -1488,20 +1488,20 @@
         <v>70</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>72</v>
@@ -1517,13 +1517,13 @@
         <v>74</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>143</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>66</v>
@@ -1535,7 +1535,7 @@
         <v>76</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>77</v>
@@ -1547,7 +1547,7 @@
         <v>79</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY3" s="1" t="s">
         <v>81</v>
@@ -1559,13 +1559,13 @@
         <v>83</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="BG3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>74</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO4" s="1" t="s">
         <v>143</v>
@@ -1706,7 +1706,7 @@
         <v>79</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY4" s="1" t="s">
         <v>81</v>
@@ -1721,7 +1721,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>74</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO5" s="1" t="s">
         <v>143</v>
@@ -1862,7 +1862,7 @@
         <v>79</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY5" s="1" t="s">
         <v>81</v>
@@ -1877,7 +1877,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>74</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO6" s="1" t="s">
         <v>143</v>
@@ -2018,7 +2018,7 @@
         <v>79</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY6" s="1" t="s">
         <v>81</v>
@@ -2033,7 +2033,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>74</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO7" s="1" t="s">
         <v>143</v>
@@ -2174,7 +2174,7 @@
         <v>79</v>
       </c>
       <c r="AX7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY7" s="1" t="s">
         <v>81</v>
@@ -2189,7 +2189,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:59" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -2246,7 +2246,7 @@
       <c r="AV8" s="7"/>
       <c r="AW8" s="7"/>
       <c r="AX8" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY8" s="7"/>
       <c r="AZ8" s="7"/>
@@ -2257,9 +2257,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>158</v>
@@ -2336,7 +2336,7 @@
         <v>160</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC9" s="1" t="s">
         <v>139</v>
@@ -2368,7 +2368,7 @@
         <v>74</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO9" s="1" t="s">
         <v>143</v>
@@ -2398,7 +2398,7 @@
         <v>79</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AY9" s="1" t="s">
         <v>81</v>
@@ -2427,22 +2427,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2566,88 +2566,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AY9" sqref="AY9"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AN8" sqref="AN8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5546875" customWidth="1"/>
-    <col min="62" max="62" width="26.88671875" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" customWidth="1"/>
-    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5546875" customWidth="1"/>
+    <col min="75" max="75" width="42.5703125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:77" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2829,58 +2829,58 @@
         <v>117</v>
       </c>
       <c r="BI1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BK1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BL1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BM1" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="BN1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="BO1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="BP1" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="BQ1" s="7" t="s">
         <v>23</v>
       </c>
       <c r="BR1" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BS1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="BT1" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="BU1" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="BU1" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="BV1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="BW1" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BX1" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="BY1" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2892,7 +2892,7 @@
       <c r="AB2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AN2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AP2" s="5"/>
       <c r="AQ2">
@@ -2902,13 +2902,13 @@
         <v>80000</v>
       </c>
       <c r="AS2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AW2" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="AW2" s="1" t="s">
-        <v>216</v>
-      </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="AB3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AN3" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AP3" s="5"/>
       <c r="AQ3">
@@ -2930,13 +2930,13 @@
         <v>80000</v>
       </c>
       <c r="AS3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AW3" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="AW3" s="1" t="s">
-        <v>216</v>
-      </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2948,7 +2948,7 @@
       <c r="AB4" s="5"/>
       <c r="AL4" s="5"/>
       <c r="AN4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AP4" s="5"/>
       <c r="AQ4">
@@ -2958,10 +2958,10 @@
         <v>15</v>
       </c>
       <c r="AS4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AW4" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="AW4" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="BB4" t="s">
         <v>118</v>
@@ -2985,7 +2985,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="AB5" s="5"/>
       <c r="AL5" s="5"/>
       <c r="AN5" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AP5" s="5"/>
       <c r="AQ5">
@@ -3007,10 +3007,10 @@
         <v>15</v>
       </c>
       <c r="AS5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AW5" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="AW5" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="BB5" t="s">
         <v>118</v>
@@ -3034,7 +3034,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
@@ -3088,7 +3088,7 @@
       <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
       <c r="AW6" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
@@ -3116,7 +3116,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:77" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>163</v>
       </c>
@@ -3159,7 +3159,7 @@
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
@@ -3170,7 +3170,7 @@
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
       <c r="AW7" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
@@ -3184,13 +3184,13 @@
       <c r="BG7" s="7"/>
       <c r="BH7" s="7"/>
       <c r="BI7" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="BJ7" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="BJ7" s="7" t="s">
+      <c r="BK7" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="BK7" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="BL7" s="7" t="s">
         <v>60</v>
@@ -3208,9 +3208,9 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:77" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3251,7 +3251,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -3262,7 +3262,7 @@
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
       <c r="AW8" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
@@ -3276,13 +3276,13 @@
       <c r="BG8" s="7"/>
       <c r="BH8" s="7"/>
       <c r="BI8" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="BJ8" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="BJ8" s="7" t="s">
+      <c r="BK8" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="BK8" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="BL8" s="7" t="s">
         <v>60</v>
@@ -3291,19 +3291,19 @@
         <v>48382</v>
       </c>
       <c r="BN8" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="BO8" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="BO8" s="7" t="s">
+      <c r="BP8" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="BP8" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="BQ8" s="7" t="s">
         <v>68</v>
       </c>
       <c r="BR8" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="BS8" s="7" t="s">
         <v>61</v>
@@ -3312,16 +3312,16 @@
         <v>6323145</v>
       </c>
       <c r="BU8" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BV8" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="BV8" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AN9" s="1" t="s">
         <v>141</v>
@@ -3330,44 +3330,41 @@
         <v>142</v>
       </c>
       <c r="BW9" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="BX9" t="s">
         <v>197</v>
       </c>
-      <c r="BX9" t="s">
-        <v>198</v>
-      </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:77" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="AN10" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW10" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="BW10" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="AN10" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="AW10" s="7">
-        <v>10171</v>
-      </c>
-      <c r="BW10" s="8" t="s">
+      <c r="S11" t="s">
+        <v>192</v>
+      </c>
+      <c r="AN11" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>215</v>
+      </c>
+      <c r="BY11" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="S11" t="s">
-        <v>193</v>
-      </c>
-      <c r="T11" t="s">
-        <v>156</v>
-      </c>
-      <c r="AN11" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>142</v>
-      </c>
-      <c r="BY11" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3380,22 +3377,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3418,7 +3415,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3447,30 +3444,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3703,25 +3676,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3738,4 +3717,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commiting new scenarios for step definition.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3717103E-7736-4631-85BA-07C3D71A7892}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C00FFB-89DE-4D43-90E1-EF52B34F6FEA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="224">
   <si>
     <t>scenario</t>
   </si>
@@ -674,6 +674,27 @@
   </si>
   <si>
     <t>sangameshwar.balur</t>
+  </si>
+  <si>
+    <t>LINE_MANAGER_PERFORMS_CHANGE_MANAGER</t>
+  </si>
+  <si>
+    <t>rakesh.ghosal</t>
+  </si>
+  <si>
+    <t>personName</t>
+  </si>
+  <si>
+    <t>Sangameshwar Balur</t>
+  </si>
+  <si>
+    <t>changeManagerReason</t>
+  </si>
+  <si>
+    <t>Addition of Assignment for Manager</t>
+  </si>
+  <si>
+    <t>Aarnet Ebenezer</t>
   </si>
 </sst>
 </file>
@@ -1012,68 +1033,68 @@
       <selection activeCell="AX2" sqref="AX2:AX9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1252,7 +1273,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1408,7 +1429,7 @@
       <c r="BE2"/>
       <c r="BF2"/>
     </row>
-    <row r="3" spans="1:59" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1565,7 +1586,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1721,7 +1742,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1877,7 +1898,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -2033,7 +2054,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2189,7 +2210,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -2257,7 +2278,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>187</v>
       </c>
@@ -2427,22 +2448,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2477,7 +2498,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2512,7 +2533,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>104</v>
       </c>
@@ -2535,7 +2556,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2566,88 +2587,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AN8" sqref="AN8"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AD10" sqref="AD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5703125" customWidth="1"/>
-    <col min="62" max="62" width="26.85546875" customWidth="1"/>
-    <col min="63" max="63" width="18.5703125" customWidth="1"/>
-    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.578125" customWidth="1"/>
+    <col min="62" max="62" width="26.83984375" customWidth="1"/>
+    <col min="63" max="63" width="18.578125" customWidth="1"/>
+    <col min="64" max="64" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.578125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5703125" customWidth="1"/>
+    <col min="75" max="75" width="42.578125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2880,7 +2901,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -2908,7 +2929,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2936,7 +2957,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2985,7 +3006,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3034,7 +3055,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:77" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>125</v>
       </c>
@@ -3116,7 +3137,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>163</v>
       </c>
@@ -3208,7 +3229,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>167</v>
       </c>
@@ -3319,7 +3340,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
         <v>185</v>
       </c>
@@ -3336,7 +3357,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
         <v>190</v>
       </c>
@@ -3350,7 +3371,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>191</v>
       </c>
@@ -3375,24 +3396,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.20703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.3671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3414,8 +3438,17 @@
       <c r="G1" t="s">
         <v>43</v>
       </c>
+      <c r="H1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J1" t="s">
+        <v>212</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3436,6 +3469,38 @@
       </c>
       <c r="G2" s="4">
         <v>80572.460000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="4">
+        <v>80572.460000000006</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Termination and Retirement scenarios are scripted.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3717103E-7736-4631-85BA-07C3D71A7892}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349442A5-354F-4050-A38C-43BFDFDEFE93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="219">
   <si>
     <t>scenario</t>
   </si>
@@ -674,6 +674,12 @@
   </si>
   <si>
     <t>sangameshwar.balur</t>
+  </si>
+  <si>
+    <t>TERMINATION</t>
+  </si>
+  <si>
+    <t>RETIREMENT</t>
   </si>
 </sst>
 </file>
@@ -2566,8 +2572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AN8" sqref="AN8"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,7 +2616,7 @@
     <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3375,21 +3381,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3438,8 +3444,31 @@
         <v>80572.460000000006</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Handled multiple person number scenario for change manager
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B915B128-0208-4BE7-9D22-2B3DA626252D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3607AF6F-D2D7-4E5A-BB42-7A480DC94E4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="212">
   <si>
     <t>scenario</t>
   </si>
@@ -626,9 +626,6 @@
   </si>
   <si>
     <t>LINE_MANAGER_PERFORMS_CHANGE_MANAGER</t>
-  </si>
-  <si>
-    <t>rakesh.ghosal</t>
   </si>
   <si>
     <t>Sangameshwar Balur</t>
@@ -1003,73 +1000,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AX2" sqref="AX2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1248,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1413,7 +1410,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1575,7 +1572,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1737,9 +1734,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>142</v>
@@ -1899,7 +1896,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -2061,7 +2058,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>144</v>
       </c>
@@ -2125,7 +2122,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2301,22 +2298,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5234375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2351,7 +2348,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -2386,7 +2383,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2409,7 +2406,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2440,88 +2437,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
-      <selection activeCell="BX8" sqref="BX8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5546875" customWidth="1"/>
-    <col min="62" max="62" width="26.88671875" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" customWidth="1"/>
-    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5234375" customWidth="1"/>
+    <col min="62" max="62" width="26.89453125" customWidth="1"/>
+    <col min="63" max="63" width="18.5234375" customWidth="1"/>
+    <col min="64" max="64" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.1015625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5234375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.1015625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5234375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5546875" customWidth="1"/>
+    <col min="75" max="75" width="42.5234375" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2754,7 +2751,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -2782,7 +2779,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -2810,7 +2807,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -2859,7 +2856,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -2908,7 +2905,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>121</v>
       </c>
@@ -2990,9 +2987,9 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3064,7 +3061,7 @@
         <v>146</v>
       </c>
       <c r="BK7" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BL7" s="7" t="s">
         <v>59</v>
@@ -3082,9 +3079,9 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3156,7 +3153,7 @@
         <v>146</v>
       </c>
       <c r="BK8" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BL8" s="7" t="s">
         <v>59</v>
@@ -3193,9 +3190,9 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AN9" s="7" t="s">
         <v>176</v>
@@ -3210,9 +3207,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AN10" s="7" t="s">
         <v>176</v>
@@ -3224,7 +3221,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>168</v>
       </c>
@@ -3251,25 +3248,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.41796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1015625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7890625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3292,16 +3289,16 @@
         <v>43</v>
       </c>
       <c r="H1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" t="s">
         <v>205</v>
-      </c>
-      <c r="I1" t="s">
-        <v>206</v>
       </c>
       <c r="J1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3324,7 +3321,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -3335,7 +3332,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3346,12 +3343,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
         <v>176</v>
@@ -3369,13 +3366,13 @@
         <v>80572.460000000006</v>
       </c>
       <c r="H5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I5" t="s">
         <v>202</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>203</v>
-      </c>
-      <c r="J5" t="s">
-        <v>204</v>
       </c>
       <c r="L5" s="4"/>
     </row>

</xml_diff>

<commit_message>
Implemented writing new hire person no from HDL load to csv
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECF40C8-BF02-4F36-AA01-7EFCA5756557}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD785BBE-2C00-4D5A-992E-ABF1437E5F05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -466,9 +466,6 @@
     <t>Adamo Ave</t>
   </si>
   <si>
-    <t>Alternate work Location Address</t>
-  </si>
-  <si>
     <t>Thomas</t>
   </si>
   <si>
@@ -662,6 +659,9 @@
   </si>
   <si>
     <t>ADD_NEW_ADDRESS_TYPE_DETAILS</t>
+  </si>
+  <si>
+    <t>Mailing Address</t>
   </si>
 </sst>
 </file>
@@ -1007,69 +1007,69 @@
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AP1" t="s">
         <v>40</v>
@@ -1245,13 +1245,13 @@
         <v>139</v>
       </c>
       <c r="BG1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>56</v>
@@ -1286,22 +1286,22 @@
         <v>60</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>137</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>62</v>
@@ -1330,23 +1330,23 @@
         <v>143</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>69</v>
@@ -1362,13 +1362,13 @@
         <v>71</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO2" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>64</v>
@@ -1380,7 +1380,7 @@
         <v>73</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>74</v>
@@ -1392,7 +1392,7 @@
         <v>76</v>
       </c>
       <c r="AX2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AY2" s="1" t="s">
         <v>78</v>
@@ -1404,16 +1404,16 @@
         <v>80</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BG2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BH2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>56</v>
@@ -1448,22 +1448,22 @@
         <v>60</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>137</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>62</v>
@@ -1492,23 +1492,23 @@
         <v>143</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>69</v>
@@ -1524,13 +1524,13 @@
         <v>71</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>64</v>
@@ -1542,7 +1542,7 @@
         <v>73</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>74</v>
@@ -1554,7 +1554,7 @@
         <v>76</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AY3" s="1" t="s">
         <v>78</v>
@@ -1566,16 +1566,16 @@
         <v>80</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BG3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BH3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>55</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>56</v>
@@ -1610,22 +1610,22 @@
         <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>137</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>62</v>
@@ -1654,23 +1654,23 @@
         <v>143</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AI4" s="1" t="s">
         <v>69</v>
@@ -1686,13 +1686,13 @@
         <v>71</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO4" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AQ4" s="1" t="s">
         <v>64</v>
@@ -1704,7 +1704,7 @@
         <v>73</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AU4" s="1" t="s">
         <v>74</v>
@@ -1716,7 +1716,7 @@
         <v>76</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AY4" s="1" t="s">
         <v>78</v>
@@ -1728,18 +1728,18 @@
         <v>80</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BG4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BH4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>142</v>
@@ -1754,7 +1754,7 @@
         <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>56</v>
@@ -1772,22 +1772,22 @@
         <v>60</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>137</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>62</v>
@@ -1816,23 +1816,23 @@
         <v>143</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AI5" s="1" t="s">
         <v>69</v>
@@ -1848,13 +1848,13 @@
         <v>71</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO5" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AQ5" s="1" t="s">
         <v>64</v>
@@ -1866,7 +1866,7 @@
         <v>73</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AU5" s="1" t="s">
         <v>74</v>
@@ -1878,7 +1878,7 @@
         <v>76</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AY5" s="1" t="s">
         <v>78</v>
@@ -1890,16 +1890,16 @@
         <v>80</v>
       </c>
       <c r="BB5" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BG5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BH5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>56</v>
@@ -1934,22 +1934,22 @@
         <v>60</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>137</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>62</v>
@@ -1978,23 +1978,23 @@
         <v>143</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AI6" s="1" t="s">
         <v>69</v>
@@ -2010,13 +2010,13 @@
         <v>71</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO6" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AQ6" s="1" t="s">
         <v>64</v>
@@ -2028,7 +2028,7 @@
         <v>73</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AU6" s="1" t="s">
         <v>74</v>
@@ -2040,7 +2040,7 @@
         <v>76</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AY6" s="1" t="s">
         <v>78</v>
@@ -2052,16 +2052,16 @@
         <v>80</v>
       </c>
       <c r="BB6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BG6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BH6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>144</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="AL7" s="1"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
@@ -2115,7 +2115,7 @@
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
       <c r="AX7" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
@@ -2125,9 +2125,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>142</v>
@@ -2142,7 +2142,7 @@
         <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>56</v>
@@ -2160,22 +2160,22 @@
         <v>60</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>137</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>62</v>
@@ -2204,23 +2204,23 @@
         <v>143</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AI8" s="1" t="s">
         <v>69</v>
@@ -2236,13 +2236,13 @@
         <v>71</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO8" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AQ8" s="1" t="s">
         <v>64</v>
@@ -2254,7 +2254,7 @@
         <v>73</v>
       </c>
       <c r="AT8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AU8" s="1" t="s">
         <v>74</v>
@@ -2266,7 +2266,7 @@
         <v>76</v>
       </c>
       <c r="AX8" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AY8" s="1" t="s">
         <v>78</v>
@@ -2278,13 +2278,13 @@
         <v>80</v>
       </c>
       <c r="BB8" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BG8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BH8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2301,22 +2301,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2440,88 +2440,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AP8" sqref="AP8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5546875" customWidth="1"/>
-    <col min="62" max="62" width="26.88671875" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" customWidth="1"/>
-    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5546875" customWidth="1"/>
+    <col min="75" max="75" width="42.5703125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:77" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2703,58 +2703,58 @@
         <v>113</v>
       </c>
       <c r="BI1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BK1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BL1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BM1" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="BN1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="BO1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BP1" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="BQ1" s="7" t="s">
         <v>23</v>
       </c>
       <c r="BR1" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BS1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="BT1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="BU1" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="BU1" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="BV1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="BW1" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="BX1" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BY1" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -2766,7 +2766,7 @@
       <c r="AB2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AN2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AP2" s="5"/>
       <c r="AQ2">
@@ -2776,13 +2776,13 @@
         <v>80000</v>
       </c>
       <c r="AS2" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW2" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AW2" s="1" t="s">
-        <v>192</v>
-      </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -2794,7 +2794,7 @@
       <c r="AB3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AN3" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AP3" s="5"/>
       <c r="AQ3">
@@ -2804,13 +2804,13 @@
         <v>80000</v>
       </c>
       <c r="AS3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AW3" s="1" t="s">
-        <v>192</v>
-      </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="AB4" s="5"/>
       <c r="AL4" s="5"/>
       <c r="AN4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AP4" s="5"/>
       <c r="AQ4">
@@ -2832,10 +2832,10 @@
         <v>15</v>
       </c>
       <c r="AS4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW4" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="AW4" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="BB4" t="s">
         <v>114</v>
@@ -2859,7 +2859,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -2871,7 +2871,7 @@
       <c r="AB5" s="5"/>
       <c r="AL5" s="5"/>
       <c r="AN5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AP5" s="5"/>
       <c r="AQ5">
@@ -2881,10 +2881,10 @@
         <v>15</v>
       </c>
       <c r="AS5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AW5" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="AW5" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="BB5" t="s">
         <v>114</v>
@@ -2908,7 +2908,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>121</v>
       </c>
@@ -2951,7 +2951,7 @@
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
@@ -2962,7 +2962,7 @@
       <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
       <c r="AW6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
@@ -2990,9 +2990,9 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:77" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3033,7 +3033,7 @@
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
@@ -3044,7 +3044,7 @@
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
       <c r="AW7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
@@ -3064,13 +3064,13 @@
         <v>146</v>
       </c>
       <c r="BK7" s="7" t="s">
-        <v>147</v>
+        <v>212</v>
       </c>
       <c r="BL7" s="7" t="s">
         <v>59</v>
       </c>
       <c r="BM7" s="7">
-        <v>48382</v>
+        <v>48634</v>
       </c>
       <c r="BN7" s="7"/>
       <c r="BO7" s="7"/>
@@ -3082,9 +3082,9 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:77" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3125,7 +3125,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -3136,7 +3136,7 @@
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
       <c r="AW8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
@@ -3156,28 +3156,28 @@
         <v>146</v>
       </c>
       <c r="BK8" s="7" t="s">
-        <v>147</v>
+        <v>212</v>
       </c>
       <c r="BL8" s="7" t="s">
         <v>59</v>
       </c>
       <c r="BM8" s="7">
-        <v>48382</v>
+        <v>48634</v>
       </c>
       <c r="BN8" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="BO8" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="BO8" s="7" t="s">
+      <c r="BP8" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="BP8" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="BQ8" s="7" t="s">
         <v>66</v>
       </c>
       <c r="BR8" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BS8" s="7" t="s">
         <v>60</v>
@@ -3186,59 +3186,59 @@
         <v>6323145</v>
       </c>
       <c r="BU8" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="BV8" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="BV8" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:77" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AN9" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW9" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="BW9" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="BX9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:77" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN10" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="BW9" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>175</v>
+      <c r="AW10" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="BW10" s="8" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="AN10" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="AW10" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="BW10" s="8" t="s">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="S11" t="s">
+        <v>169</v>
+      </c>
+      <c r="AN11" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>191</v>
+      </c>
+      <c r="BY11" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="S11" t="s">
-        <v>170</v>
-      </c>
-      <c r="AN11" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>192</v>
-      </c>
-      <c r="BY11" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3255,21 +3255,21 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3292,16 +3292,16 @@
         <v>43</v>
       </c>
       <c r="H1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" t="s">
         <v>206</v>
       </c>
-      <c r="I1" t="s">
-        <v>207</v>
-      </c>
       <c r="J1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3324,37 +3324,37 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" t="s">
-        <v>177</v>
+      <c r="B4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" t="s">
+        <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" t="s">
         <v>201</v>
       </c>
-      <c r="B5" t="s">
-        <v>202</v>
-      </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>128</v>
@@ -3369,13 +3369,13 @@
         <v>80572.460000000006</v>
       </c>
       <c r="H5" t="s">
+        <v>202</v>
+      </c>
+      <c r="I5" t="s">
         <v>203</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>204</v>
-      </c>
-      <c r="J5" t="s">
-        <v>205</v>
       </c>
       <c r="L5" s="4"/>
     </row>
@@ -3386,6 +3386,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3618,31 +3642,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3659,22 +3677,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed DemoSet2 and updated code
Signed-off-by: Raghavendran Ramasubramanian <Raghavendran.R1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3607AF6F-D2D7-4E5A-BB42-7A480DC94E4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1D7FC6-6E05-4740-833A-392DA0A6204F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="216">
   <si>
     <t>scenario</t>
   </si>
@@ -628,6 +628,9 @@
     <t>LINE_MANAGER_PERFORMS_CHANGE_MANAGER</t>
   </si>
   <si>
+    <t>rakesh.ghosal</t>
+  </si>
+  <si>
     <t>Sangameshwar Balur</t>
   </si>
   <si>
@@ -659,6 +662,15 @@
   </si>
   <si>
     <t>Mailing Address</t>
+  </si>
+  <si>
+    <t>Raghavendran.Ramasubramanian</t>
+  </si>
+  <si>
+    <t>3/12/19</t>
+  </si>
+  <si>
+    <t>3/21/19</t>
   </si>
 </sst>
 </file>
@@ -1000,73 +1012,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1260,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1310,7 +1322,7 @@
         <v>141</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>65</v>
@@ -1410,7 +1422,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>141</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>65</v>
@@ -1572,7 +1584,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1634,7 +1646,7 @@
         <v>141</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="V4" s="2" t="s">
         <v>65</v>
@@ -1734,9 +1746,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>142</v>
@@ -1796,7 +1808,7 @@
         <v>141</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>64</v>
+        <v>215</v>
       </c>
       <c r="V5" s="2" t="s">
         <v>65</v>
@@ -1896,7 +1908,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -1958,7 +1970,7 @@
         <v>141</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>65</v>
@@ -2058,7 +2070,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>144</v>
       </c>
@@ -2122,7 +2134,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2184,7 +2196,7 @@
         <v>141</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>65</v>
@@ -2298,22 +2310,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5234375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2348,7 +2360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -2383,7 +2395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2438,87 +2450,87 @@
   <dimension ref="A1:BY11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5234375" customWidth="1"/>
-    <col min="62" max="62" width="26.89453125" customWidth="1"/>
-    <col min="63" max="63" width="18.5234375" customWidth="1"/>
-    <col min="64" max="64" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5546875" customWidth="1"/>
+    <col min="62" max="62" width="26.88671875" customWidth="1"/>
+    <col min="63" max="63" width="18.5546875" customWidth="1"/>
+    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5234375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5234375" customWidth="1"/>
+    <col min="75" max="75" width="42.5546875" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2751,7 +2763,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -2779,7 +2791,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -2807,7 +2819,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -2856,7 +2868,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -2905,7 +2917,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>121</v>
       </c>
@@ -2987,9 +2999,9 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3041,7 +3053,7 @@
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
       <c r="AW7" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
@@ -3061,7 +3073,7 @@
         <v>146</v>
       </c>
       <c r="BK7" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="BL7" s="7" t="s">
         <v>59</v>
@@ -3079,9 +3091,9 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3133,7 +3145,7 @@
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
       <c r="AW8" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
@@ -3153,7 +3165,7 @@
         <v>146</v>
       </c>
       <c r="BK8" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="BL8" s="7" t="s">
         <v>59</v>
@@ -3190,9 +3202,9 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AN9" s="7" t="s">
         <v>176</v>
@@ -3207,9 +3219,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AN10" s="7" t="s">
         <v>176</v>
@@ -3221,7 +3233,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>168</v>
       </c>
@@ -3248,25 +3260,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1015625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7890625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3289,16 +3301,16 @@
         <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3321,7 +3333,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -3332,7 +3344,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3343,12 +3355,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
         <v>176</v>
@@ -3366,13 +3378,13 @@
         <v>80572.460000000006</v>
       </c>
       <c r="H5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L5" s="4"/>
     </row>
@@ -3383,6 +3395,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3615,31 +3651,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3656,22 +3686,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Code for Skills and qualification
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3607AF6F-D2D7-4E5A-BB42-7A480DC94E4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39763E07-A034-4BA4-895A-2097556AE8DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="223">
   <si>
     <t>scenario</t>
   </si>
@@ -334,15 +334,6 @@
     <t>WORK_SCHEDULE_INACTIVE</t>
   </si>
   <si>
-    <t>UPDATE_SALARY_FOR_EXISTING_EMP</t>
-  </si>
-  <si>
-    <t>CHANGE_SALARY_BASIS_FOR_EXISTING_EMP</t>
-  </si>
-  <si>
-    <t>EDIT_SALARY_PROPOSAL_REASON</t>
-  </si>
-  <si>
     <t>UPDATE_PERSONAL_PAYMENT_METHODS_EXPENSES_ONLY</t>
   </si>
   <si>
@@ -457,9 +448,6 @@
     <t>Hire</t>
   </si>
   <si>
-    <t>UPDATE_I9_STATUS</t>
-  </si>
-  <si>
     <t>Crescent Loop Dr</t>
   </si>
   <si>
@@ -547,12 +535,6 @@
     <t>C:\\testdata\\Salary.zip</t>
   </si>
   <si>
-    <t>Matt HDLNEWHIRE</t>
-  </si>
-  <si>
-    <t>koushik.kadimcherla</t>
-  </si>
-  <si>
     <t>Cloud123</t>
   </si>
   <si>
@@ -607,9 +589,6 @@
     <t>TERMINATION</t>
   </si>
   <si>
-    <t>RETIREMENT</t>
-  </si>
-  <si>
     <t>managerType</t>
   </si>
   <si>
@@ -625,9 +604,6 @@
     <t>Acme Industries, US Ltd.</t>
   </si>
   <si>
-    <t>LINE_MANAGER_PERFORMS_CHANGE_MANAGER</t>
-  </si>
-  <si>
     <t>Sangameshwar Balur</t>
   </si>
   <si>
@@ -643,9 +619,6 @@
     <t>changeManagerReason</t>
   </si>
   <si>
-    <t>NEW_HIRE_USING_HDL</t>
-  </si>
-  <si>
     <t>LEGAL_ENTITY_TRANSFER</t>
   </si>
   <si>
@@ -659,6 +632,66 @@
   </si>
   <si>
     <t>Mailing Address</t>
+  </si>
+  <si>
+    <t>NEW_HIRE_USING_HDL1</t>
+  </si>
+  <si>
+    <t>UPDATE_I9_STATUS1</t>
+  </si>
+  <si>
+    <t>EDIT_SALARY_PROPOSAL_REASON1</t>
+  </si>
+  <si>
+    <t>UPDATE_SALARY_FOR_EXISTING_EMP1</t>
+  </si>
+  <si>
+    <t>CHANGE_SALARY_BASIS_FOR_EXISTING_EMP1</t>
+  </si>
+  <si>
+    <t>LINE_MANAGER_PERFORMS_CHANGE_MANAGER1</t>
+  </si>
+  <si>
+    <t>RETIREMENT1</t>
+  </si>
+  <si>
+    <t>Cook AUTOMATIONHDL</t>
+  </si>
+  <si>
+    <t>ADD_SKILLS_AND_QUALIFICATION_DETAILS</t>
+  </si>
+  <si>
+    <t>degreeName</t>
+  </si>
+  <si>
+    <t>Master's Degree</t>
+  </si>
+  <si>
+    <t>degreeMajor</t>
+  </si>
+  <si>
+    <t>MS IT</t>
+  </si>
+  <si>
+    <t>degreeSchool</t>
+  </si>
+  <si>
+    <t>University of Florida</t>
+  </si>
+  <si>
+    <t>degreeYear</t>
+  </si>
+  <si>
+    <t>licenseName</t>
+  </si>
+  <si>
+    <t>Federal licenses</t>
+  </si>
+  <si>
+    <t>licenseNumber</t>
+  </si>
+  <si>
+    <t>PKT13</t>
   </si>
 </sst>
 </file>
@@ -1000,73 +1033,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1188,7 +1221,7 @@
         <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AP1" t="s">
         <v>40</v>
@@ -1230,30 +1263,30 @@
         <v>52</v>
       </c>
       <c r="BC1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="BD1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="BE1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="BF1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="BG1" t="s">
+        <v>182</v>
+      </c>
+      <c r="BH1" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="BH1" s="10" t="s">
-        <v>195</v>
-      </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>53</v>
@@ -1265,7 +1298,7 @@
         <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>56</v>
@@ -1283,22 +1316,22 @@
         <v>60</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>62</v>
@@ -1307,7 +1340,7 @@
         <v>63</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>64</v>
@@ -1324,26 +1357,26 @@
         <v>67</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>69</v>
@@ -1353,31 +1386,31 @@
         <v>70</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>74</v>
@@ -1389,7 +1422,7 @@
         <v>76</v>
       </c>
       <c r="AX2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="AY2" s="1" t="s">
         <v>78</v>
@@ -1401,21 +1434,21 @@
         <v>80</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BG2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="BH2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>53</v>
@@ -1427,7 +1460,7 @@
         <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>56</v>
@@ -1445,22 +1478,22 @@
         <v>60</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>62</v>
@@ -1469,7 +1502,7 @@
         <v>63</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>64</v>
@@ -1486,26 +1519,26 @@
         <v>67</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>69</v>
@@ -1515,31 +1548,31 @@
         <v>70</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>74</v>
@@ -1551,7 +1584,7 @@
         <v>76</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AY3" s="1" t="s">
         <v>78</v>
@@ -1563,21 +1596,21 @@
         <v>80</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BG3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="BH3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>53</v>
@@ -1589,7 +1622,7 @@
         <v>55</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>56</v>
@@ -1607,22 +1640,22 @@
         <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>62</v>
@@ -1631,7 +1664,7 @@
         <v>63</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>64</v>
@@ -1648,26 +1681,26 @@
         <v>67</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AI4" s="1" t="s">
         <v>69</v>
@@ -1677,31 +1710,31 @@
         <v>70</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="AQ4" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AU4" s="1" t="s">
         <v>74</v>
@@ -1713,7 +1746,7 @@
         <v>76</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AY4" s="1" t="s">
         <v>78</v>
@@ -1725,21 +1758,21 @@
         <v>80</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BG4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="BH4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>207</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>53</v>
@@ -1751,7 +1784,7 @@
         <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>56</v>
@@ -1769,22 +1802,22 @@
         <v>60</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>62</v>
@@ -1793,7 +1826,7 @@
         <v>63</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>64</v>
@@ -1810,26 +1843,26 @@
         <v>67</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="9" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AI5" s="1" t="s">
         <v>69</v>
@@ -1839,31 +1872,31 @@
         <v>70</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM5" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="AQ5" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AS5" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AU5" s="1" t="s">
         <v>74</v>
@@ -1875,7 +1908,7 @@
         <v>76</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AY5" s="1" t="s">
         <v>78</v>
@@ -1887,21 +1920,21 @@
         <v>80</v>
       </c>
       <c r="BB5" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BG5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="BH5" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>53</v>
@@ -1913,7 +1946,7 @@
         <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>56</v>
@@ -1931,22 +1964,22 @@
         <v>60</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>62</v>
@@ -1955,7 +1988,7 @@
         <v>63</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>64</v>
@@ -1972,26 +2005,26 @@
         <v>67</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AI6" s="1" t="s">
         <v>69</v>
@@ -2001,31 +2034,31 @@
         <v>70</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM6" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="AQ6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AU6" s="1" t="s">
         <v>74</v>
@@ -2037,7 +2070,7 @@
         <v>76</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AY6" s="1" t="s">
         <v>78</v>
@@ -2049,18 +2082,18 @@
         <v>80</v>
       </c>
       <c r="BB6" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BG6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="BH6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>144</v>
+        <v>204</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2101,7 +2134,7 @@
       <c r="AL7" s="1"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
@@ -2112,22 +2145,22 @@
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
       <c r="AX7" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
       <c r="BF7" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>53</v>
@@ -2139,7 +2172,7 @@
         <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>56</v>
@@ -2157,22 +2190,22 @@
         <v>60</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>62</v>
@@ -2181,7 +2214,7 @@
         <v>63</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>64</v>
@@ -2198,26 +2231,26 @@
         <v>67</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AI8" s="1" t="s">
         <v>69</v>
@@ -2227,31 +2260,31 @@
         <v>70</v>
       </c>
       <c r="AL8" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AM8" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO8" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="AQ8" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AS8" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT8" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AU8" s="1" t="s">
         <v>74</v>
@@ -2263,7 +2296,7 @@
         <v>76</v>
       </c>
       <c r="AX8" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AY8" s="1" t="s">
         <v>78</v>
@@ -2275,13 +2308,13 @@
         <v>80</v>
       </c>
       <c r="BB8" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BG8" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="BH8" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2298,22 +2331,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5234375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2348,7 +2381,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -2383,7 +2416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2406,7 +2439,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2435,90 +2468,90 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BY11"/>
+  <dimension ref="A1:CE12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5234375" customWidth="1"/>
-    <col min="62" max="62" width="26.89453125" customWidth="1"/>
-    <col min="63" max="63" width="18.5234375" customWidth="1"/>
-    <col min="64" max="64" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5234375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5234375" customWidth="1"/>
+    <col min="75" max="75" width="42.5703125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:83" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2679,81 +2712,99 @@
         <v>52</v>
       </c>
       <c r="BB1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BE1" t="s">
         <v>107</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>108</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>109</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
         <v>110</v>
       </c>
-      <c r="BF1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>113</v>
-      </c>
       <c r="BI1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BM1" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="BJ1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="BK1" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="BL1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>157</v>
       </c>
       <c r="BN1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="BO1" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="BP1" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="BQ1" s="7" t="s">
         <v>23</v>
       </c>
       <c r="BR1" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="BS1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="BT1" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="BU1" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="BV1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="BW1" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="BX1" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="BY1" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
+      </c>
+      <c r="BZ1" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="CA1" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="CB1" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="CC1" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="CD1" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="CE1" s="7" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
@@ -2763,7 +2814,7 @@
       <c r="AB2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AN2" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AP2" s="5"/>
       <c r="AQ2">
@@ -2773,15 +2824,15 @@
         <v>80000</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>207</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
@@ -2791,7 +2842,7 @@
       <c r="AB3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AN3" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AP3" s="5"/>
       <c r="AQ3">
@@ -2801,15 +2852,15 @@
         <v>80000</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>205</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
@@ -2819,7 +2870,7 @@
       <c r="AB4" s="5"/>
       <c r="AL4" s="5"/>
       <c r="AN4" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AP4" s="5"/>
       <c r="AQ4">
@@ -2829,36 +2880,36 @@
         <v>15</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="AW4" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="BB4" t="s">
+        <v>111</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="BE4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BF4" t="s">
         <v>115</v>
       </c>
-      <c r="BD4" s="6" t="s">
+      <c r="BG4" t="s">
         <v>116</v>
       </c>
-      <c r="BE4" s="2" t="s">
+      <c r="BH4" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="BF4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>119</v>
-      </c>
-      <c r="BH4" s="6" t="s">
-        <v>120</v>
-      </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
@@ -2868,7 +2919,7 @@
       <c r="AB5" s="5"/>
       <c r="AL5" s="5"/>
       <c r="AN5" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AP5" s="5"/>
       <c r="AQ5">
@@ -2878,36 +2929,36 @@
         <v>15</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="AW5" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="BB5" t="s">
+        <v>111</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD5" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="BE5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BF5" t="s">
         <v>115</v>
       </c>
-      <c r="BD5" s="6" t="s">
+      <c r="BG5" t="s">
         <v>116</v>
       </c>
-      <c r="BE5" s="2" t="s">
+      <c r="BH5" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="BF5" t="s">
+    </row>
+    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>119</v>
-      </c>
-      <c r="BH5" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2948,7 +2999,7 @@
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
@@ -2959,7 +3010,7 @@
       <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
       <c r="AW6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
@@ -2987,9 +3038,9 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:83" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3030,7 +3081,7 @@
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
@@ -3041,7 +3092,7 @@
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
       <c r="AW7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
@@ -3055,13 +3106,13 @@
       <c r="BG7" s="7"/>
       <c r="BH7" s="7"/>
       <c r="BI7" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="BJ7" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="BK7" s="7" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="BL7" s="7" t="s">
         <v>59</v>
@@ -3079,9 +3130,9 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:83" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3122,7 +3173,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -3133,7 +3184,7 @@
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
       <c r="AW8" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
@@ -3147,13 +3198,13 @@
       <c r="BG8" s="7"/>
       <c r="BH8" s="7"/>
       <c r="BI8" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="BJ8" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="BK8" s="7" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="BL8" s="7" t="s">
         <v>59</v>
@@ -3162,19 +3213,19 @@
         <v>48634</v>
       </c>
       <c r="BN8" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="BO8" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="BP8" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="BQ8" s="7" t="s">
         <v>66</v>
       </c>
       <c r="BR8" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="BS8" s="7" t="s">
         <v>60</v>
@@ -3183,59 +3234,88 @@
         <v>6323145</v>
       </c>
       <c r="BU8" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="BV8" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AN9" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AW9" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>185</v>
       </c>
       <c r="BW9" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="BX9" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:83" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="AN10" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AW10" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="BW10" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="S11" t="s">
+        <v>165</v>
+      </c>
+      <c r="AN11" s="7" t="s">
         <v>170</v>
       </c>
+      <c r="AW11" t="s">
+        <v>185</v>
+      </c>
+      <c r="BY11" t="s">
+        <v>167</v>
+      </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="S11" t="s">
-        <v>169</v>
-      </c>
-      <c r="AN11" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>191</v>
-      </c>
-      <c r="BY11" t="s">
-        <v>171</v>
+    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="AN12" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>185</v>
+      </c>
+      <c r="BZ12" t="s">
+        <v>213</v>
+      </c>
+      <c r="CA12" t="s">
+        <v>215</v>
+      </c>
+      <c r="CB12" t="s">
+        <v>217</v>
+      </c>
+      <c r="CC12">
+        <v>2015</v>
+      </c>
+      <c r="CD12" t="s">
+        <v>220</v>
+      </c>
+      <c r="CE12" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3248,25 +3328,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1015625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7890625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3277,102 +3357,102 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G1" t="s">
         <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="I1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="J1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" t="s">
         <v>127</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" t="s">
-        <v>130</v>
       </c>
       <c r="G2" s="4">
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G5" s="4">
         <v>80572.460000000006</v>
       </c>
       <c r="H5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I5" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="J5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="L5" s="4"/>
     </row>

</xml_diff>

<commit_message>
latest code from Demo
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1D7FC6-6E05-4740-833A-392DA0A6204F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BCBF8F-AB16-4C43-9F73-CEB345E2144C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="228">
   <si>
     <t>scenario</t>
   </si>
@@ -671,6 +671,42 @@
   </si>
   <si>
     <t>3/21/19</t>
+  </si>
+  <si>
+    <t>ADD_SKILLS_AND_QUALIFICATION_DETAILS</t>
+  </si>
+  <si>
+    <t>Master's Degree</t>
+  </si>
+  <si>
+    <t>MS IT</t>
+  </si>
+  <si>
+    <t>University of Florida</t>
+  </si>
+  <si>
+    <t>Federal licenses</t>
+  </si>
+  <si>
+    <t>PKT13</t>
+  </si>
+  <si>
+    <t>degreeName</t>
+  </si>
+  <si>
+    <t>degreeMajor</t>
+  </si>
+  <si>
+    <t>degreeSchool</t>
+  </si>
+  <si>
+    <t>degreeYear</t>
+  </si>
+  <si>
+    <t>licenseName</t>
+  </si>
+  <si>
+    <t>licenseNumber</t>
   </si>
 </sst>
 </file>
@@ -1012,73 +1048,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView topLeftCell="M4" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +1296,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1422,7 +1458,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1584,7 +1620,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1746,7 +1782,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>208</v>
       </c>
@@ -1908,7 +1944,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -2070,7 +2106,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>144</v>
       </c>
@@ -2134,7 +2170,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2310,22 +2346,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2360,7 +2396,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -2395,7 +2431,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2418,7 +2454,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2447,90 +2483,90 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BY11"/>
+  <dimension ref="A1:CE12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="BQ4" workbookViewId="0">
+      <selection activeCell="CE12" sqref="CE12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5546875" customWidth="1"/>
-    <col min="62" max="62" width="26.88671875" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" customWidth="1"/>
-    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5546875" customWidth="1"/>
+    <col min="75" max="75" width="42.5703125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:83" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2762,8 +2798,26 @@
       <c r="BY1" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="BZ1" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="CA1" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="CB1" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="CC1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="CD1" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="CE1" s="7" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -2791,7 +2845,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -2819,7 +2873,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -2868,7 +2922,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -2917,7 +2971,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>121</v>
       </c>
@@ -2999,7 +3053,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:83" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>211</v>
       </c>
@@ -3091,7 +3145,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:83" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>210</v>
       </c>
@@ -3202,7 +3256,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:83" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>207</v>
       </c>
@@ -3219,7 +3273,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:83" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>209</v>
       </c>
@@ -3233,7 +3287,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>168</v>
       </c>
@@ -3248,6 +3302,35 @@
       </c>
       <c r="BY11" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="AN12" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>191</v>
+      </c>
+      <c r="BZ12" t="s">
+        <v>217</v>
+      </c>
+      <c r="CA12" t="s">
+        <v>218</v>
+      </c>
+      <c r="CB12" t="s">
+        <v>219</v>
+      </c>
+      <c r="CC12">
+        <v>2015</v>
+      </c>
+      <c r="CD12" t="s">
+        <v>220</v>
+      </c>
+      <c r="CE12" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3264,21 +3347,21 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3310,7 +3393,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3333,7 +3416,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -3344,7 +3427,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3355,7 +3438,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>200</v>
       </c>
@@ -3395,30 +3478,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3651,25 +3710,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3686,4 +3751,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed contingent, pending and non worker
Signed-off-by: Raghavendran Ramasubramanian <Raghavendran.R1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBFCCA3-9D3D-41DC-BA41-3C6594F5B7CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F961C43-5BA7-426D-9232-98ED0BDFE5B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -18,18 +18,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="240">
   <si>
     <t>scenario</t>
   </si>
@@ -737,6 +731,18 @@
   </si>
   <si>
     <t>NEW_HIRE_CONTINGENT_WORKER</t>
+  </si>
+  <si>
+    <t>Add Pending Worker</t>
+  </si>
+  <si>
+    <t>Add Contingent Worker</t>
+  </si>
+  <si>
+    <t>Placement to fill vacant position</t>
+  </si>
+  <si>
+    <t>Future hire to fill vacant position</t>
   </si>
 </sst>
 </file>
@@ -1078,73 +1084,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="R4" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +1332,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1488,7 +1494,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1650,7 +1656,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1812,7 +1818,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>208</v>
       </c>
@@ -1974,7 +1980,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>144</v>
       </c>
@@ -2200,7 +2206,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2362,7 +2368,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>228</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>233</v>
       </c>
@@ -2600,13 +2606,13 @@
         <v>231</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="AB10" s="2" t="s">
         <v>166</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="AD10" s="1" t="s">
         <v>68</v>
@@ -2686,7 +2692,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>235</v>
       </c>
@@ -2762,13 +2768,13 @@
         <v>231</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="AB11" s="2" t="s">
         <v>166</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="AD11" s="1" t="s">
         <v>68</v>
@@ -2862,22 +2868,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2912,7 +2918,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2970,7 +2976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -3005,84 +3011,84 @@
       <selection activeCell="CE12" sqref="CE12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5703125" customWidth="1"/>
-    <col min="62" max="62" width="26.85546875" customWidth="1"/>
-    <col min="63" max="63" width="18.5703125" customWidth="1"/>
-    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5546875" customWidth="1"/>
+    <col min="62" max="62" width="26.88671875" customWidth="1"/>
+    <col min="63" max="63" width="18.5546875" customWidth="1"/>
+    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5703125" customWidth="1"/>
+    <col min="75" max="75" width="42.5546875" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -3361,7 +3367,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -3389,7 +3395,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -3438,7 +3444,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -3487,7 +3493,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>121</v>
       </c>
@@ -3569,7 +3575,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:83" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>211</v>
       </c>
@@ -3661,7 +3667,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:83" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:83" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>210</v>
       </c>
@@ -3772,7 +3778,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:83" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>207</v>
       </c>
@@ -3789,7 +3795,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:83" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>209</v>
       </c>
@@ -3803,7 +3809,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>168</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>216</v>
       </c>
@@ -3863,21 +3869,21 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3909,7 +3915,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3932,7 +3938,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -3943,7 +3949,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>200</v>
       </c>
@@ -3994,30 +4000,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4250,25 +4232,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4285,4 +4273,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed save to csv (trim) and create_element_Enteries
Signed-off-by: Raghavendran Ramasubramanian <Raghavendran.R1@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F961C43-5BA7-426D-9232-98ED0BDFE5B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E44798-89CA-41E0-99DE-6630B1222FA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="241">
   <si>
     <t>scenario</t>
   </si>
@@ -274,9 +274,6 @@
     <t>BILINGUAL_INDICATOR</t>
   </si>
   <si>
-    <t>UPDATE_ELEMENT_ENTRIES</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -743,6 +740,12 @@
   </si>
   <si>
     <t>Future hire to fill vacant position</t>
+  </si>
+  <si>
+    <t>ENTER_JOB_CHANGE</t>
+  </si>
+  <si>
+    <t>CREATE_ELEMENT_ENTRIES</t>
   </si>
 </sst>
 </file>
@@ -1084,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R4" workbookViewId="0">
-      <selection activeCell="AC10" sqref="AC10"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="BJ4" sqref="BJ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1272,7 +1275,7 @@
         <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AP1" t="s">
         <v>40</v>
@@ -1314,22 +1317,22 @@
         <v>52</v>
       </c>
       <c r="BC1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BD1" t="s">
         <v>132</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>133</v>
       </c>
-      <c r="BE1" t="s">
-        <v>134</v>
-      </c>
       <c r="BF1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BG1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.3">
@@ -1337,7 +1340,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>53</v>
@@ -1349,7 +1352,7 @@
         <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>56</v>
@@ -1367,22 +1370,22 @@
         <v>60</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>62</v>
@@ -1391,10 +1394,10 @@
         <v>63</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>65</v>
@@ -1408,26 +1411,26 @@
         <v>67</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>69</v>
@@ -1437,31 +1440,31 @@
         <v>70</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>74</v>
@@ -1473,7 +1476,7 @@
         <v>76</v>
       </c>
       <c r="AX2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AY2" s="1" t="s">
         <v>78</v>
@@ -1485,13 +1488,13 @@
         <v>80</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.3">
@@ -1499,7 +1502,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>53</v>
@@ -1511,7 +1514,7 @@
         <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>56</v>
@@ -1529,22 +1532,22 @@
         <v>60</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>62</v>
@@ -1553,10 +1556,10 @@
         <v>63</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>65</v>
@@ -1570,26 +1573,26 @@
         <v>67</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>69</v>
@@ -1599,31 +1602,31 @@
         <v>70</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>74</v>
@@ -1635,7 +1638,7 @@
         <v>76</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY3" s="1" t="s">
         <v>78</v>
@@ -1647,21 +1650,21 @@
         <v>80</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>240</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>53</v>
@@ -1673,7 +1676,7 @@
         <v>55</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>56</v>
@@ -1691,22 +1694,22 @@
         <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>62</v>
@@ -1715,10 +1718,10 @@
         <v>63</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V4" s="2" t="s">
         <v>65</v>
@@ -1732,26 +1735,26 @@
         <v>67</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI4" s="1" t="s">
         <v>69</v>
@@ -1761,31 +1764,31 @@
         <v>70</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ4" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU4" s="1" t="s">
         <v>74</v>
@@ -1797,7 +1800,7 @@
         <v>76</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY4" s="1" t="s">
         <v>78</v>
@@ -1809,21 +1812,21 @@
         <v>80</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>53</v>
@@ -1835,7 +1838,7 @@
         <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>56</v>
@@ -1853,22 +1856,22 @@
         <v>60</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>62</v>
@@ -1877,10 +1880,10 @@
         <v>63</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V5" s="2" t="s">
         <v>65</v>
@@ -1894,26 +1897,26 @@
         <v>67</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI5" s="1" t="s">
         <v>69</v>
@@ -1923,31 +1926,31 @@
         <v>70</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM5" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ5" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS5" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU5" s="1" t="s">
         <v>74</v>
@@ -1959,7 +1962,7 @@
         <v>76</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY5" s="1" t="s">
         <v>78</v>
@@ -1971,21 +1974,21 @@
         <v>80</v>
       </c>
       <c r="BB5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>53</v>
@@ -1997,7 +2000,7 @@
         <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>56</v>
@@ -2015,22 +2018,22 @@
         <v>60</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>62</v>
@@ -2039,10 +2042,10 @@
         <v>63</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>65</v>
@@ -2056,26 +2059,26 @@
         <v>67</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI6" s="1" t="s">
         <v>69</v>
@@ -2085,31 +2088,31 @@
         <v>70</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM6" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU6" s="1" t="s">
         <v>74</v>
@@ -2121,7 +2124,7 @@
         <v>76</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY6" s="1" t="s">
         <v>78</v>
@@ -2133,18 +2136,18 @@
         <v>80</v>
       </c>
       <c r="BB6" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2185,7 +2188,7 @@
       <c r="AL7" s="1"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
@@ -2196,22 +2199,22 @@
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
       <c r="AX7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
       <c r="BF7" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>53</v>
@@ -2223,7 +2226,7 @@
         <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>56</v>
@@ -2241,22 +2244,22 @@
         <v>60</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>62</v>
@@ -2265,10 +2268,10 @@
         <v>63</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>65</v>
@@ -2282,26 +2285,26 @@
         <v>67</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI8" s="1" t="s">
         <v>69</v>
@@ -2311,31 +2314,31 @@
         <v>70</v>
       </c>
       <c r="AL8" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM8" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO8" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ8" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS8" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU8" s="1" t="s">
         <v>74</v>
@@ -2347,7 +2350,7 @@
         <v>76</v>
       </c>
       <c r="AX8" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY8" s="1" t="s">
         <v>78</v>
@@ -2359,21 +2362,21 @@
         <v>80</v>
       </c>
       <c r="BB8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>53</v>
@@ -2385,7 +2388,7 @@
         <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>56</v>
@@ -2403,22 +2406,22 @@
         <v>60</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>62</v>
@@ -2427,10 +2430,10 @@
         <v>63</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V9" s="2" t="s">
         <v>65</v>
@@ -2441,29 +2444,29 @@
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AA9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="AD9" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI9" s="1" t="s">
         <v>69</v>
@@ -2473,31 +2476,31 @@
         <v>70</v>
       </c>
       <c r="AL9" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM9" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP9" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ9" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS9" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT9" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU9" s="1" t="s">
         <v>74</v>
@@ -2509,33 +2512,33 @@
         <v>76</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY9" s="1" t="s">
         <v>78</v>
       </c>
       <c r="AZ9" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BA9" s="1" t="s">
         <v>80</v>
       </c>
       <c r="BB9" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>53</v>
@@ -2547,7 +2550,7 @@
         <v>55</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>56</v>
@@ -2565,22 +2568,22 @@
         <v>60</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>62</v>
@@ -2589,10 +2592,10 @@
         <v>63</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V10" s="2" t="s">
         <v>65</v>
@@ -2603,29 +2606,29 @@
       </c>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD10" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI10" s="1" t="s">
         <v>69</v>
@@ -2635,31 +2638,31 @@
         <v>70</v>
       </c>
       <c r="AL10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ10" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS10" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT10" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU10" s="1" t="s">
         <v>74</v>
@@ -2671,7 +2674,7 @@
         <v>76</v>
       </c>
       <c r="AX10" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY10" s="1" t="s">
         <v>78</v>
@@ -2683,21 +2686,21 @@
         <v>80</v>
       </c>
       <c r="BB10" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>53</v>
@@ -2709,7 +2712,7 @@
         <v>55</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>56</v>
@@ -2727,22 +2730,22 @@
         <v>60</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>62</v>
@@ -2751,10 +2754,10 @@
         <v>63</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V11" s="2" t="s">
         <v>65</v>
@@ -2765,29 +2768,29 @@
       </c>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AA11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="AD11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI11" s="1" t="s">
         <v>69</v>
@@ -2797,31 +2800,31 @@
         <v>70</v>
       </c>
       <c r="AL11" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM11" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP11" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ11" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS11" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT11" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU11" s="1" t="s">
         <v>74</v>
@@ -2833,25 +2836,25 @@
         <v>76</v>
       </c>
       <c r="AX11" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY11" s="1" t="s">
         <v>78</v>
       </c>
       <c r="AZ11" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BA11" s="1" t="s">
         <v>80</v>
       </c>
       <c r="BB11" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2888,28 +2891,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>90</v>
-      </c>
-      <c r="I1" t="s">
-        <v>91</v>
       </c>
       <c r="J1" t="s">
         <v>39</v>
@@ -2920,31 +2923,31 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>72</v>
@@ -2955,16 +2958,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2978,14 +2981,14 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -3005,10 +3008,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CE12"/>
+  <dimension ref="A1:CE13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="CE12" sqref="CE12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3249,99 +3252,99 @@
         <v>52</v>
       </c>
       <c r="BB1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BC1" t="s">
         <v>107</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>108</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>109</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>110</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>111</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>112</v>
       </c>
-      <c r="BH1" t="s">
-        <v>113</v>
-      </c>
       <c r="BI1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BK1" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BL1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BM1" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>157</v>
       </c>
       <c r="BN1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="BO1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BP1" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="BQ1" s="7" t="s">
         <v>23</v>
       </c>
       <c r="BR1" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BS1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="BT1" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="BU1" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="BU1" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="BV1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="BW1" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="BX1" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BY1" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="BZ1" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="CA1" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="CA1" s="7" t="s">
+      <c r="CB1" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="CB1" s="7" t="s">
+      <c r="CC1" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="CC1" s="7" t="s">
+      <c r="CD1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="CD1" s="7" t="s">
+      <c r="CE1" s="7" t="s">
         <v>226</v>
-      </c>
-      <c r="CE1" s="7" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
@@ -3351,7 +3354,7 @@
       <c r="AB2" s="5"/>
       <c r="AL2" s="5"/>
       <c r="AN2" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AP2" s="5"/>
       <c r="AQ2">
@@ -3361,15 +3364,15 @@
         <v>80000</v>
       </c>
       <c r="AS2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AW2" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
@@ -3379,7 +3382,7 @@
       <c r="AB3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AN3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AP3" s="5"/>
       <c r="AQ3">
@@ -3389,15 +3392,15 @@
         <v>80000</v>
       </c>
       <c r="AS3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AW3" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
@@ -3407,7 +3410,7 @@
       <c r="AB4" s="5"/>
       <c r="AL4" s="5"/>
       <c r="AN4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AP4" s="5"/>
       <c r="AQ4">
@@ -3417,36 +3420,36 @@
         <v>15</v>
       </c>
       <c r="AS4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AW4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AW4" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="BB4" t="s">
+        <v>113</v>
+      </c>
+      <c r="BC4" t="s">
         <v>114</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BD4" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BD4" s="6" t="s">
+      <c r="BE4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BE4" s="2" t="s">
+      <c r="BF4" t="s">
         <v>117</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BG4" t="s">
         <v>118</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BH4" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="BH4" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
@@ -3456,7 +3459,7 @@
       <c r="AB5" s="5"/>
       <c r="AL5" s="5"/>
       <c r="AN5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AP5" s="5"/>
       <c r="AQ5">
@@ -3466,36 +3469,36 @@
         <v>15</v>
       </c>
       <c r="AS5" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AW5" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AW5" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="BB5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BC5" t="s">
         <v>114</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BD5" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BD5" s="6" t="s">
+      <c r="BE5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BE5" s="2" t="s">
+      <c r="BF5" t="s">
         <v>117</v>
       </c>
-      <c r="BF5" t="s">
+      <c r="BG5" t="s">
         <v>118</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="BH5" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="BH5" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -3536,7 +3539,7 @@
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
@@ -3547,7 +3550,7 @@
       <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
       <c r="AW6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
@@ -3577,7 +3580,7 @@
     </row>
     <row r="7" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3618,7 +3621,7 @@
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
@@ -3629,7 +3632,7 @@
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
       <c r="AW7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
@@ -3643,13 +3646,13 @@
       <c r="BG7" s="7"/>
       <c r="BH7" s="7"/>
       <c r="BI7" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BJ7" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BJ7" s="7" t="s">
-        <v>146</v>
-      </c>
       <c r="BK7" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BL7" s="7" t="s">
         <v>59</v>
@@ -3669,7 +3672,7 @@
     </row>
     <row r="8" spans="1:83" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3710,7 +3713,7 @@
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
@@ -3721,7 +3724,7 @@
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
       <c r="AW8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
@@ -3735,13 +3738,13 @@
       <c r="BG8" s="7"/>
       <c r="BH8" s="7"/>
       <c r="BI8" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BJ8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BJ8" s="7" t="s">
-        <v>146</v>
-      </c>
       <c r="BK8" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BL8" s="7" t="s">
         <v>59</v>
@@ -3750,19 +3753,19 @@
         <v>48634</v>
       </c>
       <c r="BN8" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="BO8" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="BO8" s="7" t="s">
+      <c r="BP8" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="BP8" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="BQ8" s="7" t="s">
         <v>66</v>
       </c>
       <c r="BR8" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BS8" s="7" t="s">
         <v>60</v>
@@ -3771,88 +3774,105 @@
         <v>6323145</v>
       </c>
       <c r="BU8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BV8" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="BV8" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="BW8" s="7"/>
     </row>
     <row r="9" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AN9" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AW9" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BW9" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BX9" t="s">
         <v>173</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AN10" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AW10" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="BW10" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="S11" t="s">
         <v>168</v>
       </c>
-      <c r="S11" t="s">
-        <v>169</v>
-      </c>
       <c r="AN11" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AW11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BY11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="AN12" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>190</v>
+      </c>
+      <c r="BZ12" t="s">
         <v>216</v>
       </c>
-      <c r="AN12" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AW12" t="s">
-        <v>191</v>
-      </c>
-      <c r="BZ12" t="s">
+      <c r="CA12" t="s">
         <v>217</v>
       </c>
-      <c r="CA12" t="s">
+      <c r="CB12" t="s">
         <v>218</v>
-      </c>
-      <c r="CB12" t="s">
-        <v>219</v>
       </c>
       <c r="CC12">
         <v>2015</v>
       </c>
       <c r="CD12" t="s">
+        <v>219</v>
+      </c>
+      <c r="CE12" t="s">
         <v>220</v>
       </c>
-      <c r="CE12" t="s">
-        <v>221</v>
+    </row>
+    <row r="13" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="S13" t="s">
+        <v>168</v>
+      </c>
+      <c r="AN13" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>190</v>
+      </c>
+      <c r="BY13" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3894,45 +3914,45 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
         <v>122</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>123</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
       </c>
       <c r="G1" t="s">
         <v>43</v>
       </c>
       <c r="H1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" t="s">
         <v>205</v>
       </c>
-      <c r="I1" t="s">
-        <v>206</v>
-      </c>
       <c r="J1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
         <v>129</v>
-      </c>
-      <c r="F2" t="s">
-        <v>130</v>
       </c>
       <c r="G2" s="4">
         <v>80572.460000000006</v>
@@ -3940,56 +3960,56 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" t="s">
         <v>200</v>
       </c>
-      <c r="B5" t="s">
-        <v>201</v>
-      </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" t="s">
         <v>129</v>
-      </c>
-      <c r="F5" t="s">
-        <v>130</v>
       </c>
       <c r="G5" s="4">
         <v>80572.460000000006</v>
       </c>
       <c r="H5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I5" t="s">
         <v>202</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>203</v>
-      </c>
-      <c r="J5" t="s">
-        <v>204</v>
       </c>
       <c r="L5" s="4"/>
     </row>
@@ -4000,6 +4020,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4232,31 +4276,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4273,22 +4311,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added new scenario for correct address format.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E44798-89CA-41E0-99DE-6630B1222FA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CCE230-23CA-437A-987C-411CDC24D9EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="246">
   <si>
     <t>scenario</t>
   </si>
@@ -746,6 +746,21 @@
   </si>
   <si>
     <t>CREATE_ELEMENT_ENTRIES</t>
+  </si>
+  <si>
+    <t>ADDRESS_CORRECTION</t>
+  </si>
+  <si>
+    <t>Bloomington</t>
+  </si>
+  <si>
+    <t>55438</t>
+  </si>
+  <si>
+    <t>8300 Norman Centre Dr</t>
+  </si>
+  <si>
+    <t>8th Floor</t>
   </si>
 </sst>
 </file>
@@ -1087,73 +1102,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
+    <sheetView topLeftCell="AW1" workbookViewId="0">
       <selection activeCell="BJ4" sqref="BJ4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1335,7 +1350,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1497,7 +1512,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1659,7 +1674,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -1821,7 +1836,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -1983,7 +1998,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2145,7 +2160,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>143</v>
       </c>
@@ -2209,7 +2224,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2371,7 +2386,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -2533,7 +2548,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2695,7 +2710,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>234</v>
       </c>
@@ -2871,22 +2886,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5234375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2921,7 +2936,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -2956,7 +2971,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -2979,7 +2994,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3008,90 +3023,91 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CE13"/>
+  <dimension ref="A1:CE14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5546875" customWidth="1"/>
-    <col min="62" max="62" width="26.88671875" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" customWidth="1"/>
-    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5234375" customWidth="1"/>
+    <col min="62" max="62" width="26.89453125" customWidth="1"/>
+    <col min="63" max="63" width="18.5234375" customWidth="1"/>
+    <col min="64" max="64" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.1015625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5234375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.1015625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5234375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5546875" customWidth="1"/>
+    <col min="75" max="75" width="42.5234375" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:83" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3342,7 +3358,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -3370,7 +3386,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -3398,7 +3414,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -3447,7 +3463,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -3496,7 +3512,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>120</v>
       </c>
@@ -3578,7 +3594,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:83" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>210</v>
       </c>
@@ -3670,7 +3686,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:83" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:83" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>209</v>
       </c>
@@ -3781,7 +3797,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:83" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
         <v>206</v>
       </c>
@@ -3798,7 +3814,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:83" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
         <v>208</v>
       </c>
@@ -3812,7 +3828,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>167</v>
       </c>
@@ -3829,7 +3845,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7" t="s">
         <v>215</v>
       </c>
@@ -3858,7 +3874,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
         <v>239</v>
       </c>
@@ -3873,6 +3889,47 @@
       </c>
       <c r="BY13" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" t="s">
+        <v>245</v>
+      </c>
+      <c r="G14" t="s">
+        <v>242</v>
+      </c>
+      <c r="AN14" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>190</v>
+      </c>
+      <c r="BA14" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="BZ14" t="s">
+        <v>216</v>
+      </c>
+      <c r="CA14" t="s">
+        <v>217</v>
+      </c>
+      <c r="CB14" t="s">
+        <v>218</v>
+      </c>
+      <c r="CC14">
+        <v>2015</v>
+      </c>
+      <c r="CD14" t="s">
+        <v>219</v>
+      </c>
+      <c r="CE14" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3889,21 +3946,21 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.41796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1015625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3935,7 +3992,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -3958,7 +4015,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3969,7 +4026,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -3980,7 +4037,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -4020,6 +4077,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
@@ -4032,15 +4098,6 @@
     <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4277,19 +4334,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
First two HR scenario's scripted
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1D7FC6-6E05-4740-833A-392DA0A6204F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A7058-1D3E-4189-AEBA-7BE16223F0EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,17 +13,23 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="232">
   <si>
     <t>scenario</t>
   </si>
@@ -671,6 +677,54 @@
   </si>
   <si>
     <t>3/21/19</t>
+  </si>
+  <si>
+    <t>CORRECT_PERSONAL_DESCRIPTIVE_FLEXFIELD_INFORMATION</t>
+  </si>
+  <si>
+    <t>countryOfBirth</t>
+  </si>
+  <si>
+    <t>regionOfBirth</t>
+  </si>
+  <si>
+    <t>townOfBirth</t>
+  </si>
+  <si>
+    <t>PENNSYLVANIA</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>American English</t>
+  </si>
+  <si>
+    <t>A rhesus positive</t>
+  </si>
+  <si>
+    <t>correspondenceLanguage</t>
+  </si>
+  <si>
+    <t>bloodType</t>
+  </si>
+  <si>
+    <t>1/1/90</t>
+  </si>
+  <si>
+    <t>ADDING_EXISTING_EMPLOYEE_AS_AN_EMERGENCY_CONTACT</t>
+  </si>
+  <si>
+    <t>contactType</t>
+  </si>
+  <si>
+    <t>Emergency</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>emergencyContact</t>
   </si>
 </sst>
 </file>
@@ -1012,73 +1066,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +1314,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1422,7 +1476,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1584,7 +1638,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1746,7 +1800,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>208</v>
       </c>
@@ -1908,7 +1962,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -2070,7 +2124,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>144</v>
       </c>
@@ -2134,7 +2188,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2310,22 +2364,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2360,7 +2414,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -2395,7 +2449,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2418,7 +2472,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2447,90 +2501,90 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BY11"/>
+  <dimension ref="A1:CF13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="CE1" sqref="CE1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5546875" customWidth="1"/>
-    <col min="62" max="62" width="26.88671875" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" customWidth="1"/>
-    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5546875" customWidth="1"/>
+    <col min="75" max="75" width="42.5703125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:84" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2762,8 +2816,29 @@
       <c r="BY1" s="7" t="s">
         <v>172</v>
       </c>
+      <c r="BZ1" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="CA1" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="CB1" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="CC1" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="CD1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="CE1" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="CF1" s="7" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -2791,7 +2866,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -2819,7 +2894,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -2868,7 +2943,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -2917,7 +2992,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>121</v>
       </c>
@@ -2999,7 +3074,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:84" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>211</v>
       </c>
@@ -3091,7 +3166,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:77" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:84" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>210</v>
       </c>
@@ -3202,7 +3277,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:77" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>207</v>
       </c>
@@ -3219,7 +3294,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:84" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>209</v>
       </c>
@@ -3233,7 +3308,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>168</v>
       </c>
@@ -3248,6 +3323,52 @@
       </c>
       <c r="BY11" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:84" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AN12" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>191</v>
+      </c>
+      <c r="BZ12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="CA12" t="s">
+        <v>220</v>
+      </c>
+      <c r="CB12" t="s">
+        <v>221</v>
+      </c>
+      <c r="CC12" t="s">
+        <v>222</v>
+      </c>
+      <c r="CD12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:84" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="AN13" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>191</v>
+      </c>
+      <c r="CE13" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF13" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3264,21 +3385,21 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3310,7 +3431,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -3333,7 +3454,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -3344,7 +3465,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -3355,7 +3476,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>200</v>
       </c>
@@ -3395,30 +3516,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3651,25 +3748,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3686,4 +3789,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added new scenarios to add new address type
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB30C2DF-F14F-4E4E-A96A-2528DDB66B6A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0644378E-B945-4AB1-AD1C-90621182D7FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="249">
   <si>
     <t>scenario</t>
   </si>
@@ -764,6 +764,12 @@
   </si>
   <si>
     <t>MANAGE_PERSON_ADDRESS_UPDATE</t>
+  </si>
+  <si>
+    <t>MANAGE_PERSON_ADD_ALTERNATE_ADDRESS</t>
+  </si>
+  <si>
+    <t>Resident Tax Address</t>
   </si>
 </sst>
 </file>
@@ -3026,10 +3032,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CE15"/>
+  <dimension ref="A1:CE16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BK16" sqref="BK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3976,6 +3983,50 @@
         <v>220</v>
       </c>
     </row>
+    <row r="16" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B16" t="s">
+        <v>244</v>
+      </c>
+      <c r="C16" t="s">
+        <v>245</v>
+      </c>
+      <c r="G16" t="s">
+        <v>242</v>
+      </c>
+      <c r="AN16" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>190</v>
+      </c>
+      <c r="BA16" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="BK16" t="s">
+        <v>248</v>
+      </c>
+      <c r="BZ16" t="s">
+        <v>216</v>
+      </c>
+      <c r="CA16" t="s">
+        <v>217</v>
+      </c>
+      <c r="CB16" t="s">
+        <v>218</v>
+      </c>
+      <c r="CC16">
+        <v>2015</v>
+      </c>
+      <c r="CD16" t="s">
+        <v>219</v>
+      </c>
+      <c r="CE16" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4121,6 +4172,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4353,21 +4419,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4378,6 +4429,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4396,16 +4457,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Scripted 3rd Test Case.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A7058-1D3E-4189-AEBA-7BE16223F0EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1BD54-32DE-46D9-BB8E-C159F2305203}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="239">
   <si>
     <t>scenario</t>
   </si>
@@ -725,6 +725,27 @@
   </si>
   <si>
     <t>emergencyContact</t>
+  </si>
+  <si>
+    <t>MODIFY_EXISTING_EMERGENCY_CONTACT</t>
+  </si>
+  <si>
+    <t>Home Phone</t>
+  </si>
+  <si>
+    <t>emergencyContactType</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>areaCode</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>6323145</t>
   </si>
 </sst>
 </file>
@@ -766,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -784,6 +805,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1066,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,10 +2525,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CF13"/>
+  <dimension ref="A1:CG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
-      <selection activeCell="CE1" sqref="CE1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2518,63 +2542,63 @@
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5703125" customWidth="1"/>
-    <col min="62" max="62" width="26.85546875" customWidth="1"/>
-    <col min="63" max="63" width="18.5703125" customWidth="1"/>
-    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="46" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="28.5703125" customWidth="1"/>
+    <col min="60" max="60" width="26.85546875" customWidth="1"/>
+    <col min="61" max="61" width="18.5703125" customWidth="1"/>
+    <col min="62" max="62" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8" customWidth="1"/>
+    <col min="66" max="67" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="8.140625" customWidth="1"/>
     <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -2584,7 +2608,7 @@
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2616,181 +2640,181 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="W1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="BH1" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BI1" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BL1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="BM1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="BN1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="BP1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BI1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="BJ1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="BK1" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="BL1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="BN1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="BO1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="BQ1" s="7" t="s">
-        <v>23</v>
+        <v>236</v>
       </c>
       <c r="BR1" s="7" t="s">
         <v>160</v>
@@ -2837,162 +2861,165 @@
       <c r="CF1" s="7" t="s">
         <v>231</v>
       </c>
+      <c r="CG1" s="7" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AN2" s="1" t="s">
+      <c r="L2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AL2" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AP2" s="5"/>
-      <c r="AQ2">
+      <c r="AN2" s="5"/>
+      <c r="AO2">
         <v>10043</v>
       </c>
-      <c r="AR2" s="4">
+      <c r="AP2" s="4">
         <v>80000</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AL3" s="5"/>
-      <c r="AN3" s="1" t="s">
+      <c r="L3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AL3" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AP3" s="5"/>
-      <c r="AQ3">
+      <c r="AN3" s="5"/>
+      <c r="AO3">
         <v>10043</v>
       </c>
-      <c r="AR3" s="4">
+      <c r="AP3" s="4">
         <v>80000</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AQ3" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AW3" s="1" t="s">
+      <c r="AU3" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AL4" s="5"/>
-      <c r="AN4" s="1" t="s">
+      <c r="L4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AL4" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AP4" s="5"/>
-      <c r="AQ4">
+      <c r="AN4" s="5"/>
+      <c r="AO4">
         <v>10043</v>
       </c>
-      <c r="AR4">
+      <c r="AP4">
         <v>15</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AW4" s="1" t="s">
+      <c r="AU4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="AZ4" t="s">
         <v>114</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BA4" t="s">
         <v>115</v>
       </c>
-      <c r="BD4" s="6" t="s">
+      <c r="BB4" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="BE4" s="2" t="s">
+      <c r="BC4" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BD4" t="s">
         <v>118</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BE4" t="s">
         <v>119</v>
       </c>
-      <c r="BH4" s="6" t="s">
+      <c r="BF4" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AL5" s="5"/>
-      <c r="AN5" s="1" t="s">
+      <c r="L5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AL5" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AP5" s="5"/>
-      <c r="AQ5">
+      <c r="AN5" s="5"/>
+      <c r="AO5">
         <v>10043</v>
       </c>
-      <c r="AR5">
+      <c r="AP5">
         <v>15</v>
       </c>
-      <c r="AS5" s="1" t="s">
+      <c r="AQ5" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AW5" s="1" t="s">
+      <c r="AU5" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="AZ5" t="s">
         <v>114</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BA5" t="s">
         <v>115</v>
       </c>
-      <c r="BD5" s="6" t="s">
+      <c r="BB5" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="BE5" s="2" t="s">
+      <c r="BC5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="BF5" t="s">
+      <c r="BD5" t="s">
         <v>118</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="BE5" t="s">
         <v>119</v>
       </c>
-      <c r="BH5" s="6" t="s">
+      <c r="BF5" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>121</v>
       </c>
@@ -3032,22 +3059,22 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
       <c r="AK6" s="7"/>
-      <c r="AL6" s="7"/>
+      <c r="AL6" s="7" t="s">
+        <v>176</v>
+      </c>
       <c r="AM6" s="7"/>
-      <c r="AN6" s="7" t="s">
-        <v>176</v>
-      </c>
+      <c r="AN6" s="7"/>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
       <c r="AQ6" s="7"/>
       <c r="AR6" s="7"/>
       <c r="AS6" s="7"/>
       <c r="AT6" s="7"/>
-      <c r="AU6" s="7"/>
+      <c r="AU6" t="s">
+        <v>191</v>
+      </c>
       <c r="AV6" s="7"/>
-      <c r="AW6" t="s">
-        <v>191</v>
-      </c>
+      <c r="AW6" s="7"/>
       <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
       <c r="AZ6" s="7"/>
@@ -3074,7 +3101,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:84" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>211</v>
       </c>
@@ -3114,22 +3141,22 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
       <c r="AK7" s="7"/>
-      <c r="AL7" s="7"/>
+      <c r="AL7" s="7" t="s">
+        <v>176</v>
+      </c>
       <c r="AM7" s="7"/>
-      <c r="AN7" s="7" t="s">
-        <v>176</v>
-      </c>
+      <c r="AN7" s="7"/>
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
       <c r="AQ7" s="7"/>
       <c r="AR7" s="7"/>
       <c r="AS7" s="7"/>
       <c r="AT7" s="7"/>
-      <c r="AU7" s="7"/>
+      <c r="AU7" t="s">
+        <v>213</v>
+      </c>
       <c r="AV7" s="7"/>
-      <c r="AW7" t="s">
-        <v>213</v>
-      </c>
+      <c r="AW7" s="7"/>
       <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
       <c r="AZ7" s="7"/>
@@ -3139,23 +3166,23 @@
       <c r="BD7" s="7"/>
       <c r="BE7" s="7"/>
       <c r="BF7" s="7"/>
-      <c r="BG7" s="7"/>
-      <c r="BH7" s="7"/>
+      <c r="BG7" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BH7" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="BI7" s="7" t="s">
-        <v>145</v>
+        <v>212</v>
       </c>
       <c r="BJ7" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="BK7" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="BL7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BM7" s="7">
+      <c r="BK7" s="7">
         <v>48634</v>
       </c>
+      <c r="BL7" s="7"/>
+      <c r="BM7" s="7"/>
       <c r="BN7" s="7"/>
       <c r="BO7" s="7"/>
       <c r="BP7" s="7"/>
@@ -3166,7 +3193,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:84" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>210</v>
       </c>
@@ -3206,22 +3233,22 @@
       <c r="AI8" s="7"/>
       <c r="AJ8" s="7"/>
       <c r="AK8" s="7"/>
-      <c r="AL8" s="7"/>
+      <c r="AL8" s="7" t="s">
+        <v>176</v>
+      </c>
       <c r="AM8" s="7"/>
-      <c r="AN8" s="7" t="s">
-        <v>176</v>
-      </c>
+      <c r="AN8" s="7"/>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
       <c r="AQ8" s="7"/>
       <c r="AR8" s="7"/>
       <c r="AS8" s="7"/>
       <c r="AT8" s="7"/>
-      <c r="AU8" s="7"/>
+      <c r="AU8" t="s">
+        <v>213</v>
+      </c>
       <c r="AV8" s="7"/>
-      <c r="AW8" t="s">
-        <v>213</v>
-      </c>
+      <c r="AW8" s="7"/>
       <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
       <c r="AZ8" s="7"/>
@@ -3231,35 +3258,37 @@
       <c r="BD8" s="7"/>
       <c r="BE8" s="7"/>
       <c r="BF8" s="7"/>
-      <c r="BG8" s="7"/>
-      <c r="BH8" s="7"/>
+      <c r="BG8" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BH8" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="BI8" s="7" t="s">
-        <v>145</v>
+        <v>212</v>
       </c>
       <c r="BJ8" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="BK8" s="7" t="s">
-        <v>212</v>
+        <v>59</v>
+      </c>
+      <c r="BK8" s="7">
+        <v>48634</v>
       </c>
       <c r="BL8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="BM8" s="7">
-        <v>48634</v>
+        <v>147</v>
+      </c>
+      <c r="BM8" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="BN8" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="BO8" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="BP8" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="BQ8" s="7" t="s">
         <v>66</v>
       </c>
+      <c r="BQ8" s="7"/>
       <c r="BR8" s="7" t="s">
         <v>150</v>
       </c>
@@ -3277,14 +3306,14 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:84" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="AN9" s="7" t="s">
+      <c r="AL9" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AW9" s="7" t="s">
+      <c r="AU9" s="7" t="s">
         <v>175</v>
       </c>
       <c r="BW9" s="7" t="s">
@@ -3294,48 +3323,48 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:84" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="AN10" s="7" t="s">
+      <c r="AL10" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AW10" s="7" t="s">
+      <c r="AU10" s="7" t="s">
         <v>192</v>
       </c>
       <c r="BW10" s="8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="S11" t="s">
+      <c r="R11" t="s">
         <v>169</v>
       </c>
-      <c r="AN11" s="7" t="s">
+      <c r="AL11" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AW11" t="s">
+      <c r="AU11" t="s">
         <v>191</v>
       </c>
       <c r="BY11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:84" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AN12" s="7" t="s">
+      <c r="AL12" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AW12" t="s">
+      <c r="AU12" t="s">
         <v>191</v>
       </c>
       <c r="BZ12" s="1" t="s">
@@ -3354,14 +3383,14 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:84" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="AN13" s="7" t="s">
+      <c r="AL13" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AW13" t="s">
+      <c r="AU13" t="s">
         <v>191</v>
       </c>
       <c r="CE13" t="s">
@@ -3369,6 +3398,35 @@
       </c>
       <c r="CF13" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:85" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL14" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>191</v>
+      </c>
+      <c r="BL14" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="BM14" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="BQ14" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="BS14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BT14" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="CG14" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3516,6 +3574,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3748,21 +3821,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3773,6 +3831,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3791,16 +3859,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
3rd Test case scripting completed.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1BD54-32DE-46D9-BB8E-C159F2305203}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DD38E9-7816-4EF9-9E47-C9F0610BC27F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="240">
   <si>
     <t>scenario</t>
   </si>
@@ -746,6 +746,9 @@
   </si>
   <si>
     <t>6323145</t>
+  </si>
+  <si>
+    <t>Dallas</t>
   </si>
 </sst>
 </file>
@@ -1090,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2527,8 +2530,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="AR1" sqref="AR1"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,7 +2543,7 @@
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3404,11 +3409,29 @@
       <c r="A14" s="7" t="s">
         <v>232</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="AL14" s="7" t="s">
         <v>176</v>
       </c>
+      <c r="AR14" t="s">
+        <v>74</v>
+      </c>
       <c r="AU14" t="s">
         <v>191</v>
+      </c>
+      <c r="AY14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="BG14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BH14" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="BL14" s="7" t="s">
         <v>147</v>
@@ -3574,6 +3597,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
@@ -3588,7 +3620,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3821,16 +3853,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3840,7 +3871,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3857,12 +3888,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
latest name correction changes to local branch
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0644378E-B945-4AB1-AD1C-90621182D7FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,9 +12,9 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="250">
   <si>
     <t>scenario</t>
   </si>
@@ -770,13 +769,16 @@
   </si>
   <si>
     <t>Resident Tax Address</t>
+  </si>
+  <si>
+    <t>MANANGE_PERSON_NAME_CORRECTION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1101,83 +1103,83 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="BJ4" sqref="BJ4"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="AX12" sqref="AX12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:60" ht="30">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1521,7 +1523,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:60" ht="30">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:60" ht="30">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:60" ht="45">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -2007,7 +2009,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:60" ht="30">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2169,7 +2171,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:60" ht="30">
       <c r="A7" s="7" t="s">
         <v>143</v>
       </c>
@@ -2233,7 +2235,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:60" ht="30">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:60" ht="30">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -2557,7 +2559,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:60" ht="30">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2719,7 +2721,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:60" ht="30">
       <c r="A11" s="1" t="s">
         <v>234</v>
       </c>
@@ -2879,6 +2881,17 @@
       </c>
       <c r="BH11" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:60">
+      <c r="A12" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX12" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2888,29 +2901,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5234375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2945,7 +2958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -2980,7 +2993,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -3003,7 +3016,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3031,93 +3044,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CE16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BK16" sqref="BK16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5234375" customWidth="1"/>
-    <col min="62" max="62" width="26.89453125" customWidth="1"/>
-    <col min="63" max="63" width="18.5234375" customWidth="1"/>
-    <col min="64" max="64" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5703125" customWidth="1"/>
+    <col min="62" max="62" width="26.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.5703125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5234375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5234375" customWidth="1"/>
+    <col min="75" max="75" width="42.5703125" customWidth="1"/>
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:83" ht="60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3368,7 +3381,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:83">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -3396,7 +3409,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:83">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -3424,7 +3437,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:83">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -3473,7 +3486,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:83">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -3522,7 +3535,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:83">
       <c r="A6" s="7" t="s">
         <v>120</v>
       </c>
@@ -3604,7 +3617,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:83" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:83" ht="30">
       <c r="A7" s="7" t="s">
         <v>210</v>
       </c>
@@ -3696,7 +3709,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:83" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:83" ht="75">
       <c r="A8" s="7" t="s">
         <v>209</v>
       </c>
@@ -3807,7 +3820,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:83" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:83" ht="45">
       <c r="A9" s="7" t="s">
         <v>206</v>
       </c>
@@ -3824,7 +3837,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:83" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:83" ht="45">
       <c r="A10" s="7" t="s">
         <v>208</v>
       </c>
@@ -3838,7 +3851,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:83">
       <c r="A11" s="7" t="s">
         <v>167</v>
       </c>
@@ -3855,7 +3868,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:83">
       <c r="A12" s="7" t="s">
         <v>215</v>
       </c>
@@ -3884,7 +3897,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:83">
       <c r="A13" s="7" t="s">
         <v>239</v>
       </c>
@@ -3901,7 +3914,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:83">
       <c r="A14" s="7" t="s">
         <v>241</v>
       </c>
@@ -3942,7 +3955,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:83">
       <c r="A15" s="7" t="s">
         <v>246</v>
       </c>
@@ -3983,7 +3996,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:83">
       <c r="A16" s="7" t="s">
         <v>247</v>
       </c>
@@ -4034,28 +4047,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1015625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4087,7 +4100,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4110,7 +4123,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4121,7 +4134,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -4132,7 +4145,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -4187,6 +4200,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4419,15 +4441,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>
@@ -4439,6 +4452,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4455,12 +4476,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TestData.xlsx is updated with my changes
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5128D899-7047-4ED5-8522-816DC9CF1CD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -12,17 +13,23 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="274">
   <si>
     <t>scenario</t>
   </si>
@@ -772,13 +779,85 @@
   </si>
   <si>
     <t>MANANGE_PERSON_NAME_CORRECTION</t>
+  </si>
+  <si>
+    <t>CORRECT_PERSONAL_DESCRIPTIVE_FLEXFIELD_INFORMATION</t>
+  </si>
+  <si>
+    <t>ADDING_EXISTING_EMPLOYEE_AS_AN_EMERGENCY_CONTACT</t>
+  </si>
+  <si>
+    <t>MODIFY_EXISTING_EMERGENCY_CONTACT</t>
+  </si>
+  <si>
+    <t>1/1/90</t>
+  </si>
+  <si>
+    <t>countryOfBirth</t>
+  </si>
+  <si>
+    <t>regionOfBirth</t>
+  </si>
+  <si>
+    <t>townOfBirth</t>
+  </si>
+  <si>
+    <t>correspondenceLanguage</t>
+  </si>
+  <si>
+    <t>bloodType</t>
+  </si>
+  <si>
+    <t>contactType</t>
+  </si>
+  <si>
+    <t>emergencyContact</t>
+  </si>
+  <si>
+    <t>emergencyContactType</t>
+  </si>
+  <si>
+    <t>PENNSYLVANIA</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>American English</t>
+  </si>
+  <si>
+    <t>A rhesus positive</t>
+  </si>
+  <si>
+    <t>Emergency</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Home Phone</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>areaCode</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>6323145</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -831,6 +910,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1103,21 +1185,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="AX12" sqref="AX12"/>
+    <sheetView topLeftCell="AT7" workbookViewId="0">
+      <selection activeCell="BB17" sqref="BB17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1179,7 +1261,7 @@
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1443,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="30">
+    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1523,7 +1605,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:60" ht="30">
+    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1685,7 +1767,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:60" ht="30">
+    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -1847,7 +1929,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="45">
+    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -2009,7 +2091,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:60" ht="30">
+    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2171,7 +2253,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="30">
+    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>143</v>
       </c>
@@ -2235,7 +2317,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="30">
+    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2397,7 +2479,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:60" ht="30">
+    <row r="9" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -2559,7 +2641,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:60" ht="30">
+    <row r="10" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2721,7 +2803,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="30">
+    <row r="11" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>234</v>
       </c>
@@ -2883,7 +2965,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -2901,14 +2983,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -2923,7 +3005,7 @@
     <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2958,7 +3040,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -2993,7 +3075,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -3016,7 +3098,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3044,15 +3126,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CE16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:CP19"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BK16" sqref="BK16"/>
+    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CP19" sqref="CP19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3063,74 +3145,77 @@
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5703125" customWidth="1"/>
-    <col min="62" max="62" width="26.85546875" customWidth="1"/>
-    <col min="63" max="63" width="18.5703125" customWidth="1"/>
-    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5703125" customWidth="1"/>
-    <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.5703125" customWidth="1"/>
+    <col min="63" max="63" width="26.85546875" customWidth="1"/>
+    <col min="64" max="64" width="18.5703125" customWidth="1"/>
+    <col min="65" max="65" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="8" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8" customWidth="1"/>
+    <col min="69" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.5703125" customWidth="1"/>
+    <col min="73" max="73" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="8" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="42.5703125" customWidth="1"/>
+    <col min="79" max="79" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="60">
+    <row r="1" spans="1:94" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3159,383 +3244,416 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>106</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>107</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>108</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>109</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>110</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>111</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>112</v>
       </c>
-      <c r="BI1" s="7" t="s">
+      <c r="BJ1" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BK1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BL1" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BM1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="BM1" s="7" t="s">
+      <c r="BN1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="BN1" s="7" t="s">
+      <c r="BO1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="BO1" s="7" t="s">
+      <c r="BP1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="BP1" s="7" t="s">
+      <c r="BR1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="BQ1" s="7" t="s">
+      <c r="BS1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="BR1" s="7" t="s">
+      <c r="BT1" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="BU1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="BS1" s="7" t="s">
+      <c r="BV1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="BT1" s="7" t="s">
+      <c r="BW1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="BU1" s="7" t="s">
+      <c r="BX1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="BV1" s="7" t="s">
+      <c r="BY1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="BW1" s="7" t="s">
+      <c r="BZ1" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="BX1" s="7" t="s">
+      <c r="CA1" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="BY1" s="7" t="s">
+      <c r="CB1" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="BZ1" s="7" t="s">
+      <c r="CC1" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="CA1" s="7" t="s">
+      <c r="CD1" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="CB1" s="7" t="s">
+      <c r="CE1" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="CC1" s="7" t="s">
+      <c r="CF1" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="CD1" s="7" t="s">
+      <c r="CG1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="CE1" s="7" t="s">
+      <c r="CH1" s="7" t="s">
         <v>226</v>
       </c>
+      <c r="CI1" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="CJ1" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="CK1" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="CL1" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="CM1" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="CN1" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="CO1" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="CP1" s="7" t="s">
+        <v>261</v>
+      </c>
     </row>
-    <row r="2" spans="1:83">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>102</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AN2" s="1" t="s">
+      <c r="N2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AO2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AP2" s="5"/>
-      <c r="AQ2">
+      <c r="AQ2" s="5"/>
+      <c r="AR2">
         <v>10043</v>
       </c>
-      <c r="AR2" s="4">
+      <c r="AS2" s="4">
         <v>80000</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:83">
+    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AL3" s="5"/>
-      <c r="AN3" s="1" t="s">
+      <c r="N3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AO3" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AP3" s="5"/>
-      <c r="AQ3">
+      <c r="AQ3" s="5"/>
+      <c r="AR3">
         <v>10043</v>
       </c>
-      <c r="AR3" s="4">
+      <c r="AS3" s="4">
         <v>80000</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AW3" s="1" t="s">
+      <c r="AX3" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:83">
+    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AL4" s="5"/>
-      <c r="AN4" s="1" t="s">
+      <c r="N4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AO4" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AP4" s="5"/>
-      <c r="AQ4">
+      <c r="AQ4" s="5"/>
+      <c r="AR4">
         <v>10043</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>15</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AW4" s="1" t="s">
+      <c r="AX4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BC4" t="s">
         <v>113</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BD4" t="s">
         <v>114</v>
       </c>
-      <c r="BD4" s="6" t="s">
+      <c r="BE4" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BE4" s="2" t="s">
+      <c r="BF4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BG4" t="s">
         <v>117</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>118</v>
       </c>
-      <c r="BH4" s="6" t="s">
+      <c r="BI4" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:83">
+    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AL5" s="5"/>
-      <c r="AN5" s="1" t="s">
+      <c r="N5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AO5" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AP5" s="5"/>
-      <c r="AQ5">
+      <c r="AQ5" s="5"/>
+      <c r="AR5">
         <v>10043</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>15</v>
       </c>
-      <c r="AS5" s="1" t="s">
+      <c r="AT5" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AW5" s="1" t="s">
+      <c r="AX5" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BC5" t="s">
         <v>113</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BD5" t="s">
         <v>114</v>
       </c>
-      <c r="BD5" s="6" t="s">
+      <c r="BE5" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BE5" s="2" t="s">
+      <c r="BF5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BF5" t="s">
+      <c r="BG5" t="s">
         <v>117</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="BH5" t="s">
         <v>118</v>
       </c>
-      <c r="BH5" s="6" t="s">
+      <c r="BI5" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:83">
+    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>120</v>
       </c>
@@ -3577,10 +3695,10 @@
       <c r="AK6" s="7"/>
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
-      <c r="AN6" s="7" t="s">
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
       <c r="AQ6" s="7"/>
       <c r="AR6" s="7"/>
@@ -3588,10 +3706,10 @@
       <c r="AT6" s="7"/>
       <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
-      <c r="AW6" t="s">
+      <c r="AW6" s="7"/>
+      <c r="AX6" t="s">
         <v>190</v>
       </c>
-      <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
       <c r="AZ6" s="7"/>
       <c r="BA6" s="7"/>
@@ -3616,8 +3734,11 @@
       <c r="BT6" s="7"/>
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
+      <c r="BW6" s="7"/>
+      <c r="BX6" s="7"/>
+      <c r="BY6" s="7"/>
     </row>
-    <row r="7" spans="1:83" ht="30">
+    <row r="7" spans="1:94" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>210</v>
       </c>
@@ -3659,10 +3780,10 @@
       <c r="AK7" s="7"/>
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
-      <c r="AN7" s="7" t="s">
+      <c r="AN7" s="7"/>
+      <c r="AO7" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
       <c r="AQ7" s="7"/>
       <c r="AR7" s="7"/>
@@ -3670,10 +3791,10 @@
       <c r="AT7" s="7"/>
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
-      <c r="AW7" t="s">
+      <c r="AW7" s="7"/>
+      <c r="AX7" t="s">
         <v>212</v>
       </c>
-      <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
       <c r="AZ7" s="7"/>
       <c r="BA7" s="7"/>
@@ -3684,22 +3805,22 @@
       <c r="BF7" s="7"/>
       <c r="BG7" s="7"/>
       <c r="BH7" s="7"/>
-      <c r="BI7" s="7" t="s">
+      <c r="BI7" s="7"/>
+      <c r="BJ7" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="BJ7" s="7" t="s">
+      <c r="BK7" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BK7" s="7" t="s">
+      <c r="BL7" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="BL7" s="7" t="s">
+      <c r="BM7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BM7" s="7">
+      <c r="BN7" s="7">
         <v>48634</v>
       </c>
-      <c r="BN7" s="7"/>
       <c r="BO7" s="7"/>
       <c r="BP7" s="7"/>
       <c r="BQ7" s="7"/>
@@ -3708,8 +3829,11 @@
       <c r="BT7" s="7"/>
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
+      <c r="BW7" s="7"/>
+      <c r="BX7" s="7"/>
+      <c r="BY7" s="7"/>
     </row>
-    <row r="8" spans="1:83" ht="75">
+    <row r="8" spans="1:94" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>209</v>
       </c>
@@ -3751,10 +3875,10 @@
       <c r="AK8" s="7"/>
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
-      <c r="AN8" s="7" t="s">
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
       <c r="AQ8" s="7"/>
       <c r="AR8" s="7"/>
@@ -3762,10 +3886,10 @@
       <c r="AT8" s="7"/>
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
-      <c r="AW8" t="s">
+      <c r="AW8" s="7"/>
+      <c r="AX8" t="s">
         <v>212</v>
       </c>
-      <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
       <c r="AZ8" s="7"/>
       <c r="BA8" s="7"/>
@@ -3776,145 +3900,148 @@
       <c r="BF8" s="7"/>
       <c r="BG8" s="7"/>
       <c r="BH8" s="7"/>
-      <c r="BI8" s="7" t="s">
+      <c r="BI8" s="7"/>
+      <c r="BJ8" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="BJ8" s="7" t="s">
+      <c r="BK8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BK8" s="7" t="s">
+      <c r="BL8" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="BL8" s="7" t="s">
+      <c r="BM8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BM8" s="7">
+      <c r="BN8" s="7">
         <v>48634</v>
       </c>
-      <c r="BN8" s="7" t="s">
+      <c r="BO8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="BO8" s="7" t="s">
+      <c r="BP8" s="7"/>
+      <c r="BQ8" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="BP8" s="7" t="s">
+      <c r="BR8" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="BQ8" s="7" t="s">
+      <c r="BS8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="BR8" s="7" t="s">
+      <c r="BT8" s="7"/>
+      <c r="BU8" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="BS8" s="7" t="s">
+      <c r="BV8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BT8" s="7">
+      <c r="BW8" s="7">
         <v>6323145</v>
       </c>
-      <c r="BU8" s="7" t="s">
+      <c r="BX8" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="BV8" s="7" t="s">
+      <c r="BY8" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="BW8" s="7"/>
+      <c r="BZ8" s="7"/>
     </row>
-    <row r="9" spans="1:83" ht="45">
+    <row r="9" spans="1:94" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="AN9" s="7" t="s">
+      <c r="AO9" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AW9" s="7" t="s">
+      <c r="AX9" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="BW9" s="7" t="s">
+      <c r="BZ9" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="BX9" t="s">
+      <c r="CA9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:83" ht="45">
+    <row r="10" spans="1:94" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="AN10" s="7" t="s">
+      <c r="AO10" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AW10" s="7" t="s">
+      <c r="AX10" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="BW10" s="8" t="s">
+      <c r="BZ10" s="8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:83">
+    <row r="11" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>168</v>
       </c>
-      <c r="AN11" s="7" t="s">
+      <c r="AO11" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AW11" t="s">
+      <c r="AX11" t="s">
         <v>190</v>
       </c>
-      <c r="BY11" t="s">
+      <c r="CB11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:83">
+    <row r="12" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="AN12" s="7" t="s">
+      <c r="AO12" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AW12" t="s">
+      <c r="AX12" t="s">
         <v>190</v>
       </c>
-      <c r="BZ12" t="s">
+      <c r="CC12" t="s">
         <v>216</v>
       </c>
-      <c r="CA12" t="s">
+      <c r="CD12" t="s">
         <v>217</v>
       </c>
-      <c r="CB12" t="s">
+      <c r="CE12" t="s">
         <v>218</v>
       </c>
-      <c r="CC12">
+      <c r="CF12">
         <v>2015</v>
       </c>
-      <c r="CD12" t="s">
+      <c r="CG12" t="s">
         <v>219</v>
       </c>
-      <c r="CE12" t="s">
+      <c r="CH12" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:83">
+    <row r="13" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>168</v>
       </c>
-      <c r="AN13" s="7" t="s">
+      <c r="AO13" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AW13" t="s">
+      <c r="AX13" t="s">
         <v>190</v>
       </c>
-      <c r="BY13" t="s">
+      <c r="CB13" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:83">
+    <row r="14" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>241</v>
       </c>
@@ -3927,35 +4054,35 @@
       <c r="G14" t="s">
         <v>242</v>
       </c>
-      <c r="AN14" s="7" t="s">
+      <c r="AO14" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AW14" t="s">
+      <c r="AX14" t="s">
         <v>190</v>
       </c>
-      <c r="BA14" s="6" t="s">
+      <c r="BB14" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="BZ14" t="s">
+      <c r="CC14" t="s">
         <v>216</v>
       </c>
-      <c r="CA14" t="s">
+      <c r="CD14" t="s">
         <v>217</v>
       </c>
-      <c r="CB14" t="s">
+      <c r="CE14" t="s">
         <v>218</v>
       </c>
-      <c r="CC14">
+      <c r="CF14">
         <v>2015</v>
       </c>
-      <c r="CD14" t="s">
+      <c r="CG14" t="s">
         <v>219</v>
       </c>
-      <c r="CE14" t="s">
+      <c r="CH14" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:83">
+    <row r="15" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>246</v>
       </c>
@@ -3968,35 +4095,35 @@
       <c r="G15" t="s">
         <v>242</v>
       </c>
-      <c r="AN15" s="7" t="s">
+      <c r="AO15" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AW15" t="s">
+      <c r="AX15" t="s">
         <v>190</v>
       </c>
-      <c r="BA15" s="6" t="s">
+      <c r="BB15" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="BZ15" t="s">
+      <c r="CC15" t="s">
         <v>216</v>
       </c>
-      <c r="CA15" t="s">
+      <c r="CD15" t="s">
         <v>217</v>
       </c>
-      <c r="CB15" t="s">
+      <c r="CE15" t="s">
         <v>218</v>
       </c>
-      <c r="CC15">
+      <c r="CF15">
         <v>2015</v>
       </c>
-      <c r="CD15" t="s">
+      <c r="CG15" t="s">
         <v>219</v>
       </c>
-      <c r="CE15" t="s">
+      <c r="CH15" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:83">
+    <row r="16" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>247</v>
       </c>
@@ -4009,35 +4136,128 @@
       <c r="G16" t="s">
         <v>242</v>
       </c>
-      <c r="AN16" s="7" t="s">
+      <c r="AO16" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AW16" t="s">
+      <c r="AX16" t="s">
         <v>190</v>
       </c>
-      <c r="BA16" s="6" t="s">
+      <c r="BB16" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="BK16" t="s">
+      <c r="BL16" t="s">
         <v>248</v>
       </c>
-      <c r="BZ16" t="s">
+      <c r="CC16" t="s">
         <v>216</v>
       </c>
-      <c r="CA16" t="s">
+      <c r="CD16" t="s">
         <v>217</v>
       </c>
-      <c r="CB16" t="s">
+      <c r="CE16" t="s">
         <v>218</v>
       </c>
-      <c r="CC16">
+      <c r="CF16">
         <v>2015</v>
       </c>
-      <c r="CD16" t="s">
+      <c r="CG16" t="s">
         <v>219</v>
       </c>
-      <c r="CE16" t="s">
+      <c r="CH16" t="s">
         <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AO17" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>190</v>
+      </c>
+      <c r="CI17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="CJ17" t="s">
+        <v>262</v>
+      </c>
+      <c r="CK17" t="s">
+        <v>263</v>
+      </c>
+      <c r="CL17" t="s">
+        <v>264</v>
+      </c>
+      <c r="CM17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AO18" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>190</v>
+      </c>
+      <c r="CN18" t="s">
+        <v>266</v>
+      </c>
+      <c r="CO18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AO19" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>74</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>190</v>
+      </c>
+      <c r="BB19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="BJ19" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BK19" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BO19" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="BP19" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="BT19" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="BV19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BW19" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="CP19" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4047,14 +4267,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -4068,7 +4288,7 @@
     <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4100,7 +4320,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4123,7 +4343,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4134,7 +4354,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -4145,7 +4365,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -4185,30 +4405,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4441,25 +4637,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4476,4 +4678,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added columns and updated.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DD38E9-7816-4EF9-9E47-C9F0610BC27F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5128D899-7047-4ED5-8522-816DC9CF1CD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="274">
   <si>
     <t>scenario</t>
   </si>
@@ -280,9 +280,6 @@
     <t>BILINGUAL_INDICATOR</t>
   </si>
   <si>
-    <t>UPDATE_ELEMENT_ENTRIES</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -679,9 +676,123 @@
     <t>3/21/19</t>
   </si>
   <si>
+    <t>ADD_SKILLS_AND_QUALIFICATION_DETAILS</t>
+  </si>
+  <si>
+    <t>Master's Degree</t>
+  </si>
+  <si>
+    <t>MS IT</t>
+  </si>
+  <si>
+    <t>University of Florida</t>
+  </si>
+  <si>
+    <t>Federal licenses</t>
+  </si>
+  <si>
+    <t>PKT13</t>
+  </si>
+  <si>
+    <t>degreeName</t>
+  </si>
+  <si>
+    <t>degreeMajor</t>
+  </si>
+  <si>
+    <t>degreeSchool</t>
+  </si>
+  <si>
+    <t>degreeYear</t>
+  </si>
+  <si>
+    <t>licenseName</t>
+  </si>
+  <si>
+    <t>licenseNumber</t>
+  </si>
+  <si>
+    <t>NEW_HIRE_NON_WORKER</t>
+  </si>
+  <si>
+    <t>Add Non-Worker</t>
+  </si>
+  <si>
+    <t>Creation of Non-Worker</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>Nonworker</t>
+  </si>
+  <si>
+    <t>NEW_HIRE_PENDING_WORKER</t>
+  </si>
+  <si>
+    <t>Contingent worker</t>
+  </si>
+  <si>
+    <t>NEW_HIRE_CONTINGENT_WORKER</t>
+  </si>
+  <si>
+    <t>Add Pending Worker</t>
+  </si>
+  <si>
+    <t>Add Contingent Worker</t>
+  </si>
+  <si>
+    <t>Placement to fill vacant position</t>
+  </si>
+  <si>
+    <t>Future hire to fill vacant position</t>
+  </si>
+  <si>
+    <t>ENTER_JOB_CHANGE</t>
+  </si>
+  <si>
+    <t>CREATE_ELEMENT_ENTRIES</t>
+  </si>
+  <si>
+    <t>ADDRESS_CORRECTION</t>
+  </si>
+  <si>
+    <t>Bloomington</t>
+  </si>
+  <si>
+    <t>55438</t>
+  </si>
+  <si>
+    <t>8300 Norman Centre Dr</t>
+  </si>
+  <si>
+    <t>8th Floor</t>
+  </si>
+  <si>
+    <t>MANAGE_PERSON_ADDRESS_UPDATE</t>
+  </si>
+  <si>
+    <t>MANAGE_PERSON_ADD_ALTERNATE_ADDRESS</t>
+  </si>
+  <si>
+    <t>Resident Tax Address</t>
+  </si>
+  <si>
+    <t>MANANGE_PERSON_NAME_CORRECTION</t>
+  </si>
+  <si>
     <t>CORRECT_PERSONAL_DESCRIPTIVE_FLEXFIELD_INFORMATION</t>
   </si>
   <si>
+    <t>ADDING_EXISTING_EMPLOYEE_AS_AN_EMERGENCY_CONTACT</t>
+  </si>
+  <si>
+    <t>MODIFY_EXISTING_EMERGENCY_CONTACT</t>
+  </si>
+  <si>
+    <t>1/1/90</t>
+  </si>
+  <si>
     <t>countryOfBirth</t>
   </si>
   <si>
@@ -691,6 +802,21 @@
     <t>townOfBirth</t>
   </si>
   <si>
+    <t>correspondenceLanguage</t>
+  </si>
+  <si>
+    <t>bloodType</t>
+  </si>
+  <si>
+    <t>contactType</t>
+  </si>
+  <si>
+    <t>emergencyContact</t>
+  </si>
+  <si>
+    <t>emergencyContactType</t>
+  </si>
+  <si>
     <t>PENNSYLVANIA</t>
   </si>
   <si>
@@ -703,37 +829,16 @@
     <t>A rhesus positive</t>
   </si>
   <si>
-    <t>correspondenceLanguage</t>
-  </si>
-  <si>
-    <t>bloodType</t>
-  </si>
-  <si>
-    <t>1/1/90</t>
-  </si>
-  <si>
-    <t>ADDING_EXISTING_EMPLOYEE_AS_AN_EMERGENCY_CONTACT</t>
-  </si>
-  <si>
-    <t>contactType</t>
-  </si>
-  <si>
     <t>Emergency</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>emergencyContact</t>
-  </si>
-  <si>
-    <t>MODIFY_EXISTING_EMERGENCY_CONTACT</t>
-  </si>
-  <si>
     <t>Home Phone</t>
   </si>
   <si>
-    <t>emergencyContactType</t>
+    <t>Dallas</t>
   </si>
   <si>
     <t>Nick</t>
@@ -746,9 +851,6 @@
   </si>
   <si>
     <t>6323145</t>
-  </si>
-  <si>
-    <t>Dallas</t>
   </si>
 </sst>
 </file>
@@ -1091,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH8"/>
+  <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="AT7" workbookViewId="0">
+      <selection activeCell="BB17" sqref="BB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,7 +1383,7 @@
         <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AP1" t="s">
         <v>40</v>
@@ -1323,22 +1425,22 @@
         <v>52</v>
       </c>
       <c r="BC1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BD1" t="s">
         <v>132</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>133</v>
       </c>
-      <c r="BE1" t="s">
-        <v>134</v>
-      </c>
       <c r="BF1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BG1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
@@ -1346,7 +1448,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>53</v>
@@ -1358,7 +1460,7 @@
         <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>56</v>
@@ -1376,22 +1478,22 @@
         <v>60</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>62</v>
@@ -1400,10 +1502,10 @@
         <v>63</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>65</v>
@@ -1417,26 +1519,26 @@
         <v>67</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>69</v>
@@ -1446,31 +1548,31 @@
         <v>70</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>74</v>
@@ -1482,7 +1584,7 @@
         <v>76</v>
       </c>
       <c r="AX2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AY2" s="1" t="s">
         <v>78</v>
@@ -1494,13 +1596,13 @@
         <v>80</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
@@ -1508,7 +1610,7 @@
         <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>53</v>
@@ -1520,7 +1622,7 @@
         <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>56</v>
@@ -1538,22 +1640,22 @@
         <v>60</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>62</v>
@@ -1562,10 +1664,10 @@
         <v>63</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>65</v>
@@ -1579,26 +1681,26 @@
         <v>67</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>69</v>
@@ -1608,31 +1710,31 @@
         <v>70</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU3" s="1" t="s">
         <v>74</v>
@@ -1644,7 +1746,7 @@
         <v>76</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY3" s="1" t="s">
         <v>78</v>
@@ -1656,21 +1758,21 @@
         <v>80</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>240</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>53</v>
@@ -1682,7 +1784,7 @@
         <v>55</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>56</v>
@@ -1700,22 +1802,22 @@
         <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>62</v>
@@ -1724,10 +1826,10 @@
         <v>63</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V4" s="2" t="s">
         <v>65</v>
@@ -1741,26 +1843,26 @@
         <v>67</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI4" s="1" t="s">
         <v>69</v>
@@ -1770,31 +1872,31 @@
         <v>70</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ4" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU4" s="1" t="s">
         <v>74</v>
@@ -1806,7 +1908,7 @@
         <v>76</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY4" s="1" t="s">
         <v>78</v>
@@ -1818,21 +1920,21 @@
         <v>80</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>53</v>
@@ -1844,7 +1946,7 @@
         <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>56</v>
@@ -1862,22 +1964,22 @@
         <v>60</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>62</v>
@@ -1886,10 +1988,10 @@
         <v>63</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V5" s="2" t="s">
         <v>65</v>
@@ -1903,26 +2005,26 @@
         <v>67</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI5" s="1" t="s">
         <v>69</v>
@@ -1932,31 +2034,31 @@
         <v>70</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM5" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ5" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS5" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU5" s="1" t="s">
         <v>74</v>
@@ -1968,7 +2070,7 @@
         <v>76</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY5" s="1" t="s">
         <v>78</v>
@@ -1980,21 +2082,21 @@
         <v>80</v>
       </c>
       <c r="BB5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>53</v>
@@ -2006,7 +2108,7 @@
         <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>56</v>
@@ -2024,22 +2126,22 @@
         <v>60</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>62</v>
@@ -2048,10 +2150,10 @@
         <v>63</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>65</v>
@@ -2065,26 +2167,26 @@
         <v>67</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI6" s="1" t="s">
         <v>69</v>
@@ -2094,31 +2196,31 @@
         <v>70</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM6" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU6" s="1" t="s">
         <v>74</v>
@@ -2130,7 +2232,7 @@
         <v>76</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY6" s="1" t="s">
         <v>78</v>
@@ -2142,18 +2244,18 @@
         <v>80</v>
       </c>
       <c r="BB6" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BG6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2194,7 +2296,7 @@
       <c r="AL7" s="1"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
@@ -2205,22 +2307,22 @@
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
       <c r="AX7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
       <c r="BF7" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>53</v>
@@ -2232,7 +2334,7 @@
         <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>56</v>
@@ -2250,22 +2352,22 @@
         <v>60</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>62</v>
@@ -2274,10 +2376,10 @@
         <v>63</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>65</v>
@@ -2291,26 +2393,26 @@
         <v>67</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI8" s="1" t="s">
         <v>69</v>
@@ -2320,31 +2422,31 @@
         <v>70</v>
       </c>
       <c r="AL8" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM8" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AO8" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ8" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AR8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AS8" s="1" t="s">
         <v>73</v>
       </c>
       <c r="AT8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AU8" s="1" t="s">
         <v>74</v>
@@ -2356,7 +2458,7 @@
         <v>76</v>
       </c>
       <c r="AX8" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY8" s="1" t="s">
         <v>78</v>
@@ -2368,13 +2470,510 @@
         <v>80</v>
       </c>
       <c r="BB8" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG8" t="s">
+        <v>188</v>
+      </c>
+      <c r="BH8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="BG8" t="s">
-        <v>189</v>
-      </c>
-      <c r="BH8" t="s">
-        <v>198</v>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT9" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB9" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>188</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT10" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG10" t="s">
+        <v>188</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT11" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AU11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX11" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AY11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="BA11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB11" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG11" t="s">
+        <v>188</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX12" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2411,28 +3010,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>90</v>
-      </c>
-      <c r="I1" t="s">
-        <v>91</v>
       </c>
       <c r="J1" t="s">
         <v>39</v>
@@ -2443,31 +3042,31 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>72</v>
@@ -2478,16 +3077,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2501,14 +3100,14 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2528,92 +3127,95 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CG14"/>
+  <dimension ref="A1:CP19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="AR1" sqref="AR1"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CP19" sqref="CP19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="46" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="28.5703125" customWidth="1"/>
-    <col min="60" max="60" width="26.85546875" customWidth="1"/>
-    <col min="61" max="61" width="18.5703125" customWidth="1"/>
-    <col min="62" max="62" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8" customWidth="1"/>
-    <col min="66" max="67" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="8.140625" customWidth="1"/>
-    <col min="70" max="70" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.5703125" customWidth="1"/>
-    <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.5703125" customWidth="1"/>
+    <col min="63" max="63" width="26.85546875" customWidth="1"/>
+    <col min="64" max="64" width="18.5703125" customWidth="1"/>
+    <col min="65" max="65" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="8" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8" customWidth="1"/>
+    <col min="69" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.5703125" customWidth="1"/>
+    <col min="73" max="73" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="8" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="42.5703125" customWidth="1"/>
+    <col min="79" max="79" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:94" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2642,391 +3244,418 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BD1" t="s">
         <v>107</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BE1" t="s">
         <v>108</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BF1" t="s">
         <v>109</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BG1" t="s">
         <v>110</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BH1" t="s">
         <v>111</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BI1" t="s">
         <v>112</v>
       </c>
-      <c r="BF1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BJ1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BK1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="BH1" s="7" t="s">
+      <c r="BL1" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="BI1" s="7" t="s">
+      <c r="BM1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BN1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BO1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="BL1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="BN1" s="7" t="s">
+      <c r="BR1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="BO1" s="7" t="s">
+      <c r="BS1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="BT1" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="BU1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="BP1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="BQ1" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="BR1" s="7" t="s">
+      <c r="BV1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BW1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="BS1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="BT1" s="7" t="s">
+      <c r="BX1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="BU1" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="BV1" s="7" t="s">
+      <c r="BY1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="BW1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="BX1" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="BY1" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="BZ1" s="7" t="s">
-        <v>217</v>
+        <v>166</v>
       </c>
       <c r="CA1" s="7" t="s">
-        <v>218</v>
+        <v>163</v>
       </c>
       <c r="CB1" s="7" t="s">
-        <v>219</v>
+        <v>171</v>
       </c>
       <c r="CC1" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="CD1" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="CE1" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="CF1" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="CD1" s="7" t="s">
+      <c r="CG1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="CE1" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="CF1" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="CG1" s="7" t="s">
-        <v>234</v>
+      <c r="CH1" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="CI1" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="CJ1" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="CK1" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="CL1" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="CM1" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="CN1" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="CO1" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="CP1" s="7" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AL2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN2" s="5"/>
-      <c r="AO2">
+      <c r="N2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AO2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AQ2" s="5"/>
+      <c r="AR2">
         <v>10043</v>
       </c>
-      <c r="AP2" s="4">
+      <c r="AS2" s="4">
         <v>80000</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX2" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AU2" s="1" t="s">
-        <v>191</v>
-      </c>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AJ3" s="5"/>
-      <c r="AL3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN3" s="5"/>
-      <c r="AO3">
+      <c r="N3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AO3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AQ3" s="5"/>
+      <c r="AR3">
         <v>10043</v>
       </c>
-      <c r="AP3" s="4">
+      <c r="AS3" s="4">
         <v>80000</v>
       </c>
-      <c r="AQ3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX3" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AU3" s="1" t="s">
-        <v>191</v>
-      </c>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AJ4" s="5"/>
-      <c r="AL4" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN4" s="5"/>
-      <c r="AO4">
+      <c r="N4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AO4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AQ4" s="5"/>
+      <c r="AR4">
         <v>10043</v>
       </c>
-      <c r="AP4">
+      <c r="AS4">
         <v>15</v>
       </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AU4" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AZ4" t="s">
+      <c r="BC4" t="s">
+        <v>113</v>
+      </c>
+      <c r="BD4" t="s">
         <v>114</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BE4" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BB4" s="6" t="s">
+      <c r="BF4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BC4" s="2" t="s">
+      <c r="BG4" t="s">
         <v>117</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BH4" t="s">
         <v>118</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BI4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="BF4" s="6" t="s">
-        <v>120</v>
-      </c>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AJ5" s="5"/>
-      <c r="AL5" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN5" s="5"/>
-      <c r="AO5">
+      <c r="N5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AO5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AQ5" s="5"/>
+      <c r="AR5">
         <v>10043</v>
       </c>
-      <c r="AP5">
+      <c r="AS5">
         <v>15</v>
       </c>
-      <c r="AQ5" s="1" t="s">
+      <c r="AT5" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX5" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AU5" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AZ5" t="s">
+      <c r="BC5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BD5" t="s">
         <v>114</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BE5" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BB5" s="6" t="s">
+      <c r="BF5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BC5" s="2" t="s">
+      <c r="BG5" t="s">
         <v>117</v>
       </c>
-      <c r="BD5" t="s">
+      <c r="BH5" t="s">
         <v>118</v>
       </c>
-      <c r="BE5" t="s">
+      <c r="BI5" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="BF5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -3064,23 +3693,23 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
       <c r="AK6" s="7"/>
-      <c r="AL6" s="7" t="s">
-        <v>176</v>
-      </c>
+      <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7"/>
-      <c r="AO6" s="7"/>
+      <c r="AO6" s="7" t="s">
+        <v>175</v>
+      </c>
       <c r="AP6" s="7"/>
       <c r="AQ6" s="7"/>
       <c r="AR6" s="7"/>
       <c r="AS6" s="7"/>
       <c r="AT6" s="7"/>
-      <c r="AU6" t="s">
-        <v>191</v>
-      </c>
+      <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
       <c r="AW6" s="7"/>
-      <c r="AX6" s="7"/>
+      <c r="AX6" t="s">
+        <v>190</v>
+      </c>
       <c r="AY6" s="7"/>
       <c r="AZ6" s="7"/>
       <c r="BA6" s="7"/>
@@ -3105,10 +3734,13 @@
       <c r="BT6" s="7"/>
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
+      <c r="BW6" s="7"/>
+      <c r="BX6" s="7"/>
+      <c r="BY6" s="7"/>
     </row>
-    <row r="7" spans="1:85" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:94" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3146,23 +3778,23 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
       <c r="AK7" s="7"/>
-      <c r="AL7" s="7" t="s">
-        <v>176</v>
-      </c>
+      <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
+      <c r="AO7" s="7" t="s">
+        <v>175</v>
+      </c>
       <c r="AP7" s="7"/>
       <c r="AQ7" s="7"/>
       <c r="AR7" s="7"/>
       <c r="AS7" s="7"/>
       <c r="AT7" s="7"/>
-      <c r="AU7" t="s">
-        <v>213</v>
-      </c>
+      <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
       <c r="AW7" s="7"/>
-      <c r="AX7" s="7"/>
+      <c r="AX7" t="s">
+        <v>212</v>
+      </c>
       <c r="AY7" s="7"/>
       <c r="AZ7" s="7"/>
       <c r="BA7" s="7"/>
@@ -3171,24 +3803,24 @@
       <c r="BD7" s="7"/>
       <c r="BE7" s="7"/>
       <c r="BF7" s="7"/>
-      <c r="BG7" s="7" t="s">
+      <c r="BG7" s="7"/>
+      <c r="BH7" s="7"/>
+      <c r="BI7" s="7"/>
+      <c r="BJ7" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BK7" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BH7" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="BI7" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="BJ7" s="7" t="s">
+      <c r="BL7" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="BM7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BK7" s="7">
+      <c r="BN7" s="7">
         <v>48634</v>
       </c>
-      <c r="BL7" s="7"/>
-      <c r="BM7" s="7"/>
-      <c r="BN7" s="7"/>
       <c r="BO7" s="7"/>
       <c r="BP7" s="7"/>
       <c r="BQ7" s="7"/>
@@ -3197,10 +3829,13 @@
       <c r="BT7" s="7"/>
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
+      <c r="BW7" s="7"/>
+      <c r="BX7" s="7"/>
+      <c r="BY7" s="7"/>
     </row>
-    <row r="8" spans="1:85" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:94" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3238,23 +3873,23 @@
       <c r="AI8" s="7"/>
       <c r="AJ8" s="7"/>
       <c r="AK8" s="7"/>
-      <c r="AL8" s="7" t="s">
-        <v>176</v>
-      </c>
+      <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7"/>
-      <c r="AO8" s="7"/>
+      <c r="AO8" s="7" t="s">
+        <v>175</v>
+      </c>
       <c r="AP8" s="7"/>
       <c r="AQ8" s="7"/>
       <c r="AR8" s="7"/>
       <c r="AS8" s="7"/>
       <c r="AT8" s="7"/>
-      <c r="AU8" t="s">
-        <v>213</v>
-      </c>
+      <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
       <c r="AW8" s="7"/>
-      <c r="AX8" s="7"/>
+      <c r="AX8" t="s">
+        <v>212</v>
+      </c>
       <c r="AY8" s="7"/>
       <c r="AZ8" s="7"/>
       <c r="BA8" s="7"/>
@@ -3263,193 +3898,366 @@
       <c r="BD8" s="7"/>
       <c r="BE8" s="7"/>
       <c r="BF8" s="7"/>
-      <c r="BG8" s="7" t="s">
+      <c r="BG8" s="7"/>
+      <c r="BH8" s="7"/>
+      <c r="BI8" s="7"/>
+      <c r="BJ8" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BK8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BH8" s="7" t="s">
+      <c r="BL8" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="BM8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="BN8" s="7">
+        <v>48634</v>
+      </c>
+      <c r="BO8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="BI8" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="BJ8" s="7" t="s">
+      <c r="BP8" s="7"/>
+      <c r="BQ8" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="BR8" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="BS8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="BT8" s="7"/>
+      <c r="BU8" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="BV8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BW8" s="7">
+        <v>6323145</v>
+      </c>
+      <c r="BX8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BY8" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="BZ8" s="7"/>
+    </row>
+    <row r="9" spans="1:94" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO9" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX9" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="BZ9" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="CA9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:94" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="AO10" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX10" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="BZ10" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="T11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AO11" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>190</v>
+      </c>
+      <c r="CB11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="AO12" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>190</v>
+      </c>
+      <c r="CC12" t="s">
+        <v>216</v>
+      </c>
+      <c r="CD12" t="s">
+        <v>217</v>
+      </c>
+      <c r="CE12" t="s">
+        <v>218</v>
+      </c>
+      <c r="CF12">
+        <v>2015</v>
+      </c>
+      <c r="CG12" t="s">
+        <v>219</v>
+      </c>
+      <c r="CH12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="T13" t="s">
+        <v>168</v>
+      </c>
+      <c r="AO13" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>190</v>
+      </c>
+      <c r="CB13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" t="s">
+        <v>245</v>
+      </c>
+      <c r="G14" t="s">
+        <v>242</v>
+      </c>
+      <c r="AO14" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>190</v>
+      </c>
+      <c r="BB14" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="CC14" t="s">
+        <v>216</v>
+      </c>
+      <c r="CD14" t="s">
+        <v>217</v>
+      </c>
+      <c r="CE14" t="s">
+        <v>218</v>
+      </c>
+      <c r="CF14">
+        <v>2015</v>
+      </c>
+      <c r="CG14" t="s">
+        <v>219</v>
+      </c>
+      <c r="CH14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" t="s">
+        <v>244</v>
+      </c>
+      <c r="C15" t="s">
+        <v>245</v>
+      </c>
+      <c r="G15" t="s">
+        <v>242</v>
+      </c>
+      <c r="AO15" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>190</v>
+      </c>
+      <c r="BB15" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="CC15" t="s">
+        <v>216</v>
+      </c>
+      <c r="CD15" t="s">
+        <v>217</v>
+      </c>
+      <c r="CE15" t="s">
+        <v>218</v>
+      </c>
+      <c r="CF15">
+        <v>2015</v>
+      </c>
+      <c r="CG15" t="s">
+        <v>219</v>
+      </c>
+      <c r="CH15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B16" t="s">
+        <v>244</v>
+      </c>
+      <c r="C16" t="s">
+        <v>245</v>
+      </c>
+      <c r="G16" t="s">
+        <v>242</v>
+      </c>
+      <c r="AO16" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>190</v>
+      </c>
+      <c r="BB16" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="BL16" t="s">
+        <v>248</v>
+      </c>
+      <c r="CC16" t="s">
+        <v>216</v>
+      </c>
+      <c r="CD16" t="s">
+        <v>217</v>
+      </c>
+      <c r="CE16" t="s">
+        <v>218</v>
+      </c>
+      <c r="CF16">
+        <v>2015</v>
+      </c>
+      <c r="CG16" t="s">
+        <v>219</v>
+      </c>
+      <c r="CH16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AO17" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>190</v>
+      </c>
+      <c r="CI17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BK8" s="7">
-        <v>48634</v>
-      </c>
-      <c r="BL8" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="BM8" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="BN8" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="BO8" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="BP8" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="BQ8" s="7"/>
-      <c r="BR8" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="BS8" s="7" t="s">
+      <c r="CJ17" t="s">
+        <v>262</v>
+      </c>
+      <c r="CK17" t="s">
+        <v>263</v>
+      </c>
+      <c r="CL17" t="s">
+        <v>264</v>
+      </c>
+      <c r="CM17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AO18" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>190</v>
+      </c>
+      <c r="CN18" t="s">
+        <v>266</v>
+      </c>
+      <c r="CO18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AO19" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>74</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>190</v>
+      </c>
+      <c r="BB19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="BJ19" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BK19" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BO19" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="BP19" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="BT19" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="BV19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BT8" s="7">
-        <v>6323145</v>
-      </c>
-      <c r="BU8" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="BV8" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="BW8" s="7"/>
-    </row>
-    <row r="9" spans="1:85" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="AL9" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AU9" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="BW9" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:85" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="AL10" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AU10" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="BW10" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="R11" t="s">
-        <v>169</v>
-      </c>
-      <c r="AL11" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>191</v>
-      </c>
-      <c r="BY11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:85" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="AL12" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>191</v>
-      </c>
-      <c r="BZ12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="CA12" t="s">
-        <v>220</v>
-      </c>
-      <c r="CB12" t="s">
-        <v>221</v>
-      </c>
-      <c r="CC12" t="s">
-        <v>222</v>
-      </c>
-      <c r="CD12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="13" spans="1:85" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="AL13" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>191</v>
-      </c>
-      <c r="CE13" t="s">
-        <v>229</v>
-      </c>
-      <c r="CF13" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:85" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="AL14" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="AR14" t="s">
-        <v>74</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>191</v>
-      </c>
-      <c r="AY14" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="BG14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="BH14" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="BL14" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="BM14" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="BQ14" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="BS14" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="BT14" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="CG14" t="s">
-        <v>233</v>
+      <c r="BW19" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="CP19" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3491,45 +4299,45 @@
         <v>39</v>
       </c>
       <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
         <v>122</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>123</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
       </c>
       <c r="G1" t="s">
         <v>43</v>
       </c>
       <c r="H1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" t="s">
         <v>205</v>
       </c>
-      <c r="I1" t="s">
-        <v>206</v>
-      </c>
       <c r="J1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
         <v>129</v>
-      </c>
-      <c r="F2" t="s">
-        <v>130</v>
       </c>
       <c r="G2" s="4">
         <v>80572.460000000006</v>
@@ -3537,56 +4345,56 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" t="s">
         <v>200</v>
       </c>
-      <c r="B5" t="s">
-        <v>201</v>
-      </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" t="s">
         <v>129</v>
-      </c>
-      <c r="F5" t="s">
-        <v>130</v>
       </c>
       <c r="G5" s="4">
         <v>80572.460000000006</v>
       </c>
       <c r="H5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I5" t="s">
         <v>202</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>203</v>
-      </c>
-      <c r="J5" t="s">
-        <v>204</v>
       </c>
       <c r="L5" s="4"/>
     </row>
@@ -3597,30 +4405,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -3853,25 +4637,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3888,4 +4678,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feature file for Quick Convert,Reverse Termination & Convert Contingent worker
Signed-off-by: Venkatesan Manivannan <venkatesan.manivannan@cognizant.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4972878F-86DA-46BD-8210-E8949DB43003}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -12,9 +13,9 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="252">
   <si>
     <t>scenario</t>
   </si>
@@ -772,13 +773,19 @@
   </si>
   <si>
     <t>MANANGE_PERSON_NAME_CORRECTION</t>
+  </si>
+  <si>
+    <t>CONVERT_PENDING_WORKER_TO_EMPLOYEE</t>
+  </si>
+  <si>
+    <t>QUICK_CONVERT_PENDING_WORKER_TO_EMPLOYEE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1103,21 +1110,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BH12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BH14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="AX12" sqref="AX12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AX13" sqref="AX13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1179,7 +1186,7 @@
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1368,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="30">
+    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1523,7 +1530,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:60" ht="30">
+    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1685,7 +1692,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:60" ht="30">
+    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -1847,7 +1854,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="45">
+    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -2009,7 +2016,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:60" ht="30">
+    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2171,7 +2178,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="30">
+    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>143</v>
       </c>
@@ -2235,7 +2242,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="30">
+    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2397,7 +2404,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:60" ht="30">
+    <row r="9" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -2559,7 +2566,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:60" ht="30">
+    <row r="10" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2721,7 +2728,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="30">
+    <row r="11" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>234</v>
       </c>
@@ -2883,7 +2890,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -2891,6 +2898,28 @@
         <v>175</v>
       </c>
       <c r="AX12" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AN13" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX13" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AN14" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX14" s="1" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2901,14 +2930,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -2923,7 +2952,7 @@
     <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2958,7 +2987,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -2993,7 +3022,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -3016,7 +3045,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3044,7 +3073,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CE16"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -3052,7 +3081,7 @@
       <selection pane="bottomLeft" activeCell="BK16" sqref="BK16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3130,7 +3159,7 @@
     <col min="76" max="76" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="60">
+    <row r="1" spans="1:83" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3381,7 +3410,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:83">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -3409,7 +3438,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:83">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -3437,7 +3466,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:83">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -3486,7 +3515,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:83">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -3535,7 +3564,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:83">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>120</v>
       </c>
@@ -3617,7 +3646,7 @@
       <c r="BU6" s="7"/>
       <c r="BV6" s="7"/>
     </row>
-    <row r="7" spans="1:83" ht="30">
+    <row r="7" spans="1:83" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>210</v>
       </c>
@@ -3709,7 +3738,7 @@
       <c r="BU7" s="7"/>
       <c r="BV7" s="7"/>
     </row>
-    <row r="8" spans="1:83" ht="75">
+    <row r="8" spans="1:83" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>209</v>
       </c>
@@ -3820,7 +3849,7 @@
       </c>
       <c r="BW8" s="7"/>
     </row>
-    <row r="9" spans="1:83" ht="45">
+    <row r="9" spans="1:83" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>206</v>
       </c>
@@ -3837,7 +3866,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:83" ht="45">
+    <row r="10" spans="1:83" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>208</v>
       </c>
@@ -3851,7 +3880,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:83">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>167</v>
       </c>
@@ -3868,7 +3897,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:83">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>215</v>
       </c>
@@ -3897,7 +3926,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:83">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>239</v>
       </c>
@@ -3914,7 +3943,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:83">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>241</v>
       </c>
@@ -3955,7 +3984,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:83">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>246</v>
       </c>
@@ -3996,7 +4025,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:83">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>247</v>
       </c>
@@ -4047,14 +4076,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -4068,7 +4097,7 @@
     <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4100,7 +4129,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4123,7 +4152,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4134,7 +4163,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -4145,7 +4174,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -4185,30 +4214,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4441,25 +4446,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4476,4 +4487,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Termination from quick action page completed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5128D899-7047-4ED5-8522-816DC9CF1CD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A274D9-8248-4388-8D89-655BB855AFDC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,23 +13,17 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="282">
   <si>
     <t>scenario</t>
   </si>
@@ -851,6 +845,30 @@
   </si>
   <si>
     <t>6323145</t>
+  </si>
+  <si>
+    <t>QUICK_ACTION_TERMINATION</t>
+  </si>
+  <si>
+    <t>terminationAction</t>
+  </si>
+  <si>
+    <t>terminationReason</t>
+  </si>
+  <si>
+    <t>Termination</t>
+  </si>
+  <si>
+    <t>Work Incident or Work Related Illness</t>
+  </si>
+  <si>
+    <t>revokeUserAccess</t>
+  </si>
+  <si>
+    <t>recommendedForRehire</t>
+  </si>
+  <si>
+    <t>Immediately</t>
   </si>
 </sst>
 </file>
@@ -1195,73 +1213,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH12"/>
   <sheetViews>
-    <sheetView topLeftCell="AT7" workbookViewId="0">
-      <selection activeCell="BB17" sqref="BB17"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1443,7 +1461,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1605,7 +1623,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1767,7 +1785,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -1929,7 +1947,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -2091,7 +2109,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2253,7 +2271,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>143</v>
       </c>
@@ -2317,7 +2335,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2479,7 +2497,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -2641,7 +2659,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2803,7 +2821,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>234</v>
       </c>
@@ -2965,7 +2983,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -2990,22 +3008,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.26171875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3040,7 +3058,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -3075,7 +3093,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -3098,7 +3116,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3129,93 +3147,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CP19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CP19" sqref="CP19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="28.5703125" customWidth="1"/>
-    <col min="63" max="63" width="26.85546875" customWidth="1"/>
-    <col min="64" max="64" width="18.5703125" customWidth="1"/>
-    <col min="65" max="65" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="28.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.578125" customWidth="1"/>
+    <col min="63" max="63" width="26.83984375" customWidth="1"/>
+    <col min="64" max="64" width="18.578125" customWidth="1"/>
+    <col min="65" max="65" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="8" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="8" customWidth="1"/>
-    <col min="69" max="70" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="6.5703125" customWidth="1"/>
-    <col min="73" max="73" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="6.578125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.578125" customWidth="1"/>
+    <col min="73" max="73" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.41796875" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="8" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="42.5703125" customWidth="1"/>
+    <col min="78" max="78" width="42.578125" customWidth="1"/>
     <col min="79" max="79" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:94" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3499,7 +3517,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -3527,7 +3545,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -3555,7 +3573,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -3604,7 +3622,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -3653,7 +3671,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>120</v>
       </c>
@@ -3738,7 +3756,7 @@
       <c r="BX6" s="7"/>
       <c r="BY6" s="7"/>
     </row>
-    <row r="7" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:94" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>210</v>
       </c>
@@ -3833,7 +3851,7 @@
       <c r="BX7" s="7"/>
       <c r="BY7" s="7"/>
     </row>
-    <row r="8" spans="1:94" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:94" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>209</v>
       </c>
@@ -3947,7 +3965,7 @@
       </c>
       <c r="BZ8" s="7"/>
     </row>
-    <row r="9" spans="1:94" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:94" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
         <v>206</v>
       </c>
@@ -3964,7 +3982,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:94" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:94" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
         <v>208</v>
       </c>
@@ -3978,7 +3996,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>167</v>
       </c>
@@ -3995,7 +4013,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7" t="s">
         <v>215</v>
       </c>
@@ -4024,7 +4042,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
         <v>239</v>
       </c>
@@ -4041,7 +4059,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
         <v>241</v>
       </c>
@@ -4082,7 +4100,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
         <v>246</v>
       </c>
@@ -4123,7 +4141,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7" t="s">
         <v>247</v>
       </c>
@@ -4167,7 +4185,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7" t="s">
         <v>250</v>
       </c>
@@ -4196,7 +4214,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:94" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7" t="s">
         <v>251</v>
       </c>
@@ -4213,7 +4231,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="19" spans="1:94" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:94" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="7" t="s">
         <v>252</v>
       </c>
@@ -4268,27 +4286,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.41796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.15625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1015625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5234375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.89453125" customWidth="1"/>
+    <col min="14" max="14" width="20.05078125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4319,8 +4341,20 @@
       <c r="J1" t="s">
         <v>187</v>
       </c>
+      <c r="K1" t="s">
+        <v>275</v>
+      </c>
+      <c r="L1" t="s">
+        <v>276</v>
+      </c>
+      <c r="M1" t="s">
+        <v>279</v>
+      </c>
+      <c r="N1" t="s">
+        <v>280</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4343,7 +4377,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4354,7 +4388,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -4365,7 +4399,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -4397,6 +4431,29 @@
         <v>203</v>
       </c>
       <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>175</v>
+      </c>
+      <c r="K6" t="s">
+        <v>277</v>
+      </c>
+      <c r="L6" t="s">
+        <v>278</v>
+      </c>
+      <c r="M6" t="s">
+        <v>281</v>
+      </c>
+      <c r="N6" t="s">
+        <v>267</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4405,6 +4462,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4637,31 +4718,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4678,22 +4753,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Scripting of test case "Manage Person - Add Extra Information (EIT) " completed
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A274D9-8248-4388-8D89-655BB855AFDC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68137559-9C92-4F3D-A59F-D966AF511CBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,17 +13,23 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="296">
   <si>
     <t>scenario</t>
   </si>
@@ -869,6 +875,48 @@
   </si>
   <si>
     <t>Immediately</t>
+  </si>
+  <si>
+    <t>ADD_EXTRA_INFORMATION_EIT</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>casteTribe</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>exServicePerson</t>
+  </si>
+  <si>
+    <t>residentialStatus</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>Nonresident Indian</t>
+  </si>
+  <si>
+    <t>panNumber</t>
+  </si>
+  <si>
+    <t>bnhoc3327h</t>
+  </si>
+  <si>
+    <t>Forward</t>
   </si>
 </sst>
 </file>
@@ -1217,69 +1265,69 @@
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1509,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1623,7 +1671,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1785,7 +1833,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -1947,7 +1995,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -2109,7 +2157,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2271,7 +2319,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>143</v>
       </c>
@@ -2335,7 +2383,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2497,7 +2545,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -2659,7 +2707,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2821,7 +2869,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>234</v>
       </c>
@@ -2983,7 +3031,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -3008,22 +3056,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3058,7 +3106,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -3093,7 +3141,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -3116,7 +3164,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3145,95 +3193,95 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CP19"/>
+  <dimension ref="A1:CW20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CQ20" sqref="CQ20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="22.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="20.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="5.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="18.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="11.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="33.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="6.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="28.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="25.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="10.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="14.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="17.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="13.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="28.578125" customWidth="1"/>
-    <col min="63" max="63" width="26.83984375" customWidth="1"/>
-    <col min="64" max="64" width="18.578125" customWidth="1"/>
-    <col min="65" max="65" width="8.26171875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.5703125" customWidth="1"/>
+    <col min="63" max="63" width="26.85546875" customWidth="1"/>
+    <col min="64" max="64" width="18.5703125" customWidth="1"/>
+    <col min="65" max="65" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="8" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="8" customWidth="1"/>
-    <col min="69" max="70" width="8.15625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="6.578125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="6.578125" customWidth="1"/>
-    <col min="73" max="73" width="8.15625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8.26171875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.578125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.5703125" customWidth="1"/>
+    <col min="73" max="73" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="8" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="42.578125" customWidth="1"/>
+    <col min="78" max="78" width="42.5703125" customWidth="1"/>
     <col min="79" max="79" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:101" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3516,8 +3564,29 @@
       <c r="CP1" s="7" t="s">
         <v>261</v>
       </c>
+      <c r="CQ1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="CR1" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="CS1" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="CT1" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="CU1" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="CV1" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="CW1" s="7" t="s">
+        <v>293</v>
+      </c>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -3545,7 +3614,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -3573,7 +3642,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -3622,7 +3691,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -3671,7 +3740,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>120</v>
       </c>
@@ -3756,7 +3825,7 @@
       <c r="BX6" s="7"/>
       <c r="BY6" s="7"/>
     </row>
-    <row r="7" spans="1:94" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:101" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>210</v>
       </c>
@@ -3851,7 +3920,7 @@
       <c r="BX7" s="7"/>
       <c r="BY7" s="7"/>
     </row>
-    <row r="8" spans="1:94" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:101" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>209</v>
       </c>
@@ -3965,7 +4034,7 @@
       </c>
       <c r="BZ8" s="7"/>
     </row>
-    <row r="9" spans="1:94" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>206</v>
       </c>
@@ -3982,7 +4051,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:94" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>208</v>
       </c>
@@ -3996,7 +4065,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>167</v>
       </c>
@@ -4013,7 +4082,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>215</v>
       </c>
@@ -4042,7 +4111,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>239</v>
       </c>
@@ -4059,7 +4128,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>241</v>
       </c>
@@ -4100,7 +4169,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>246</v>
       </c>
@@ -4141,7 +4210,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>247</v>
       </c>
@@ -4185,7 +4254,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:101" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>250</v>
       </c>
@@ -4214,7 +4283,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:101" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>251</v>
       </c>
@@ -4231,7 +4300,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="19" spans="1:94" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:101" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>252</v>
       </c>
@@ -4276,6 +4345,38 @@
       </c>
       <c r="CP19" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="AO20" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX20" t="s">
+        <v>190</v>
+      </c>
+      <c r="CQ20" t="s">
+        <v>295</v>
+      </c>
+      <c r="CR20" t="s">
+        <v>285</v>
+      </c>
+      <c r="CS20" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="CT20" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="CU20" t="s">
+        <v>267</v>
+      </c>
+      <c r="CV20" t="s">
+        <v>292</v>
+      </c>
+      <c r="CW20" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -4288,29 +4389,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.15625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1015625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.89453125" customWidth="1"/>
-    <col min="14" max="14" width="20.05078125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4354,7 +4453,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4377,7 +4476,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4388,7 +4487,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -4399,7 +4498,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -4432,7 +4531,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>274</v>
       </c>
@@ -4471,21 +4570,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4718,6 +4802,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
   <ds:schemaRefs>
@@ -4727,16 +4826,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4753,4 +4842,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Scripting completed for tcs "Manage Person - Modify Extra Information (EIT) "
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68137559-9C92-4F3D-A59F-D966AF511CBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DD8FF6-558B-4A91-99DE-CD82E2E04A5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="302">
   <si>
     <t>scenario</t>
   </si>
@@ -917,6 +917,24 @@
   </si>
   <si>
     <t>Forward</t>
+  </si>
+  <si>
+    <t>MODIFY_EXTRA_INFORMATION_EIT</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>Resident and ordinarily resident in India</t>
+  </si>
+  <si>
+    <t>bnhoc1122h</t>
   </si>
 </sst>
 </file>
@@ -3193,11 +3211,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CW20"/>
+  <dimension ref="A1:CW21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CC1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CQ20" sqref="CQ20"/>
+      <selection pane="bottomLeft" activeCell="CQ21" sqref="CQ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4379,6 +4397,38 @@
         <v>294</v>
       </c>
     </row>
+    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="AO21" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>190</v>
+      </c>
+      <c r="CQ21" t="s">
+        <v>297</v>
+      </c>
+      <c r="CR21" t="s">
+        <v>285</v>
+      </c>
+      <c r="CS21" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="CT21" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="CU21" t="s">
+        <v>80</v>
+      </c>
+      <c r="CV21" t="s">
+        <v>300</v>
+      </c>
+      <c r="CW21" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4561,15 +4611,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4802,6 +4843,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4818,14 +4868,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4844,6 +4886,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Removed duplicate column county from employee details sheets
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DD8FF6-558B-4A91-99DE-CD82E2E04A5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195122F1-7AE4-4CF9-AA49-7D8C78083597}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -13,23 +13,17 @@
     <sheet name="Employee_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Line_Manager" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="302">
   <si>
     <t>scenario</t>
   </si>
@@ -1283,69 +1277,69 @@
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +1521,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1689,7 +1683,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1851,7 +1845,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -2013,7 +2007,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -2175,7 +2169,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2337,7 +2331,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>143</v>
       </c>
@@ -2401,7 +2395,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2563,7 +2557,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -2725,7 +2719,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2887,7 +2881,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>234</v>
       </c>
@@ -3049,7 +3043,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -3074,22 +3068,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3124,7 +3118,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -3159,7 +3153,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -3182,7 +3176,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3211,95 +3205,94 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CW21"/>
+  <dimension ref="A1:CV21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CC1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CQ21" sqref="CQ21"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="28.5703125" customWidth="1"/>
-    <col min="63" max="63" width="26.85546875" customWidth="1"/>
-    <col min="64" max="64" width="18.5703125" customWidth="1"/>
-    <col min="65" max="65" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8" customWidth="1"/>
-    <col min="69" max="70" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="6.5703125" customWidth="1"/>
-    <col min="73" max="73" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="8" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="42.5703125" customWidth="1"/>
-    <col min="79" max="79" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="28.5546875" customWidth="1"/>
+    <col min="62" max="62" width="26.88671875" customWidth="1"/>
+    <col min="63" max="63" width="18.5546875" customWidth="1"/>
+    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="8" customWidth="1"/>
+    <col min="68" max="69" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="6.5546875" customWidth="1"/>
+    <col min="72" max="72" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="42.5546875" customWidth="1"/>
+    <col min="78" max="78" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:100" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3337,428 +3330,425 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BI1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BR1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="BS1" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="BT1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="BU1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BV1" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="BW1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="BX1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BJ1" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="BK1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="BL1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="BM1" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="BN1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="BO1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="BQ1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="BR1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="BS1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="BT1" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="BU1" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="BV1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="BW1" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="BX1" s="7" t="s">
-        <v>161</v>
-      </c>
       <c r="BY1" s="7" t="s">
-        <v>17</v>
+        <v>166</v>
       </c>
       <c r="BZ1" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="CA1" s="7" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="CB1" s="7" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="CC1" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="CD1" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="CE1" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="CF1" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="CG1" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="CH1" s="7" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
       <c r="CI1" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="CJ1" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="CK1" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="CL1" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="CM1" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="CN1" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="CO1" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="CP1" s="7" t="s">
-        <v>261</v>
+        <v>283</v>
       </c>
       <c r="CQ1" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CR1" s="7" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="CS1" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CT1" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="CU1" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="CV1" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="CW1" s="7" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>102</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AO2" s="1" t="s">
+      <c r="M2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AN2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AQ2" s="5"/>
-      <c r="AR2">
+      <c r="AP2" s="5"/>
+      <c r="AQ2">
         <v>10043</v>
       </c>
-      <c r="AS2" s="4">
+      <c r="AR2" s="4">
         <v>80000</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AM3" s="5"/>
-      <c r="AO3" s="1" t="s">
+      <c r="M3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AN3" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AQ3" s="5"/>
-      <c r="AR3">
+      <c r="AP3" s="5"/>
+      <c r="AQ3">
         <v>10043</v>
       </c>
-      <c r="AS3" s="4">
+      <c r="AR3" s="4">
         <v>80000</v>
       </c>
-      <c r="AT3" s="1" t="s">
+      <c r="AS3" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="AW3" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>104</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AM4" s="5"/>
-      <c r="AO4" s="1" t="s">
+      <c r="M4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AN4" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AQ4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4">
+        <v>10043</v>
+      </c>
       <c r="AR4">
-        <v>10043</v>
-      </c>
-      <c r="AS4">
         <v>15</v>
       </c>
-      <c r="AT4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AX4" s="1" t="s">
+      <c r="AW4" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="BB4" t="s">
+        <v>113</v>
+      </c>
       <c r="BC4" t="s">
-        <v>113</v>
-      </c>
-      <c r="BD4" t="s">
         <v>114</v>
       </c>
-      <c r="BE4" s="6" t="s">
+      <c r="BD4" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BF4" s="2" t="s">
+      <c r="BE4" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="BF4" t="s">
+        <v>117</v>
+      </c>
       <c r="BG4" t="s">
-        <v>117</v>
-      </c>
-      <c r="BH4" t="s">
         <v>118</v>
       </c>
-      <c r="BI4" s="6" t="s">
+      <c r="BH4" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>105</v>
       </c>
       <c r="D5" s="4">
         <v>1000</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AM5" s="5"/>
-      <c r="AO5" s="1" t="s">
+      <c r="M5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AN5" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AQ5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5">
+        <v>10043</v>
+      </c>
       <c r="AR5">
-        <v>10043</v>
-      </c>
-      <c r="AS5">
         <v>15</v>
       </c>
-      <c r="AT5" s="1" t="s">
+      <c r="AS5" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AX5" s="1" t="s">
+      <c r="AW5" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="BB5" t="s">
+        <v>113</v>
+      </c>
       <c r="BC5" t="s">
-        <v>113</v>
-      </c>
-      <c r="BD5" t="s">
         <v>114</v>
       </c>
-      <c r="BE5" s="6" t="s">
+      <c r="BD5" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="BF5" s="2" t="s">
+      <c r="BE5" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="BF5" t="s">
+        <v>117</v>
+      </c>
       <c r="BG5" t="s">
-        <v>117</v>
-      </c>
-      <c r="BH5" t="s">
         <v>118</v>
       </c>
-      <c r="BI5" s="6" t="s">
+      <c r="BH5" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>120</v>
       </c>
@@ -3800,10 +3790,10 @@
       <c r="AK6" s="7"/>
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
-      <c r="AN6" s="7"/>
-      <c r="AO6" s="7" t="s">
+      <c r="AN6" s="7" t="s">
         <v>175</v>
       </c>
+      <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
       <c r="AQ6" s="7"/>
       <c r="AR6" s="7"/>
@@ -3811,10 +3801,10 @@
       <c r="AT6" s="7"/>
       <c r="AU6" s="7"/>
       <c r="AV6" s="7"/>
-      <c r="AW6" s="7"/>
-      <c r="AX6" t="s">
+      <c r="AW6" t="s">
         <v>190</v>
       </c>
+      <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
       <c r="AZ6" s="7"/>
       <c r="BA6" s="7"/>
@@ -3841,9 +3831,8 @@
       <c r="BV6" s="7"/>
       <c r="BW6" s="7"/>
       <c r="BX6" s="7"/>
-      <c r="BY6" s="7"/>
     </row>
-    <row r="7" spans="1:101" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:100" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>210</v>
       </c>
@@ -3885,10 +3874,10 @@
       <c r="AK7" s="7"/>
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
-      <c r="AN7" s="7"/>
-      <c r="AO7" s="7" t="s">
+      <c r="AN7" s="7" t="s">
         <v>175</v>
       </c>
+      <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
       <c r="AQ7" s="7"/>
       <c r="AR7" s="7"/>
@@ -3896,10 +3885,10 @@
       <c r="AT7" s="7"/>
       <c r="AU7" s="7"/>
       <c r="AV7" s="7"/>
-      <c r="AW7" s="7"/>
-      <c r="AX7" t="s">
+      <c r="AW7" t="s">
         <v>212</v>
       </c>
+      <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
       <c r="AZ7" s="7"/>
       <c r="BA7" s="7"/>
@@ -3910,22 +3899,22 @@
       <c r="BF7" s="7"/>
       <c r="BG7" s="7"/>
       <c r="BH7" s="7"/>
-      <c r="BI7" s="7"/>
+      <c r="BI7" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="BJ7" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BK7" s="7" t="s">
-        <v>145</v>
+        <v>211</v>
       </c>
       <c r="BL7" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="BM7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BN7" s="7">
+      <c r="BM7" s="7">
         <v>48634</v>
       </c>
+      <c r="BN7" s="7"/>
       <c r="BO7" s="7"/>
       <c r="BP7" s="7"/>
       <c r="BQ7" s="7"/>
@@ -3936,9 +3925,8 @@
       <c r="BV7" s="7"/>
       <c r="BW7" s="7"/>
       <c r="BX7" s="7"/>
-      <c r="BY7" s="7"/>
     </row>
-    <row r="8" spans="1:101" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:100" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>209</v>
       </c>
@@ -3980,10 +3968,10 @@
       <c r="AK8" s="7"/>
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
-      <c r="AN8" s="7"/>
-      <c r="AO8" s="7" t="s">
+      <c r="AN8" s="7" t="s">
         <v>175</v>
       </c>
+      <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
       <c r="AQ8" s="7"/>
       <c r="AR8" s="7"/>
@@ -3991,10 +3979,10 @@
       <c r="AT8" s="7"/>
       <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
-      <c r="AW8" s="7"/>
-      <c r="AX8" t="s">
+      <c r="AW8" t="s">
         <v>212</v>
       </c>
+      <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
       <c r="AZ8" s="7"/>
       <c r="BA8" s="7"/>
@@ -4005,148 +3993,147 @@
       <c r="BF8" s="7"/>
       <c r="BG8" s="7"/>
       <c r="BH8" s="7"/>
-      <c r="BI8" s="7"/>
+      <c r="BI8" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="BJ8" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BK8" s="7" t="s">
-        <v>145</v>
+        <v>211</v>
       </c>
       <c r="BL8" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="BM8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BN8" s="7">
+      <c r="BM8" s="7">
         <v>48634</v>
       </c>
-      <c r="BO8" s="7" t="s">
+      <c r="BN8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="BP8" s="7"/>
+      <c r="BO8" s="7"/>
+      <c r="BP8" s="7" t="s">
+        <v>147</v>
+      </c>
       <c r="BQ8" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="BR8" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="BS8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="BT8" s="7"/>
+      <c r="BS8" s="7"/>
+      <c r="BT8" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="BU8" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="BV8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BW8" s="7">
+      <c r="BV8" s="7">
         <v>6323145</v>
       </c>
+      <c r="BW8" s="7" t="s">
+        <v>150</v>
+      </c>
       <c r="BX8" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="BY8" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="BZ8" s="7"/>
+      <c r="BY8" s="7"/>
     </row>
-    <row r="9" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:100" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="AO9" s="7" t="s">
+      <c r="AN9" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX9" s="7" t="s">
+      <c r="AW9" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="BZ9" s="7" t="s">
+      <c r="BY9" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="CA9" t="s">
+      <c r="BZ9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:100" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="AO10" s="7" t="s">
+      <c r="AN10" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX10" s="7" t="s">
+      <c r="AW10" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="BZ10" s="8" t="s">
+      <c r="BY10" s="8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="T11" t="s">
+      <c r="S11" t="s">
         <v>168</v>
       </c>
-      <c r="AO11" s="7" t="s">
+      <c r="AN11" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX11" t="s">
+      <c r="AW11" t="s">
         <v>190</v>
       </c>
-      <c r="CB11" t="s">
+      <c r="CA11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="AO12" s="7" t="s">
+      <c r="AN12" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX12" t="s">
+      <c r="AW12" t="s">
         <v>190</v>
       </c>
+      <c r="CB12" t="s">
+        <v>216</v>
+      </c>
       <c r="CC12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="CD12" t="s">
-        <v>217</v>
-      </c>
-      <c r="CE12" t="s">
         <v>218</v>
       </c>
-      <c r="CF12">
+      <c r="CE12">
         <v>2015</v>
       </c>
+      <c r="CF12" t="s">
+        <v>219</v>
+      </c>
       <c r="CG12" t="s">
-        <v>219</v>
-      </c>
-      <c r="CH12" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="T13" t="s">
+      <c r="S13" t="s">
         <v>168</v>
       </c>
-      <c r="AO13" s="7" t="s">
+      <c r="AN13" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX13" t="s">
+      <c r="AW13" t="s">
         <v>190</v>
       </c>
-      <c r="CB13" t="s">
+      <c r="CA13" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>241</v>
       </c>
@@ -4159,35 +4146,35 @@
       <c r="G14" t="s">
         <v>242</v>
       </c>
-      <c r="AO14" s="7" t="s">
+      <c r="AN14" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX14" t="s">
+      <c r="AW14" t="s">
         <v>190</v>
       </c>
-      <c r="BB14" s="6" t="s">
+      <c r="BA14" s="6" t="s">
         <v>243</v>
       </c>
+      <c r="CB14" t="s">
+        <v>216</v>
+      </c>
       <c r="CC14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="CD14" t="s">
-        <v>217</v>
-      </c>
-      <c r="CE14" t="s">
         <v>218</v>
       </c>
-      <c r="CF14">
+      <c r="CE14">
         <v>2015</v>
       </c>
+      <c r="CF14" t="s">
+        <v>219</v>
+      </c>
       <c r="CG14" t="s">
-        <v>219</v>
-      </c>
-      <c r="CH14" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>246</v>
       </c>
@@ -4200,35 +4187,35 @@
       <c r="G15" t="s">
         <v>242</v>
       </c>
-      <c r="AO15" s="7" t="s">
+      <c r="AN15" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX15" t="s">
+      <c r="AW15" t="s">
         <v>190</v>
       </c>
-      <c r="BB15" s="6" t="s">
+      <c r="BA15" s="6" t="s">
         <v>243</v>
       </c>
+      <c r="CB15" t="s">
+        <v>216</v>
+      </c>
       <c r="CC15" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="CD15" t="s">
-        <v>217</v>
-      </c>
-      <c r="CE15" t="s">
         <v>218</v>
       </c>
-      <c r="CF15">
+      <c r="CE15">
         <v>2015</v>
       </c>
+      <c r="CF15" t="s">
+        <v>219</v>
+      </c>
       <c r="CG15" t="s">
-        <v>219</v>
-      </c>
-      <c r="CH15" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>247</v>
       </c>
@@ -4241,84 +4228,84 @@
       <c r="G16" t="s">
         <v>242</v>
       </c>
-      <c r="AO16" s="7" t="s">
+      <c r="AN16" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX16" t="s">
+      <c r="AW16" t="s">
         <v>190</v>
       </c>
-      <c r="BB16" s="6" t="s">
+      <c r="BA16" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="BL16" t="s">
+      <c r="BK16" t="s">
         <v>248</v>
       </c>
+      <c r="CB16" t="s">
+        <v>216</v>
+      </c>
       <c r="CC16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="CD16" t="s">
-        <v>217</v>
-      </c>
-      <c r="CE16" t="s">
         <v>218</v>
       </c>
-      <c r="CF16">
+      <c r="CE16">
         <v>2015</v>
       </c>
+      <c r="CF16" t="s">
+        <v>219</v>
+      </c>
       <c r="CG16" t="s">
-        <v>219</v>
-      </c>
-      <c r="CH16" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:101" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:100" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AO17" s="7" t="s">
+      <c r="AN17" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX17" t="s">
+      <c r="AW17" t="s">
         <v>190</v>
       </c>
-      <c r="CI17" s="1" t="s">
+      <c r="CH17" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="CI17" t="s">
+        <v>262</v>
+      </c>
       <c r="CJ17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="CK17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="CL17" t="s">
-        <v>264</v>
-      </c>
-      <c r="CM17" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:101" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:100" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="AO18" s="7" t="s">
+      <c r="AN18" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX18" t="s">
+      <c r="AW18" t="s">
         <v>190</v>
       </c>
+      <c r="CM18" t="s">
+        <v>266</v>
+      </c>
       <c r="CN18" t="s">
-        <v>266</v>
-      </c>
-      <c r="CO18" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="19" spans="1:101" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:100" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>252</v>
       </c>
@@ -4328,104 +4315,104 @@
       <c r="J19" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AO19" s="7" t="s">
+      <c r="AN19" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AU19" t="s">
+      <c r="AT19" t="s">
         <v>74</v>
       </c>
-      <c r="AX19" t="s">
+      <c r="AW19" t="s">
         <v>190</v>
       </c>
-      <c r="BB19" s="1" t="s">
+      <c r="BA19" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="BI19" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="BJ19" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="BK19" s="7" t="s">
         <v>145</v>
       </c>
+      <c r="BN19" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="BO19" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="BP19" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="BT19" s="6" t="s">
+      <c r="BS19" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="BV19" s="7" t="s">
+      <c r="BU19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BW19" s="11" t="s">
+      <c r="BV19" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="CP19" t="s">
+      <c r="CO19" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="AO20" s="7" t="s">
+      <c r="AN20" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX20" t="s">
+      <c r="AW20" t="s">
         <v>190</v>
       </c>
+      <c r="CP20" t="s">
+        <v>295</v>
+      </c>
       <c r="CQ20" t="s">
-        <v>295</v>
-      </c>
-      <c r="CR20" t="s">
         <v>285</v>
       </c>
+      <c r="CR20" s="6" t="s">
+        <v>290</v>
+      </c>
       <c r="CS20" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="CT20" s="6" t="s">
         <v>291</v>
       </c>
+      <c r="CT20" t="s">
+        <v>267</v>
+      </c>
       <c r="CU20" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
       <c r="CV20" t="s">
-        <v>292</v>
-      </c>
-      <c r="CW20" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="AO21" s="7" t="s">
+      <c r="AN21" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AX21" t="s">
+      <c r="AW21" t="s">
         <v>190</v>
       </c>
+      <c r="CP21" t="s">
+        <v>297</v>
+      </c>
       <c r="CQ21" t="s">
-        <v>297</v>
-      </c>
-      <c r="CR21" t="s">
         <v>285</v>
       </c>
+      <c r="CR21" s="6" t="s">
+        <v>298</v>
+      </c>
       <c r="CS21" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="CT21" s="6" t="s">
         <v>299</v>
       </c>
+      <c r="CT21" t="s">
+        <v>80</v>
+      </c>
       <c r="CU21" t="s">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="CV21" t="s">
-        <v>300</v>
-      </c>
-      <c r="CW21" t="s">
         <v>301</v>
       </c>
     </row>
@@ -4441,25 +4428,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4503,7 +4490,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4526,7 +4513,7 @@
         <v>80572.460000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4537,7 +4524,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -4548,7 +4535,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -4581,7 +4568,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>274</v>
       </c>
@@ -4611,6 +4598,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Person>
+    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005379EE688168984CB30A24F2C465E3DD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bddd9ee50b267174c9b2614a6b605944">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xmlns:ns3="291e76ac-d7a2-47ec-9d94-2ce14ee9642e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd96377d3804d9b42530bcefed490e5a" ns2:_="" ns3:_="">
     <xsd:import namespace="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
@@ -4843,31 +4854,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Person xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Person>
-    <Location xmlns="2bd4a952-cad1-49cd-99aa-57f2f6f4190f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA4A3D4-3A26-4BD8-90F6-19A283515544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4884,22 +4889,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{537C96FB-F45D-4D29-B327-04D5B96D79B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C0F3F9A-307A-4B4F-87DA-5655073F1EAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2bd4a952-cad1-49cd-99aa-57f2f6f4190f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Contingent worker termination scenario added
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestData.xlsx
+++ b/src/main/resources/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195122F1-7AE4-4CF9-AA49-7D8C78083597}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537D2BA9-235A-4D5B-8C9F-22759F4241A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Talent_Acquisition" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="303">
   <si>
     <t>scenario</t>
   </si>
@@ -929,6 +929,9 @@
   </si>
   <si>
     <t>bnhoc1122h</t>
+  </si>
+  <si>
+    <t>CONTINGENT_WORKER_TERMINATION</t>
   </si>
 </sst>
 </file>
@@ -1277,69 +1280,69 @@
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="19.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="19.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="4.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="9.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="24.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="31.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -2007,7 +2010,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2331,7 +2334,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>143</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>227</v>
       </c>
@@ -2719,7 +2722,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>234</v>
       </c>
@@ -3043,7 +3046,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -3068,22 +3071,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.3125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.41796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.5234375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3118,7 +3121,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -3153,7 +3156,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -3176,7 +3179,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -3207,92 +3210,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CV21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.68359375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="6.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="20.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="33.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="5.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="26.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="17.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5546875" customWidth="1"/>
-    <col min="62" max="62" width="26.88671875" customWidth="1"/>
-    <col min="63" max="63" width="18.5546875" customWidth="1"/>
-    <col min="64" max="64" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="18.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="8.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.5234375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.1015625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="7.41796875" bestFit="1" customWidth="1" collapsed